<commit_message>
Finish Main Logic in TestingProgram1, Change it to English(Sorry for the Chinese...)
</commit_message>
<xml_diff>
--- a/TestProgram1.xlsx
+++ b/TestProgram1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QiTianYi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8BAC55AA-3227-42F6-9FB9-9C8E4AEE86AE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8CB56C-FBE7-4757-BE41-9377FB1F0327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5181C135-F803-4CA6-AFB1-3DD996B2224A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5181C135-F803-4CA6-AFB1-3DD996B2224A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="166" uniqueCount="76">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="110">
   <si>
     <t>Memory Location</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -94,258 +94,429 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t xml:space="preserve">检查R1是ASCII的0-9
+    <t>IN R1,KEYBOARD</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDA R0=13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSR IX0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIR R1,10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIR R1,18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIR R1,30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Reserved (HALT)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R1,MEM[30]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R0,MEM[30]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDA R2=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MLT R0,R2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R1,MEM[29]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交换空间：读取的之前的数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>交换空间：读取的现在的数</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMR R1,MEM[29]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDX IX0,MEM[28]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AIR R0,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R0,MEM[8]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R0,MEM[7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R0,MEM[8]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDA R0,9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMR R0, MEM[8]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STX IX2,MEM[7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R3,IX2,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JGE R1, IX0, 13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JGE R1,IX0, 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R3,IX2,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SIR R0,1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JCC CC(3), IX0,12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNE R0,IX0,12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JCC CC(0),IX0,12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JCC CC(3), IX0,29</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JMA IX0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSR IX0,27</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDA R0,13</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R0,MEM[27]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMR R0,MEM[26]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDX IX0,MEM[7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R0,IX0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R0,MEM[27]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDX IX0,MEM[25]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JGE R0,IX0,8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R2,MEM[7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMR R1,MEM[7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RFS(IMM=1)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RFS(IMM=0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMR R1,MEM[7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDX IX0,MEM[24]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JGE R1, IX0, 12</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDX IX2,MEM[7]</t>
+  </si>
+  <si>
+    <t>LDA R0,20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R0,MEM[26]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>AMR R0,MEM[27]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R1,IX0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1=MEM[520]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R2,MEM[30]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JSR IX0,30</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R1,MEM[7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>SMR R2,MEM[7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDX IX0,MEM[22]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R1,MEM[23]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDR R2,MEM[7]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>STR R2,MEM[23]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEM[23]=ENUM-MEM[30]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEM[29]=ENUM</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JZ R0,IX0,15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JMA IX0,20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JGE R0,IX0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>LDX IX0,MEM[21]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JZ R0,IX0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CALL READ_A_NUMBER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CALL READ_20_NUMBER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JKR IX0,22</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CALL FIND_NUMBER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAIN</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JMA IX0,14 (AFTER THE INSTR, THE SPACE USE AS SWAP)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESULT AT MEM[29]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TODO: CALL PRINT TO PRINT MEM[29]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>存PC(R3)到运行栈
+SAVE PC(R3) TO 
+RUNNING STACK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>当前程序运行栈深度，初始为0(RUNNING STACK DEPTH,DEFAULT 0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RUNNING STACK SPACE BELOW(INCLUDING THIS LINE)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>从运行栈恢复PC(R3)
+RETURN PC(R3) TO
+RUNNING STACK</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>检查R1是ASCII的0-9
 如果不是，HALT
 如果是，跳出子程序
- </t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>IN R1,KEYBOARD</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDA R0=13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JSR IX0,0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AIR R1,10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AIR R1,18</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AIR R1,30</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>Reserved (HALT)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR R1,MEM[30]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDR R0,MEM[30]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDA R2=10</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>MLT R0,R2</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR R1,MEM[29]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交换空间：读取的之前的数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>交换空间：读取的现在的数</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AMR R1,MEM[29]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDX IX0,MEM[28]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>当前程序运行栈深度，初始为0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AIR R0,1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SWAP</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDR R0,MEM[8]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR R0,MEM[7]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR R0,MEM[8]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDA R0,9</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AMR R0, MEM[8]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STX IX2,MEM[7]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR R3,IX2,0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JGE R1, IX0, 13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JGE R1,IX0, 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LTX IX2,MEM[7]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDR R3,IX2,0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SIR R0,1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>存PC(R3)到运行栈</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>从运行栈恢复PC(R3)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JCC CC(3), IX0,12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JNE R0,IX0,12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JCC CC(0),IX0,12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JCC CC(3), IX0,29</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JMA IX0,0</t>
+CHECK IF R1 IS '0'-'9'(ASCII)
+IF NOT,HALT
+IF IS, RETURN NORMALLY
+WITH NO RETURN VALUE</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>从IO读取一个数字
 转化为数字
-存入MEM[30]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JSR IX0,27</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDA R0,13</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDR R0,MEM[27]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AMR R0,MEM[26]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDX IX0,MEM[7]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR R0,IX0,0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR R0,MEM[27]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDX IX0,MEM[25]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JGE R0,IX0,8</t>
+存入MEM[30]
+READ A NUMBER FROM IO
+CHECK IF LEGIT
+CONVERT TO INTEGER
+STORE TO MEM[30]</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>读取20个数字
 存入MEM[500]~MEM[520]
 逆序存储
-第一个读入的数字存到520地址</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>STR R2,MEM[7]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>SMR R1,MEM[7]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RFS(IMM=1)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R2大,R0=1</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>RFS(IMM=0)</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>R1大,R0=0</t>
+第一个读入的数字存到520地址
+READ 20 NUMBERS
+SAVE TO MEM[500~520]
+SAVE IN REVERSE ORDER
+THAT IS:
+THE 1ST NUMBER READED
+SAVE TO MEM[520]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>RESTORE THE VALUE OF R1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2 IS BIGGER,R0=1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1 IS BIGGER,R0=0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
     <t>比较R1，R2谁大
 如果R1大，返回0
 R2大或者相等，返回1
-返回值存入R0</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>AMR R1,MEM[7]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>LDX IX0,MEM[24]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JGE R1, IX0, 12</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>恢复R1数值</t>
+返回值存入R0
+COMPARE R1,R2
+IF R1 IS BIGGER
+RETURN 0(R0)
+IF R2 IS BIGGER OR EQUAL
+RETURN 1(R0)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>逆序遍历MEM[500]-[520]
+将最接近MEM[30]的数字
+放到MEM[29]
+REVERSE VISITING MEM500~520]
+FIND THE NEAREST NUMBER
+OF MEM[30]
+PLACE IT TO MEM[29]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAIN LOGIC START HERE()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2 BIGGER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MEM[7]=ABS(ENUM-MEM[30])</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1 BIGGER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>MAIN LOGIC:
+B IS MEM[29]
+A IS MEM[23]. WITH INITIAL VALUE OF 65535
+FOR ENUM IN MEM[500~520] (MACHINE CODE VISITED IN REVERSE ORDER,FROM 520 TO 500):
+IF ABSOLUTEVALUE(ENUM-MEM[30])&gt;A:
+A=ABSOLUTEVALUE(ENUM-MEM[30])
+B=ENUM
+ELSE:
+DO_NOTHING</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,7 +578,7 @@
       <family val="1"/>
     </font>
   </fonts>
-  <fills count="4">
+  <fills count="5">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -423,6 +594,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -633,7 +810,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -706,6 +883,21 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="17" xfId="0" applyFont="1" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -724,18 +916,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -748,12 +928,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -763,14 +937,26 @@
     <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1086,16 +1272,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72887D96-2685-464A-84B6-218C724B7504}">
-  <dimension ref="A1:F1026"/>
+  <dimension ref="A1:R1026"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A135" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D107" sqref="D107:F136"/>
+    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
+      <pane ySplit="33" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="P200" sqref="P200"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="9.125" style="1" customWidth="1"/>
-    <col min="2" max="2" width="45.125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="73.75" style="1" customWidth="1"/>
     <col min="3" max="3" width="28.25" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1114,12 +1301,12 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="40" t="s">
+      <c r="C2" s="39" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="40"/>
-      <c r="E2" s="40"/>
-      <c r="F2" s="40"/>
+      <c r="D2" s="39"/>
+      <c r="E2" s="39"/>
+      <c r="F2" s="39"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -1128,10 +1315,10 @@
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="40"/>
-      <c r="D3" s="40"/>
-      <c r="E3" s="40"/>
-      <c r="F3" s="40"/>
+      <c r="C3" s="39"/>
+      <c r="D3" s="39"/>
+      <c r="E3" s="39"/>
+      <c r="F3" s="39"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
@@ -1140,22 +1327,22 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="40"/>
-      <c r="D4" s="40"/>
-      <c r="E4" s="40"/>
-      <c r="F4" s="40"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
         <v>3</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C5" s="40"/>
-      <c r="D5" s="40"/>
-      <c r="E5" s="40"/>
-      <c r="F5" s="40"/>
+        <v>21</v>
+      </c>
+      <c r="C5" s="39"/>
+      <c r="D5" s="39"/>
+      <c r="E5" s="39"/>
+      <c r="F5" s="39"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
@@ -1164,208 +1351,218 @@
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="40"/>
-      <c r="D6" s="40"/>
-      <c r="E6" s="40"/>
-      <c r="F6" s="40"/>
+      <c r="C6" s="39"/>
+      <c r="D6" s="39"/>
+      <c r="E6" s="39"/>
+      <c r="F6" s="39"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
         <v>5</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" s="40"/>
-      <c r="D7" s="40"/>
-      <c r="E7" s="40"/>
-      <c r="F7" s="40"/>
+        <v>21</v>
+      </c>
+      <c r="C7" s="39"/>
+      <c r="D7" s="39"/>
+      <c r="E7" s="39"/>
+      <c r="F7" s="39"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
         <v>6</v>
       </c>
-      <c r="B8" s="3"/>
-      <c r="C8" s="41" t="s">
+      <c r="B8" s="3" t="s">
+        <v>83</v>
+      </c>
+      <c r="C8" s="40" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="42"/>
-      <c r="E8" s="42"/>
-      <c r="F8" s="42"/>
+      <c r="D8" s="41"/>
+      <c r="E8" s="41"/>
+      <c r="F8" s="41"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>34</v>
-      </c>
-      <c r="C9" s="42"/>
-      <c r="D9" s="42"/>
-      <c r="E9" s="42"/>
-      <c r="F9" s="42"/>
+        <v>90</v>
+      </c>
+      <c r="C9" s="41"/>
+      <c r="D9" s="41"/>
+      <c r="E9" s="41"/>
+      <c r="F9" s="41"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>32</v>
-      </c>
-      <c r="C10" s="42"/>
-      <c r="D10" s="42"/>
-      <c r="E10" s="42"/>
-      <c r="F10" s="42"/>
+        <v>94</v>
+      </c>
+      <c r="C10" s="41"/>
+      <c r="D10" s="41"/>
+      <c r="E10" s="41"/>
+      <c r="F10" s="41"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
-      <c r="B11" s="13"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
+      <c r="B11" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="C11" s="41"/>
+      <c r="D11" s="41"/>
+      <c r="E11" s="41"/>
+      <c r="F11" s="41"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="C12" s="42"/>
-      <c r="D12" s="42"/>
-      <c r="E12" s="42"/>
-      <c r="F12" s="42"/>
+      <c r="C12" s="41"/>
+      <c r="D12" s="41"/>
+      <c r="E12" s="41"/>
+      <c r="F12" s="41"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="42"/>
-      <c r="D13" s="42"/>
-      <c r="E13" s="42"/>
-      <c r="F13" s="42"/>
+      <c r="C13" s="41"/>
+      <c r="D13" s="41"/>
+      <c r="E13" s="41"/>
+      <c r="F13" s="41"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="13"/>
-      <c r="C14" s="42"/>
-      <c r="D14" s="42"/>
-      <c r="E14" s="42"/>
-      <c r="F14" s="42"/>
+      <c r="C14" s="41"/>
+      <c r="D14" s="41"/>
+      <c r="E14" s="41"/>
+      <c r="F14" s="41"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="13"/>
-      <c r="C15" s="42"/>
-      <c r="D15" s="42"/>
-      <c r="E15" s="42"/>
-      <c r="F15" s="42"/>
+      <c r="C15" s="41"/>
+      <c r="D15" s="41"/>
+      <c r="E15" s="41"/>
+      <c r="F15" s="41"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="13"/>
-      <c r="C16" s="42"/>
-      <c r="D16" s="42"/>
-      <c r="E16" s="42"/>
-      <c r="F16" s="42"/>
+      <c r="C16" s="41"/>
+      <c r="D16" s="41"/>
+      <c r="E16" s="41"/>
+      <c r="F16" s="41"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="42"/>
-      <c r="D17" s="42"/>
-      <c r="E17" s="42"/>
-      <c r="F17" s="42"/>
+      <c r="C17" s="41"/>
+      <c r="D17" s="41"/>
+      <c r="E17" s="41"/>
+      <c r="F17" s="41"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="42"/>
-      <c r="D18" s="42"/>
-      <c r="E18" s="42"/>
-      <c r="F18" s="42"/>
+      <c r="C18" s="41"/>
+      <c r="D18" s="41"/>
+      <c r="E18" s="41"/>
+      <c r="F18" s="41"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="13"/>
-      <c r="C19" s="42"/>
-      <c r="D19" s="42"/>
-      <c r="E19" s="42"/>
-      <c r="F19" s="42"/>
+      <c r="C19" s="41"/>
+      <c r="D19" s="41"/>
+      <c r="E19" s="41"/>
+      <c r="F19" s="41"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="42"/>
-      <c r="D20" s="42"/>
-      <c r="E20" s="42"/>
-      <c r="F20" s="42"/>
+      <c r="C20" s="41"/>
+      <c r="D20" s="41"/>
+      <c r="E20" s="41"/>
+      <c r="F20" s="41"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="42"/>
-      <c r="D21" s="42"/>
-      <c r="E21" s="42"/>
-      <c r="F21" s="42"/>
+      <c r="C21" s="41"/>
+      <c r="D21" s="41"/>
+      <c r="E21" s="41"/>
+      <c r="F21" s="41"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="42"/>
-      <c r="D22" s="42"/>
-      <c r="E22" s="42"/>
-      <c r="F22" s="42"/>
+      <c r="C22" s="41"/>
+      <c r="D22" s="41"/>
+      <c r="E22" s="41"/>
+      <c r="F22" s="41"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
         <v>21</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="42"/>
-      <c r="D23" s="42"/>
-      <c r="E23" s="42"/>
-      <c r="F23" s="42"/>
+      <c r="B23" s="3">
+        <v>210</v>
+      </c>
+      <c r="C23" s="41"/>
+      <c r="D23" s="41"/>
+      <c r="E23" s="41"/>
+      <c r="F23" s="41"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
         <v>22</v>
       </c>
-      <c r="B24" s="3"/>
-      <c r="C24" s="42"/>
-      <c r="D24" s="42"/>
-      <c r="E24" s="42"/>
-      <c r="F24" s="42"/>
+      <c r="B24" s="3">
+        <v>177</v>
+      </c>
+      <c r="C24" s="41"/>
+      <c r="D24" s="41"/>
+      <c r="E24" s="41"/>
+      <c r="F24" s="41"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
         <v>23</v>
       </c>
-      <c r="B25" s="3"/>
-      <c r="C25" s="42"/>
-      <c r="D25" s="42"/>
-      <c r="E25" s="42"/>
-      <c r="F25" s="42"/>
+      <c r="B25" s="3">
+        <v>65535</v>
+      </c>
+      <c r="C25" s="41"/>
+      <c r="D25" s="41"/>
+      <c r="E25" s="41"/>
+      <c r="F25" s="41"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
@@ -1374,10 +1571,10 @@
       <c r="B26" s="3">
         <v>145</v>
       </c>
-      <c r="C26" s="42"/>
-      <c r="D26" s="42"/>
-      <c r="E26" s="42"/>
-      <c r="F26" s="42"/>
+      <c r="C26" s="41"/>
+      <c r="D26" s="41"/>
+      <c r="E26" s="41"/>
+      <c r="F26" s="41"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
@@ -1386,10 +1583,10 @@
       <c r="B27" s="3">
         <v>105</v>
       </c>
-      <c r="C27" s="42"/>
-      <c r="D27" s="42"/>
-      <c r="E27" s="42"/>
-      <c r="F27" s="42"/>
+      <c r="C27" s="41"/>
+      <c r="D27" s="41"/>
+      <c r="E27" s="41"/>
+      <c r="F27" s="41"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
@@ -1398,10 +1595,10 @@
       <c r="B28" s="3">
         <v>500</v>
       </c>
-      <c r="C28" s="42"/>
-      <c r="D28" s="42"/>
-      <c r="E28" s="42"/>
-      <c r="F28" s="42"/>
+      <c r="C28" s="41"/>
+      <c r="D28" s="41"/>
+      <c r="E28" s="41"/>
+      <c r="F28" s="41"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
@@ -1410,10 +1607,10 @@
       <c r="B29" s="3">
         <v>20</v>
       </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="42"/>
-      <c r="E29" s="42"/>
-      <c r="F29" s="42"/>
+      <c r="C29" s="41"/>
+      <c r="D29" s="41"/>
+      <c r="E29" s="41"/>
+      <c r="F29" s="41"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
@@ -1422,34 +1619,34 @@
       <c r="B30" s="3">
         <v>67</v>
       </c>
-      <c r="C30" s="42"/>
-      <c r="D30" s="42"/>
-      <c r="E30" s="42"/>
-      <c r="F30" s="42"/>
+      <c r="C30" s="41"/>
+      <c r="D30" s="41"/>
+      <c r="E30" s="41"/>
+      <c r="F30" s="41"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
         <v>29</v>
       </c>
       <c r="B31" s="10" t="s">
-        <v>29</v>
-      </c>
-      <c r="C31" s="42"/>
-      <c r="D31" s="42"/>
-      <c r="E31" s="42"/>
-      <c r="F31" s="42"/>
+        <v>28</v>
+      </c>
+      <c r="C31" s="41"/>
+      <c r="D31" s="41"/>
+      <c r="E31" s="41"/>
+      <c r="F31" s="41"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
         <v>30</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="C32" s="42"/>
-      <c r="D32" s="42"/>
-      <c r="E32" s="42"/>
-      <c r="F32" s="42"/>
+        <v>27</v>
+      </c>
+      <c r="C32" s="41"/>
+      <c r="D32" s="41"/>
+      <c r="E32" s="41"/>
+      <c r="F32" s="41"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -1458,110 +1655,110 @@
       <c r="B33" s="5">
         <v>32</v>
       </c>
-      <c r="C33" s="42"/>
-      <c r="D33" s="42"/>
-      <c r="E33" s="42"/>
-      <c r="F33" s="42"/>
+      <c r="C33" s="41"/>
+      <c r="D33" s="41"/>
+      <c r="E33" s="41"/>
+      <c r="F33" s="41"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
         <v>32</v>
       </c>
       <c r="B34" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C34" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D34" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="E34" s="24"/>
-      <c r="F34" s="25"/>
+        <v>32</v>
+      </c>
+      <c r="C34" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="D34" s="29" t="s">
+        <v>97</v>
+      </c>
+      <c r="E34" s="29"/>
+      <c r="F34" s="30"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
         <v>33</v>
       </c>
       <c r="B35" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C35" s="31"/>
-      <c r="D35" s="26"/>
-      <c r="E35" s="26"/>
-      <c r="F35" s="27"/>
+        <v>31</v>
+      </c>
+      <c r="C35" s="27"/>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
+      <c r="F35" s="32"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
         <v>34</v>
       </c>
       <c r="B36" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C36" s="31"/>
-      <c r="D36" s="26"/>
-      <c r="E36" s="26"/>
-      <c r="F36" s="27"/>
+        <v>34</v>
+      </c>
+      <c r="C36" s="27"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
+      <c r="F36" s="32"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
         <v>35</v>
       </c>
       <c r="B37" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C37" s="31"/>
-      <c r="D37" s="26"/>
-      <c r="E37" s="26"/>
-      <c r="F37" s="27"/>
+        <v>35</v>
+      </c>
+      <c r="C37" s="27"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
+      <c r="F37" s="32"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="15">
         <v>36</v>
       </c>
       <c r="B38" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C38" s="31"/>
-      <c r="D38" s="26"/>
-      <c r="E38" s="26"/>
-      <c r="F38" s="27"/>
+        <v>36</v>
+      </c>
+      <c r="C38" s="27"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
+      <c r="F38" s="32"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
         <v>37</v>
       </c>
       <c r="B39" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C39" s="31"/>
-      <c r="D39" s="26"/>
-      <c r="E39" s="26"/>
-      <c r="F39" s="27"/>
+        <v>33</v>
+      </c>
+      <c r="C39" s="27"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
+      <c r="F39" s="32"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
         <v>38</v>
       </c>
       <c r="B40" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C40" s="31"/>
-      <c r="D40" s="26"/>
-      <c r="E40" s="26"/>
-      <c r="F40" s="27"/>
+        <v>37</v>
+      </c>
+      <c r="C40" s="27"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
+      <c r="F40" s="32"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
         <v>39</v>
       </c>
       <c r="B41" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C41" s="32"/>
-      <c r="D41" s="26"/>
-      <c r="E41" s="26"/>
-      <c r="F41" s="27"/>
+        <v>38</v>
+      </c>
+      <c r="C41" s="28"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
+      <c r="F41" s="32"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -1571,9 +1768,9 @@
         <v>12</v>
       </c>
       <c r="C42" s="17"/>
-      <c r="D42" s="26"/>
-      <c r="E42" s="26"/>
-      <c r="F42" s="27"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
+      <c r="F42" s="32"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -1583,9 +1780,9 @@
         <v>13</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="26"/>
-      <c r="E43" s="26"/>
-      <c r="F43" s="27"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
+      <c r="F43" s="32"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -1595,21 +1792,21 @@
         <v>11</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="26"/>
-      <c r="E44" s="26"/>
-      <c r="F44" s="27"/>
+      <c r="D44" s="31"/>
+      <c r="E44" s="31"/>
+      <c r="F44" s="32"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
         <v>43</v>
       </c>
       <c r="B45" s="6" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="D45" s="26"/>
-      <c r="E45" s="26"/>
-      <c r="F45" s="27"/>
+      <c r="D45" s="31"/>
+      <c r="E45" s="31"/>
+      <c r="F45" s="32"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
@@ -1619,9 +1816,9 @@
         <v>9</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="26"/>
-      <c r="E46" s="26"/>
-      <c r="F46" s="27"/>
+      <c r="D46" s="31"/>
+      <c r="E46" s="31"/>
+      <c r="F46" s="32"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -1631,155 +1828,155 @@
         <v>14</v>
       </c>
       <c r="C47" s="7"/>
-      <c r="D47" s="26"/>
-      <c r="E47" s="26"/>
-      <c r="F47" s="27"/>
+      <c r="D47" s="31"/>
+      <c r="E47" s="31"/>
+      <c r="F47" s="32"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
         <v>46</v>
       </c>
       <c r="B48" s="6" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="26"/>
-      <c r="E48" s="26"/>
-      <c r="F48" s="27"/>
+      <c r="D48" s="31"/>
+      <c r="E48" s="31"/>
+      <c r="F48" s="32"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
         <v>47</v>
       </c>
       <c r="B49" s="6" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="D49" s="26"/>
-      <c r="E49" s="26"/>
-      <c r="F49" s="27"/>
+      <c r="D49" s="31"/>
+      <c r="E49" s="31"/>
+      <c r="F49" s="32"/>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
         <v>48</v>
       </c>
       <c r="B50" s="6" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="26"/>
-      <c r="E50" s="26"/>
-      <c r="F50" s="27"/>
+      <c r="D50" s="31"/>
+      <c r="E50" s="31"/>
+      <c r="F50" s="32"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
         <v>49</v>
       </c>
       <c r="B51" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="26"/>
-      <c r="E51" s="26"/>
-      <c r="F51" s="27"/>
+      <c r="D51" s="31"/>
+      <c r="E51" s="31"/>
+      <c r="F51" s="32"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
         <v>50</v>
       </c>
       <c r="B52" s="18" t="s">
-        <v>38</v>
-      </c>
-      <c r="C52" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D52" s="26"/>
-      <c r="E52" s="26"/>
-      <c r="F52" s="27"/>
+        <v>35</v>
+      </c>
+      <c r="C52" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D52" s="31"/>
+      <c r="E52" s="31"/>
+      <c r="F52" s="32"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
         <v>51</v>
       </c>
       <c r="B53" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C53" s="31"/>
-      <c r="D53" s="26"/>
-      <c r="E53" s="26"/>
-      <c r="F53" s="27"/>
+        <v>36</v>
+      </c>
+      <c r="C53" s="27"/>
+      <c r="D53" s="31"/>
+      <c r="E53" s="31"/>
+      <c r="F53" s="32"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
         <v>52</v>
       </c>
       <c r="B54" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C54" s="31"/>
-      <c r="D54" s="26"/>
-      <c r="E54" s="26"/>
-      <c r="F54" s="27"/>
+        <v>33</v>
+      </c>
+      <c r="C54" s="27"/>
+      <c r="D54" s="31"/>
+      <c r="E54" s="31"/>
+      <c r="F54" s="32"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
         <v>53</v>
       </c>
       <c r="B55" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C55" s="31"/>
-      <c r="D55" s="26"/>
-      <c r="E55" s="26"/>
-      <c r="F55" s="27"/>
+        <v>64</v>
+      </c>
+      <c r="C55" s="27"/>
+      <c r="D55" s="31"/>
+      <c r="E55" s="31"/>
+      <c r="F55" s="32"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
         <v>54</v>
       </c>
       <c r="B56" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C56" s="31"/>
-      <c r="D56" s="26"/>
-      <c r="E56" s="26"/>
-      <c r="F56" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="C56" s="27"/>
+      <c r="D56" s="31"/>
+      <c r="E56" s="31"/>
+      <c r="F56" s="32"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
         <v>55</v>
       </c>
       <c r="B57" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C57" s="31"/>
-      <c r="D57" s="26"/>
-      <c r="E57" s="26"/>
-      <c r="F57" s="27"/>
+        <v>32</v>
+      </c>
+      <c r="C57" s="27"/>
+      <c r="D57" s="31"/>
+      <c r="E57" s="31"/>
+      <c r="F57" s="32"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
         <v>56</v>
       </c>
       <c r="B58" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C58" s="31"/>
-      <c r="D58" s="26"/>
-      <c r="E58" s="26"/>
-      <c r="F58" s="27"/>
+        <v>42</v>
+      </c>
+      <c r="C58" s="27"/>
+      <c r="D58" s="31"/>
+      <c r="E58" s="31"/>
+      <c r="F58" s="32"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
         <v>57</v>
       </c>
       <c r="B59" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C59" s="32"/>
-      <c r="D59" s="26"/>
-      <c r="E59" s="26"/>
-      <c r="F59" s="27"/>
+        <v>34</v>
+      </c>
+      <c r="C59" s="28"/>
+      <c r="D59" s="31"/>
+      <c r="E59" s="31"/>
+      <c r="F59" s="32"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
@@ -1789,133 +1986,133 @@
         <v>10</v>
       </c>
       <c r="C60" s="9"/>
-      <c r="D60" s="28"/>
-      <c r="E60" s="28"/>
-      <c r="F60" s="29"/>
+      <c r="D60" s="33"/>
+      <c r="E60" s="33"/>
+      <c r="F60" s="34"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
         <v>59</v>
       </c>
       <c r="B61" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C61" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D61" s="24" t="s">
-        <v>54</v>
-      </c>
-      <c r="E61" s="34"/>
-      <c r="F61" s="35"/>
+        <v>32</v>
+      </c>
+      <c r="C61" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="D61" s="29" t="s">
+        <v>98</v>
+      </c>
+      <c r="E61" s="35"/>
+      <c r="F61" s="36"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
         <v>60</v>
       </c>
       <c r="B62" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C62" s="31"/>
-      <c r="D62" s="36"/>
-      <c r="E62" s="36"/>
-      <c r="F62" s="37"/>
+        <v>31</v>
+      </c>
+      <c r="C62" s="27"/>
+      <c r="D62" s="37"/>
+      <c r="E62" s="37"/>
+      <c r="F62" s="38"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
         <v>61</v>
       </c>
       <c r="B63" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C63" s="31"/>
-      <c r="D63" s="36"/>
-      <c r="E63" s="36"/>
-      <c r="F63" s="37"/>
+        <v>34</v>
+      </c>
+      <c r="C63" s="27"/>
+      <c r="D63" s="37"/>
+      <c r="E63" s="37"/>
+      <c r="F63" s="38"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
         <v>62</v>
       </c>
       <c r="B64" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C64" s="31"/>
-      <c r="D64" s="36"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="37"/>
+        <v>35</v>
+      </c>
+      <c r="C64" s="27"/>
+      <c r="D64" s="37"/>
+      <c r="E64" s="37"/>
+      <c r="F64" s="38"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
         <v>63</v>
       </c>
       <c r="B65" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C65" s="31"/>
-      <c r="D65" s="36"/>
-      <c r="E65" s="36"/>
-      <c r="F65" s="37"/>
+        <v>36</v>
+      </c>
+      <c r="C65" s="27"/>
+      <c r="D65" s="37"/>
+      <c r="E65" s="37"/>
+      <c r="F65" s="38"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
         <v>64</v>
       </c>
       <c r="B66" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C66" s="31"/>
-      <c r="D66" s="36"/>
-      <c r="E66" s="36"/>
-      <c r="F66" s="37"/>
+        <v>33</v>
+      </c>
+      <c r="C66" s="27"/>
+      <c r="D66" s="37"/>
+      <c r="E66" s="37"/>
+      <c r="F66" s="38"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
         <v>65</v>
       </c>
       <c r="B67" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C67" s="31"/>
-      <c r="D67" s="36"/>
-      <c r="E67" s="36"/>
-      <c r="F67" s="37"/>
+        <v>37</v>
+      </c>
+      <c r="C67" s="27"/>
+      <c r="D67" s="37"/>
+      <c r="E67" s="37"/>
+      <c r="F67" s="38"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
         <v>66</v>
       </c>
       <c r="B68" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C68" s="32"/>
-      <c r="D68" s="36"/>
-      <c r="E68" s="36"/>
-      <c r="F68" s="37"/>
+        <v>38</v>
+      </c>
+      <c r="C68" s="28"/>
+      <c r="D68" s="37"/>
+      <c r="E68" s="37"/>
+      <c r="F68" s="38"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
         <v>67</v>
       </c>
       <c r="B69" s="11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C69" s="7"/>
-      <c r="D69" s="36"/>
-      <c r="E69" s="36"/>
-      <c r="F69" s="37"/>
+      <c r="D69" s="37"/>
+      <c r="E69" s="37"/>
+      <c r="F69" s="38"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
         <v>68</v>
       </c>
       <c r="B70" s="6" t="s">
-        <v>56</v>
+        <v>49</v>
       </c>
       <c r="C70" s="7"/>
-      <c r="D70" s="36"/>
-      <c r="E70" s="36"/>
-      <c r="F70" s="37"/>
+      <c r="D70" s="37"/>
+      <c r="E70" s="37"/>
+      <c r="F70" s="38"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
@@ -1925,9 +2122,9 @@
         <v>11</v>
       </c>
       <c r="C71" s="7"/>
-      <c r="D71" s="36"/>
-      <c r="E71" s="36"/>
-      <c r="F71" s="37"/>
+      <c r="D71" s="37"/>
+      <c r="E71" s="37"/>
+      <c r="F71" s="38"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
@@ -1937,33 +2134,33 @@
         <v>8</v>
       </c>
       <c r="C72" s="7"/>
-      <c r="D72" s="36"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="37"/>
+      <c r="D72" s="37"/>
+      <c r="E72" s="37"/>
+      <c r="F72" s="38"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="15">
         <v>71</v>
       </c>
       <c r="B73" s="19" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
       <c r="C73" s="7"/>
-      <c r="D73" s="36"/>
-      <c r="E73" s="36"/>
-      <c r="F73" s="37"/>
+      <c r="D73" s="37"/>
+      <c r="E73" s="37"/>
+      <c r="F73" s="38"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
         <v>72</v>
       </c>
       <c r="B74" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C74" s="7"/>
-      <c r="D74" s="36"/>
-      <c r="E74" s="36"/>
-      <c r="F74" s="37"/>
+      <c r="D74" s="37"/>
+      <c r="E74" s="37"/>
+      <c r="F74" s="38"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
@@ -1973,9 +2170,9 @@
         <v>12</v>
       </c>
       <c r="C75" s="7"/>
-      <c r="D75" s="36"/>
-      <c r="E75" s="36"/>
-      <c r="F75" s="37"/>
+      <c r="D75" s="37"/>
+      <c r="E75" s="37"/>
+      <c r="F75" s="38"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -1985,45 +2182,45 @@
         <v>13</v>
       </c>
       <c r="C76" s="7"/>
-      <c r="D76" s="36"/>
-      <c r="E76" s="36"/>
-      <c r="F76" s="37"/>
+      <c r="D76" s="37"/>
+      <c r="E76" s="37"/>
+      <c r="F76" s="38"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
         <v>75</v>
       </c>
       <c r="B77" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C77" s="7"/>
-      <c r="D77" s="36"/>
-      <c r="E77" s="36"/>
-      <c r="F77" s="37"/>
+      <c r="D77" s="37"/>
+      <c r="E77" s="37"/>
+      <c r="F77" s="38"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
         <v>76</v>
       </c>
       <c r="B78" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C78" s="7"/>
-      <c r="D78" s="36"/>
-      <c r="E78" s="36"/>
-      <c r="F78" s="37"/>
+      <c r="D78" s="37"/>
+      <c r="E78" s="37"/>
+      <c r="F78" s="38"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
         <v>77</v>
       </c>
       <c r="B79" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C79" s="7"/>
-      <c r="D79" s="36"/>
-      <c r="E79" s="36"/>
-      <c r="F79" s="37"/>
+      <c r="D79" s="37"/>
+      <c r="E79" s="37"/>
+      <c r="F79" s="38"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
@@ -2033,33 +2230,33 @@
         <v>8</v>
       </c>
       <c r="C80" s="7"/>
-      <c r="D80" s="36"/>
-      <c r="E80" s="36"/>
-      <c r="F80" s="37"/>
+      <c r="D80" s="37"/>
+      <c r="E80" s="37"/>
+      <c r="F80" s="38"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
         <v>79</v>
       </c>
       <c r="B81" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C81" s="7"/>
-      <c r="D81" s="36"/>
-      <c r="E81" s="36"/>
-      <c r="F81" s="37"/>
+      <c r="D81" s="37"/>
+      <c r="E81" s="37"/>
+      <c r="F81" s="38"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
         <v>80</v>
       </c>
       <c r="B82" s="19" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C82" s="7"/>
-      <c r="D82" s="36"/>
-      <c r="E82" s="36"/>
-      <c r="F82" s="37"/>
+      <c r="D82" s="37"/>
+      <c r="E82" s="37"/>
+      <c r="F82" s="38"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
@@ -2069,21 +2266,21 @@
         <v>11</v>
       </c>
       <c r="C83" s="7"/>
-      <c r="D83" s="36"/>
-      <c r="E83" s="36"/>
-      <c r="F83" s="37"/>
+      <c r="D83" s="37"/>
+      <c r="E83" s="37"/>
+      <c r="F83" s="38"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
         <v>82</v>
       </c>
       <c r="B84" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C84" s="7"/>
-      <c r="D84" s="36"/>
-      <c r="E84" s="36"/>
-      <c r="F84" s="37"/>
+      <c r="D84" s="37"/>
+      <c r="E84" s="37"/>
+      <c r="F84" s="38"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
@@ -2093,9 +2290,9 @@
         <v>12</v>
       </c>
       <c r="C85" s="7"/>
-      <c r="D85" s="36"/>
-      <c r="E85" s="36"/>
-      <c r="F85" s="37"/>
+      <c r="D85" s="37"/>
+      <c r="E85" s="37"/>
+      <c r="F85" s="38"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
@@ -2105,57 +2302,57 @@
         <v>13</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="36"/>
-      <c r="E86" s="36"/>
-      <c r="F86" s="37"/>
+      <c r="D86" s="37"/>
+      <c r="E86" s="37"/>
+      <c r="F86" s="38"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
         <v>85</v>
       </c>
       <c r="B87" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C87" s="7"/>
-      <c r="D87" s="36"/>
-      <c r="E87" s="36"/>
-      <c r="F87" s="37"/>
+      <c r="D87" s="37"/>
+      <c r="E87" s="37"/>
+      <c r="F87" s="38"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
         <v>86</v>
       </c>
       <c r="B88" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C88" s="7"/>
-      <c r="D88" s="36"/>
-      <c r="E88" s="36"/>
-      <c r="F88" s="37"/>
+      <c r="D88" s="37"/>
+      <c r="E88" s="37"/>
+      <c r="F88" s="38"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
         <v>87</v>
       </c>
       <c r="B89" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C89" s="7"/>
-      <c r="D89" s="36"/>
-      <c r="E89" s="36"/>
-      <c r="F89" s="37"/>
+      <c r="D89" s="37"/>
+      <c r="E89" s="37"/>
+      <c r="F89" s="38"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
         <v>88</v>
       </c>
       <c r="B90" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="36"/>
-      <c r="E90" s="36"/>
-      <c r="F90" s="37"/>
+      <c r="D90" s="37"/>
+      <c r="E90" s="37"/>
+      <c r="F90" s="38"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
@@ -2165,179 +2362,179 @@
         <v>11</v>
       </c>
       <c r="C91" s="7"/>
-      <c r="D91" s="36"/>
-      <c r="E91" s="36"/>
-      <c r="F91" s="37"/>
+      <c r="D91" s="37"/>
+      <c r="E91" s="37"/>
+      <c r="F91" s="38"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
         <v>90</v>
       </c>
       <c r="B92" s="6" t="s">
-        <v>50</v>
+        <v>44</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="36"/>
-      <c r="E92" s="36"/>
-      <c r="F92" s="37"/>
+      <c r="D92" s="37"/>
+      <c r="E92" s="37"/>
+      <c r="F92" s="38"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
         <v>91</v>
       </c>
       <c r="B93" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C93" s="7"/>
-      <c r="D93" s="36"/>
-      <c r="E93" s="36"/>
-      <c r="F93" s="37"/>
+      <c r="D93" s="37"/>
+      <c r="E93" s="37"/>
+      <c r="F93" s="38"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
         <v>92</v>
       </c>
       <c r="B94" s="6" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="36"/>
-      <c r="E94" s="36"/>
-      <c r="F94" s="37"/>
+      <c r="D94" s="37"/>
+      <c r="E94" s="37"/>
+      <c r="F94" s="38"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
         <v>93</v>
       </c>
       <c r="B95" s="6" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C95" s="7"/>
-      <c r="D95" s="36"/>
-      <c r="E95" s="36"/>
-      <c r="F95" s="37"/>
+      <c r="D95" s="37"/>
+      <c r="E95" s="37"/>
+      <c r="F95" s="38"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
         <v>94</v>
       </c>
       <c r="B96" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C96" s="7"/>
-      <c r="D96" s="36"/>
-      <c r="E96" s="36"/>
-      <c r="F96" s="37"/>
+      <c r="D96" s="37"/>
+      <c r="E96" s="37"/>
+      <c r="F96" s="38"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
         <v>95</v>
       </c>
       <c r="B97" s="6" t="s">
-        <v>53</v>
+        <v>47</v>
       </c>
       <c r="C97" s="7"/>
-      <c r="D97" s="36"/>
-      <c r="E97" s="36"/>
-      <c r="F97" s="37"/>
+      <c r="D97" s="37"/>
+      <c r="E97" s="37"/>
+      <c r="F97" s="38"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
         <v>96</v>
       </c>
       <c r="B98" s="21" t="s">
-        <v>38</v>
-      </c>
-      <c r="C98" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D98" s="36"/>
-      <c r="E98" s="36"/>
-      <c r="F98" s="37"/>
+        <v>35</v>
+      </c>
+      <c r="C98" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D98" s="37"/>
+      <c r="E98" s="37"/>
+      <c r="F98" s="38"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
         <v>97</v>
       </c>
       <c r="B99" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C99" s="31"/>
-      <c r="D99" s="36"/>
-      <c r="E99" s="36"/>
-      <c r="F99" s="37"/>
+        <v>36</v>
+      </c>
+      <c r="C99" s="27"/>
+      <c r="D99" s="37"/>
+      <c r="E99" s="37"/>
+      <c r="F99" s="38"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
         <v>98</v>
       </c>
       <c r="B100" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C100" s="31"/>
-      <c r="D100" s="36"/>
-      <c r="E100" s="36"/>
-      <c r="F100" s="37"/>
+        <v>33</v>
+      </c>
+      <c r="C100" s="27"/>
+      <c r="D100" s="37"/>
+      <c r="E100" s="37"/>
+      <c r="F100" s="38"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
         <v>99</v>
       </c>
       <c r="B101" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C101" s="31"/>
-      <c r="D101" s="36"/>
-      <c r="E101" s="36"/>
-      <c r="F101" s="37"/>
+        <v>64</v>
+      </c>
+      <c r="C101" s="27"/>
+      <c r="D101" s="37"/>
+      <c r="E101" s="37"/>
+      <c r="F101" s="38"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
         <v>100</v>
       </c>
       <c r="B102" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C102" s="31"/>
-      <c r="D102" s="36"/>
-      <c r="E102" s="36"/>
-      <c r="F102" s="37"/>
+        <v>41</v>
+      </c>
+      <c r="C102" s="27"/>
+      <c r="D102" s="37"/>
+      <c r="E102" s="37"/>
+      <c r="F102" s="38"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
         <v>101</v>
       </c>
       <c r="B103" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C103" s="31"/>
-      <c r="D103" s="36"/>
-      <c r="E103" s="36"/>
-      <c r="F103" s="37"/>
+        <v>32</v>
+      </c>
+      <c r="C103" s="27"/>
+      <c r="D103" s="37"/>
+      <c r="E103" s="37"/>
+      <c r="F103" s="38"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
         <v>102</v>
       </c>
       <c r="B104" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C104" s="31"/>
-      <c r="D104" s="36"/>
-      <c r="E104" s="36"/>
-      <c r="F104" s="37"/>
+        <v>42</v>
+      </c>
+      <c r="C104" s="27"/>
+      <c r="D104" s="37"/>
+      <c r="E104" s="37"/>
+      <c r="F104" s="38"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
         <v>103</v>
       </c>
       <c r="B105" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C105" s="32"/>
-      <c r="D105" s="36"/>
-      <c r="E105" s="36"/>
-      <c r="F105" s="37"/>
+        <v>34</v>
+      </c>
+      <c r="C105" s="28"/>
+      <c r="D105" s="37"/>
+      <c r="E105" s="37"/>
+      <c r="F105" s="38"/>
     </row>
     <row r="106" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
@@ -2347,109 +2544,109 @@
         <v>10</v>
       </c>
       <c r="C106" s="9"/>
-      <c r="D106" s="38"/>
-      <c r="E106" s="38"/>
-      <c r="F106" s="39"/>
+      <c r="D106" s="42"/>
+      <c r="E106" s="42"/>
+      <c r="F106" s="43"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
         <v>105</v>
       </c>
       <c r="B107" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C107" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D107" s="24" t="s">
-        <v>64</v>
-      </c>
-      <c r="E107" s="34"/>
-      <c r="F107" s="35"/>
+        <v>32</v>
+      </c>
+      <c r="C107" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="D107" s="29" t="s">
+        <v>99</v>
+      </c>
+      <c r="E107" s="35"/>
+      <c r="F107" s="36"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
         <v>106</v>
       </c>
       <c r="B108" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C108" s="31"/>
-      <c r="D108" s="36"/>
-      <c r="E108" s="36"/>
-      <c r="F108" s="37"/>
+        <v>31</v>
+      </c>
+      <c r="C108" s="27"/>
+      <c r="D108" s="37"/>
+      <c r="E108" s="37"/>
+      <c r="F108" s="38"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
         <v>107</v>
       </c>
       <c r="B109" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C109" s="31"/>
-      <c r="D109" s="36"/>
-      <c r="E109" s="36"/>
-      <c r="F109" s="37"/>
+        <v>34</v>
+      </c>
+      <c r="C109" s="27"/>
+      <c r="D109" s="37"/>
+      <c r="E109" s="37"/>
+      <c r="F109" s="38"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
         <v>108</v>
       </c>
       <c r="B110" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C110" s="31"/>
-      <c r="D110" s="36"/>
-      <c r="E110" s="36"/>
-      <c r="F110" s="37"/>
+        <v>35</v>
+      </c>
+      <c r="C110" s="27"/>
+      <c r="D110" s="37"/>
+      <c r="E110" s="37"/>
+      <c r="F110" s="38"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
         <v>109</v>
       </c>
       <c r="B111" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C111" s="31"/>
-      <c r="D111" s="36"/>
-      <c r="E111" s="36"/>
-      <c r="F111" s="37"/>
+        <v>36</v>
+      </c>
+      <c r="C111" s="27"/>
+      <c r="D111" s="37"/>
+      <c r="E111" s="37"/>
+      <c r="F111" s="38"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
         <v>110</v>
       </c>
       <c r="B112" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C112" s="31"/>
-      <c r="D112" s="36"/>
-      <c r="E112" s="36"/>
-      <c r="F112" s="37"/>
+        <v>33</v>
+      </c>
+      <c r="C112" s="27"/>
+      <c r="D112" s="37"/>
+      <c r="E112" s="37"/>
+      <c r="F112" s="38"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
         <v>111</v>
       </c>
       <c r="B113" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C113" s="31"/>
-      <c r="D113" s="36"/>
-      <c r="E113" s="36"/>
-      <c r="F113" s="37"/>
+        <v>37</v>
+      </c>
+      <c r="C113" s="27"/>
+      <c r="D113" s="37"/>
+      <c r="E113" s="37"/>
+      <c r="F113" s="38"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
         <v>112</v>
       </c>
       <c r="B114" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C114" s="32"/>
-      <c r="D114" s="36"/>
-      <c r="E114" s="36"/>
-      <c r="F114" s="37"/>
+        <v>38</v>
+      </c>
+      <c r="C114" s="28"/>
+      <c r="D114" s="37"/>
+      <c r="E114" s="37"/>
+      <c r="F114" s="38"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
@@ -2459,251 +2656,251 @@
         <v>11</v>
       </c>
       <c r="C115" s="7"/>
-      <c r="D115" s="36"/>
-      <c r="E115" s="36"/>
-      <c r="F115" s="37"/>
+      <c r="D115" s="37"/>
+      <c r="E115" s="37"/>
+      <c r="F115" s="38"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
         <v>114</v>
       </c>
       <c r="B116" s="6" t="s">
-        <v>55</v>
+        <v>48</v>
       </c>
       <c r="C116" s="7"/>
-      <c r="D116" s="36"/>
-      <c r="E116" s="36"/>
-      <c r="F116" s="37"/>
+      <c r="D116" s="37"/>
+      <c r="E116" s="37"/>
+      <c r="F116" s="38"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
         <v>115</v>
       </c>
       <c r="B117" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C117" s="7"/>
-      <c r="D117" s="36"/>
-      <c r="E117" s="36"/>
-      <c r="F117" s="37"/>
+      <c r="D117" s="37"/>
+      <c r="E117" s="37"/>
+      <c r="F117" s="38"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
         <v>116</v>
       </c>
       <c r="B118" s="6" t="s">
-        <v>58</v>
+        <v>51</v>
       </c>
       <c r="C118" s="7"/>
-      <c r="D118" s="36"/>
-      <c r="E118" s="36"/>
-      <c r="F118" s="37"/>
+      <c r="D118" s="37"/>
+      <c r="E118" s="37"/>
+      <c r="F118" s="38"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
         <v>117</v>
       </c>
       <c r="B119" s="6" t="s">
-        <v>36</v>
+        <v>33</v>
       </c>
       <c r="C119" s="7"/>
-      <c r="D119" s="36"/>
-      <c r="E119" s="36"/>
-      <c r="F119" s="37"/>
+      <c r="D119" s="37"/>
+      <c r="E119" s="37"/>
+      <c r="F119" s="38"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
         <v>118</v>
       </c>
       <c r="B120" s="6" t="s">
-        <v>59</v>
+        <v>52</v>
       </c>
       <c r="C120" s="7"/>
-      <c r="D120" s="36"/>
-      <c r="E120" s="36"/>
-      <c r="F120" s="37"/>
+      <c r="D120" s="37"/>
+      <c r="E120" s="37"/>
+      <c r="F120" s="38"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
         <v>119</v>
       </c>
       <c r="B121" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C121" s="7"/>
-      <c r="D121" s="36"/>
-      <c r="E121" s="36"/>
-      <c r="F121" s="37"/>
+      <c r="D121" s="37"/>
+      <c r="E121" s="37"/>
+      <c r="F121" s="38"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
         <v>120</v>
       </c>
       <c r="B122" s="6" t="s">
-        <v>60</v>
+        <v>53</v>
       </c>
       <c r="C122" s="7"/>
-      <c r="D122" s="36"/>
-      <c r="E122" s="36"/>
-      <c r="F122" s="37"/>
+      <c r="D122" s="37"/>
+      <c r="E122" s="37"/>
+      <c r="F122" s="38"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
         <v>121</v>
       </c>
       <c r="B123" s="6" t="s">
-        <v>57</v>
+        <v>50</v>
       </c>
       <c r="C123" s="7"/>
-      <c r="D123" s="36"/>
-      <c r="E123" s="36"/>
-      <c r="F123" s="37"/>
+      <c r="D123" s="37"/>
+      <c r="E123" s="37"/>
+      <c r="F123" s="38"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
         <v>122</v>
       </c>
       <c r="B124" s="6" t="s">
-        <v>46</v>
+        <v>42</v>
       </c>
       <c r="C124" s="7"/>
-      <c r="D124" s="36"/>
-      <c r="E124" s="36"/>
-      <c r="F124" s="37"/>
+      <c r="D124" s="37"/>
+      <c r="E124" s="37"/>
+      <c r="F124" s="38"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
         <v>123</v>
       </c>
       <c r="B125" s="6" t="s">
-        <v>61</v>
+        <v>54</v>
       </c>
       <c r="C125" s="7"/>
-      <c r="D125" s="36"/>
-      <c r="E125" s="36"/>
-      <c r="F125" s="37"/>
+      <c r="D125" s="37"/>
+      <c r="E125" s="37"/>
+      <c r="F125" s="38"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
         <v>124</v>
       </c>
       <c r="B126" s="6" t="s">
-        <v>62</v>
+        <v>55</v>
       </c>
       <c r="C126" s="7"/>
-      <c r="D126" s="36"/>
-      <c r="E126" s="36"/>
-      <c r="F126" s="37"/>
+      <c r="D126" s="37"/>
+      <c r="E126" s="37"/>
+      <c r="F126" s="38"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
         <v>125</v>
       </c>
       <c r="B127" s="6" t="s">
-        <v>63</v>
+        <v>56</v>
       </c>
       <c r="C127" s="7"/>
-      <c r="D127" s="36"/>
-      <c r="E127" s="36"/>
-      <c r="F127" s="37"/>
+      <c r="D127" s="37"/>
+      <c r="E127" s="37"/>
+      <c r="F127" s="38"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="15">
         <v>126</v>
       </c>
       <c r="B128" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C128" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D128" s="36"/>
-      <c r="E128" s="36"/>
-      <c r="F128" s="37"/>
+        <v>35</v>
+      </c>
+      <c r="C128" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D128" s="37"/>
+      <c r="E128" s="37"/>
+      <c r="F128" s="38"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
         <v>127</v>
       </c>
       <c r="B129" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C129" s="31"/>
-      <c r="D129" s="36"/>
-      <c r="E129" s="36"/>
-      <c r="F129" s="37"/>
+        <v>36</v>
+      </c>
+      <c r="C129" s="27"/>
+      <c r="D129" s="37"/>
+      <c r="E129" s="37"/>
+      <c r="F129" s="38"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
         <v>128</v>
       </c>
       <c r="B130" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C130" s="31"/>
-      <c r="D130" s="36"/>
-      <c r="E130" s="36"/>
-      <c r="F130" s="37"/>
+        <v>33</v>
+      </c>
+      <c r="C130" s="27"/>
+      <c r="D130" s="37"/>
+      <c r="E130" s="37"/>
+      <c r="F130" s="38"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
         <v>129</v>
       </c>
       <c r="B131" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C131" s="31"/>
-      <c r="D131" s="36"/>
-      <c r="E131" s="36"/>
-      <c r="F131" s="37"/>
+        <v>64</v>
+      </c>
+      <c r="C131" s="27"/>
+      <c r="D131" s="37"/>
+      <c r="E131" s="37"/>
+      <c r="F131" s="38"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
         <v>130</v>
       </c>
       <c r="B132" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C132" s="31"/>
-      <c r="D132" s="36"/>
-      <c r="E132" s="36"/>
-      <c r="F132" s="37"/>
+        <v>41</v>
+      </c>
+      <c r="C132" s="27"/>
+      <c r="D132" s="37"/>
+      <c r="E132" s="37"/>
+      <c r="F132" s="38"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
         <v>131</v>
       </c>
       <c r="B133" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C133" s="31"/>
-      <c r="D133" s="36"/>
-      <c r="E133" s="36"/>
-      <c r="F133" s="37"/>
+        <v>32</v>
+      </c>
+      <c r="C133" s="27"/>
+      <c r="D133" s="37"/>
+      <c r="E133" s="37"/>
+      <c r="F133" s="38"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
         <v>132</v>
       </c>
       <c r="B134" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C134" s="31"/>
-      <c r="D134" s="36"/>
-      <c r="E134" s="36"/>
-      <c r="F134" s="37"/>
+        <v>42</v>
+      </c>
+      <c r="C134" s="27"/>
+      <c r="D134" s="37"/>
+      <c r="E134" s="37"/>
+      <c r="F134" s="38"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
         <v>133</v>
       </c>
       <c r="B135" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C135" s="32"/>
-      <c r="D135" s="36"/>
-      <c r="E135" s="36"/>
-      <c r="F135" s="37"/>
+        <v>34</v>
+      </c>
+      <c r="C135" s="28"/>
+      <c r="D135" s="37"/>
+      <c r="E135" s="37"/>
+      <c r="F135" s="38"/>
     </row>
     <row r="136" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
@@ -2713,766 +2910,1482 @@
         <v>10</v>
       </c>
       <c r="C136" s="7"/>
-      <c r="D136" s="36"/>
-      <c r="E136" s="36"/>
-      <c r="F136" s="37"/>
+      <c r="D136" s="37"/>
+      <c r="E136" s="37"/>
+      <c r="F136" s="38"/>
     </row>
     <row r="137" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
         <v>135</v>
       </c>
       <c r="B137" s="22" t="s">
-        <v>35</v>
-      </c>
-      <c r="C137" s="30" t="s">
-        <v>47</v>
-      </c>
-      <c r="D137" s="24" t="s">
-        <v>71</v>
-      </c>
-      <c r="E137" s="24"/>
-      <c r="F137" s="25"/>
+        <v>32</v>
+      </c>
+      <c r="C137" s="46" t="s">
+        <v>93</v>
+      </c>
+      <c r="D137" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E137" s="29"/>
+      <c r="F137" s="30"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
         <v>136</v>
       </c>
       <c r="B138" s="6" t="s">
-        <v>33</v>
-      </c>
-      <c r="C138" s="31"/>
-      <c r="D138" s="26"/>
-      <c r="E138" s="26"/>
-      <c r="F138" s="27"/>
+        <v>31</v>
+      </c>
+      <c r="C138" s="27"/>
+      <c r="D138" s="31"/>
+      <c r="E138" s="31"/>
+      <c r="F138" s="32"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
         <v>137</v>
       </c>
       <c r="B139" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="C139" s="31"/>
-      <c r="D139" s="26"/>
-      <c r="E139" s="26"/>
-      <c r="F139" s="27"/>
+        <v>34</v>
+      </c>
+      <c r="C139" s="27"/>
+      <c r="D139" s="31"/>
+      <c r="E139" s="31"/>
+      <c r="F139" s="32"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
         <v>138</v>
       </c>
       <c r="B140" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="C140" s="31"/>
-      <c r="D140" s="26"/>
-      <c r="E140" s="26"/>
-      <c r="F140" s="27"/>
+        <v>35</v>
+      </c>
+      <c r="C140" s="27"/>
+      <c r="D140" s="31"/>
+      <c r="E140" s="31"/>
+      <c r="F140" s="32"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
         <v>139</v>
       </c>
       <c r="B141" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C141" s="31"/>
-      <c r="D141" s="26"/>
-      <c r="E141" s="26"/>
-      <c r="F141" s="27"/>
+        <v>36</v>
+      </c>
+      <c r="C141" s="27"/>
+      <c r="D141" s="31"/>
+      <c r="E141" s="31"/>
+      <c r="F141" s="32"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
         <v>140</v>
       </c>
       <c r="B142" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C142" s="31"/>
-      <c r="D142" s="26"/>
-      <c r="E142" s="26"/>
-      <c r="F142" s="27"/>
+        <v>33</v>
+      </c>
+      <c r="C142" s="27"/>
+      <c r="D142" s="31"/>
+      <c r="E142" s="31"/>
+      <c r="F142" s="32"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
         <v>141</v>
       </c>
       <c r="B143" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C143" s="31"/>
-      <c r="D143" s="26"/>
-      <c r="E143" s="26"/>
-      <c r="F143" s="27"/>
+        <v>37</v>
+      </c>
+      <c r="C143" s="27"/>
+      <c r="D143" s="31"/>
+      <c r="E143" s="31"/>
+      <c r="F143" s="32"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
         <v>142</v>
       </c>
       <c r="B144" s="16" t="s">
-        <v>41</v>
-      </c>
-      <c r="C144" s="32"/>
-      <c r="D144" s="26"/>
-      <c r="E144" s="26"/>
-      <c r="F144" s="27"/>
+        <v>38</v>
+      </c>
+      <c r="C144" s="28"/>
+      <c r="D144" s="31"/>
+      <c r="E144" s="31"/>
+      <c r="F144" s="32"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
         <v>143</v>
       </c>
       <c r="B145" s="6" t="s">
-        <v>65</v>
+        <v>57</v>
       </c>
       <c r="C145" s="7"/>
-      <c r="D145" s="26"/>
-      <c r="E145" s="26"/>
-      <c r="F145" s="27"/>
+      <c r="D145" s="31"/>
+      <c r="E145" s="31"/>
+      <c r="F145" s="32"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
         <v>144</v>
       </c>
       <c r="B146" s="6" t="s">
-        <v>66</v>
+        <v>58</v>
       </c>
       <c r="C146" s="7"/>
-      <c r="D146" s="26"/>
-      <c r="E146" s="26"/>
-      <c r="F146" s="27"/>
+      <c r="D146" s="31"/>
+      <c r="E146" s="31"/>
+      <c r="F146" s="32"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
         <v>145</v>
       </c>
       <c r="B147" s="6" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
       <c r="C147" s="7"/>
-      <c r="D147" s="26"/>
-      <c r="E147" s="26"/>
-      <c r="F147" s="27"/>
+      <c r="D147" s="31"/>
+      <c r="E147" s="31"/>
+      <c r="F147" s="32"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
         <v>146</v>
       </c>
       <c r="B148" s="6" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
       <c r="C148" s="7"/>
-      <c r="D148" s="26"/>
-      <c r="E148" s="26"/>
-      <c r="F148" s="27"/>
+      <c r="D148" s="31"/>
+      <c r="E148" s="31"/>
+      <c r="F148" s="32"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
         <v>147</v>
       </c>
       <c r="B149" s="18" t="s">
-        <v>72</v>
-      </c>
-      <c r="C149" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="D149" s="26"/>
-      <c r="E149" s="26"/>
-      <c r="F149" s="27"/>
+        <v>61</v>
+      </c>
+      <c r="C149" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D149" s="31"/>
+      <c r="E149" s="31"/>
+      <c r="F149" s="32"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
         <v>148</v>
       </c>
       <c r="B150" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C150" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D150" s="26"/>
-      <c r="E150" s="26"/>
-      <c r="F150" s="27"/>
+        <v>35</v>
+      </c>
+      <c r="C150" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D150" s="31"/>
+      <c r="E150" s="31"/>
+      <c r="F150" s="32"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
         <v>149</v>
       </c>
       <c r="B151" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C151" s="31"/>
-      <c r="D151" s="26"/>
-      <c r="E151" s="26"/>
-      <c r="F151" s="27"/>
+        <v>36</v>
+      </c>
+      <c r="C151" s="27"/>
+      <c r="D151" s="31"/>
+      <c r="E151" s="31"/>
+      <c r="F151" s="32"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
         <v>150</v>
       </c>
       <c r="B152" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C152" s="31"/>
-      <c r="D152" s="26"/>
-      <c r="E152" s="26"/>
-      <c r="F152" s="27"/>
+        <v>33</v>
+      </c>
+      <c r="C152" s="27"/>
+      <c r="D152" s="31"/>
+      <c r="E152" s="31"/>
+      <c r="F152" s="32"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
         <v>151</v>
       </c>
       <c r="B153" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C153" s="31"/>
-      <c r="D153" s="26"/>
-      <c r="E153" s="26"/>
-      <c r="F153" s="27"/>
+        <v>64</v>
+      </c>
+      <c r="C153" s="27"/>
+      <c r="D153" s="31"/>
+      <c r="E153" s="31"/>
+      <c r="F153" s="32"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
         <v>152</v>
       </c>
       <c r="B154" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C154" s="31"/>
-      <c r="D154" s="26"/>
-      <c r="E154" s="26"/>
-      <c r="F154" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="C154" s="27"/>
+      <c r="D154" s="31"/>
+      <c r="E154" s="31"/>
+      <c r="F154" s="32"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
         <v>153</v>
       </c>
       <c r="B155" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C155" s="31"/>
-      <c r="D155" s="26"/>
-      <c r="E155" s="26"/>
-      <c r="F155" s="27"/>
+        <v>32</v>
+      </c>
+      <c r="C155" s="27"/>
+      <c r="D155" s="31"/>
+      <c r="E155" s="31"/>
+      <c r="F155" s="32"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
         <v>154</v>
       </c>
       <c r="B156" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C156" s="31"/>
-      <c r="D156" s="26"/>
-      <c r="E156" s="26"/>
-      <c r="F156" s="27"/>
+        <v>42</v>
+      </c>
+      <c r="C156" s="27"/>
+      <c r="D156" s="31"/>
+      <c r="E156" s="31"/>
+      <c r="F156" s="32"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
         <v>155</v>
       </c>
       <c r="B157" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C157" s="32"/>
-      <c r="D157" s="26"/>
-      <c r="E157" s="26"/>
-      <c r="F157" s="27"/>
+        <v>34</v>
+      </c>
+      <c r="C157" s="28"/>
+      <c r="D157" s="31"/>
+      <c r="E157" s="31"/>
+      <c r="F157" s="32"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="15">
         <v>156</v>
       </c>
       <c r="B158" s="16" t="s">
-        <v>67</v>
-      </c>
-      <c r="C158" s="44" t="s">
-        <v>68</v>
-      </c>
-      <c r="D158" s="26"/>
-      <c r="E158" s="26"/>
-      <c r="F158" s="27"/>
+        <v>59</v>
+      </c>
+      <c r="C158" s="25" t="s">
+        <v>101</v>
+      </c>
+      <c r="D158" s="31"/>
+      <c r="E158" s="31"/>
+      <c r="F158" s="32"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
         <v>157</v>
       </c>
       <c r="B159" s="21" t="s">
-        <v>72</v>
-      </c>
-      <c r="C159" s="43" t="s">
-        <v>75</v>
-      </c>
-      <c r="D159" s="26"/>
-      <c r="E159" s="26"/>
-      <c r="F159" s="27"/>
+        <v>61</v>
+      </c>
+      <c r="C159" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="D159" s="31"/>
+      <c r="E159" s="31"/>
+      <c r="F159" s="32"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
         <v>158</v>
       </c>
       <c r="B160" s="23" t="s">
-        <v>38</v>
-      </c>
-      <c r="C160" s="33" t="s">
-        <v>48</v>
-      </c>
-      <c r="D160" s="26"/>
-      <c r="E160" s="26"/>
-      <c r="F160" s="27"/>
+        <v>35</v>
+      </c>
+      <c r="C160" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D160" s="31"/>
+      <c r="E160" s="31"/>
+      <c r="F160" s="32"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
         <v>159</v>
       </c>
       <c r="B161" s="6" t="s">
-        <v>39</v>
-      </c>
-      <c r="C161" s="31"/>
-      <c r="D161" s="26"/>
-      <c r="E161" s="26"/>
-      <c r="F161" s="27"/>
+        <v>36</v>
+      </c>
+      <c r="C161" s="27"/>
+      <c r="D161" s="31"/>
+      <c r="E161" s="31"/>
+      <c r="F161" s="32"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
         <v>160</v>
       </c>
       <c r="B162" s="6" t="s">
-        <v>36</v>
-      </c>
-      <c r="C162" s="31"/>
-      <c r="D162" s="26"/>
-      <c r="E162" s="26"/>
-      <c r="F162" s="27"/>
+        <v>33</v>
+      </c>
+      <c r="C162" s="27"/>
+      <c r="D162" s="31"/>
+      <c r="E162" s="31"/>
+      <c r="F162" s="32"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
         <v>161</v>
       </c>
       <c r="B163" s="6" t="s">
-        <v>44</v>
-      </c>
-      <c r="C163" s="31"/>
-      <c r="D163" s="26"/>
-      <c r="E163" s="26"/>
-      <c r="F163" s="27"/>
+        <v>64</v>
+      </c>
+      <c r="C163" s="27"/>
+      <c r="D163" s="31"/>
+      <c r="E163" s="31"/>
+      <c r="F163" s="32"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
         <v>162</v>
       </c>
       <c r="B164" s="6" t="s">
-        <v>45</v>
-      </c>
-      <c r="C164" s="31"/>
-      <c r="D164" s="26"/>
-      <c r="E164" s="26"/>
-      <c r="F164" s="27"/>
+        <v>41</v>
+      </c>
+      <c r="C164" s="27"/>
+      <c r="D164" s="31"/>
+      <c r="E164" s="31"/>
+      <c r="F164" s="32"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
         <v>163</v>
       </c>
       <c r="B165" s="6" t="s">
-        <v>35</v>
-      </c>
-      <c r="C165" s="31"/>
-      <c r="D165" s="26"/>
-      <c r="E165" s="26"/>
-      <c r="F165" s="27"/>
+        <v>32</v>
+      </c>
+      <c r="C165" s="27"/>
+      <c r="D165" s="31"/>
+      <c r="E165" s="31"/>
+      <c r="F165" s="32"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
         <v>164</v>
       </c>
       <c r="B166" s="6" t="s">
-        <v>46</v>
-      </c>
-      <c r="C166" s="31"/>
-      <c r="D166" s="26"/>
-      <c r="E166" s="26"/>
-      <c r="F166" s="27"/>
+        <v>42</v>
+      </c>
+      <c r="C166" s="27"/>
+      <c r="D166" s="31"/>
+      <c r="E166" s="31"/>
+      <c r="F166" s="32"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
         <v>165</v>
       </c>
       <c r="B167" s="16" t="s">
-        <v>37</v>
-      </c>
-      <c r="C167" s="32"/>
-      <c r="D167" s="26"/>
-      <c r="E167" s="26"/>
-      <c r="F167" s="27"/>
+        <v>34</v>
+      </c>
+      <c r="C167" s="28"/>
+      <c r="D167" s="31"/>
+      <c r="E167" s="31"/>
+      <c r="F167" s="32"/>
     </row>
     <row r="168" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
         <v>166</v>
       </c>
       <c r="B168" s="8" t="s">
-        <v>69</v>
-      </c>
-      <c r="C168" s="45" t="s">
-        <v>70</v>
-      </c>
-      <c r="D168" s="28"/>
-      <c r="E168" s="28"/>
-      <c r="F168" s="29"/>
+        <v>60</v>
+      </c>
+      <c r="C168" s="26" t="s">
+        <v>102</v>
+      </c>
+      <c r="D168" s="33"/>
+      <c r="E168" s="33"/>
+      <c r="F168" s="34"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
         <v>167</v>
       </c>
+      <c r="B169" s="22" t="s">
+        <v>32</v>
+      </c>
+      <c r="C169" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D169" s="29" t="s">
+        <v>104</v>
+      </c>
+      <c r="E169" s="35"/>
+      <c r="F169" s="36"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
         <v>168</v>
       </c>
+      <c r="B170" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C170" s="27"/>
+      <c r="D170" s="37"/>
+      <c r="E170" s="37"/>
+      <c r="F170" s="38"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
         <v>169</v>
       </c>
+      <c r="B171" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C171" s="27"/>
+      <c r="D171" s="37"/>
+      <c r="E171" s="37"/>
+      <c r="F171" s="38"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
         <v>170</v>
       </c>
+      <c r="B172" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="C172" s="27"/>
+      <c r="D172" s="37"/>
+      <c r="E172" s="37"/>
+      <c r="F172" s="38"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
         <v>171</v>
       </c>
+      <c r="B173" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C173" s="27"/>
+      <c r="D173" s="37"/>
+      <c r="E173" s="37"/>
+      <c r="F173" s="38"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
         <v>172</v>
       </c>
+      <c r="B174" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C174" s="27"/>
+      <c r="D174" s="37"/>
+      <c r="E174" s="37"/>
+      <c r="F174" s="38"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
         <v>173</v>
       </c>
+      <c r="B175" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="C175" s="27"/>
+      <c r="D175" s="37"/>
+      <c r="E175" s="37"/>
+      <c r="F175" s="38"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
         <v>174</v>
       </c>
-    </row>
-    <row r="177" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B176" s="16" t="s">
+        <v>38</v>
+      </c>
+      <c r="C176" s="28"/>
+      <c r="D176" s="37"/>
+      <c r="E176" s="37"/>
+      <c r="F176" s="38"/>
+    </row>
+    <row r="177" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
         <v>175</v>
       </c>
-    </row>
-    <row r="178" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B177" s="6" t="s">
+        <v>65</v>
+      </c>
+      <c r="C177" s="7"/>
+      <c r="D177" s="37"/>
+      <c r="E177" s="37"/>
+      <c r="F177" s="38"/>
+      <c r="H177" s="48" t="s">
+        <v>109</v>
+      </c>
+      <c r="I177" s="44"/>
+      <c r="J177" s="44"/>
+      <c r="K177" s="44"/>
+      <c r="L177" s="44"/>
+      <c r="M177" s="44"/>
+      <c r="N177" s="44"/>
+      <c r="O177" s="44"/>
+      <c r="P177" s="44"/>
+      <c r="Q177" s="44"/>
+      <c r="R177" s="44"/>
+    </row>
+    <row r="178" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
         <v>176</v>
       </c>
-    </row>
-    <row r="179" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A179" s="1">
+      <c r="B178" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C178" s="7"/>
+      <c r="D178" s="37"/>
+      <c r="E178" s="37"/>
+      <c r="F178" s="38"/>
+      <c r="H178" s="44"/>
+      <c r="I178" s="44"/>
+      <c r="J178" s="44"/>
+      <c r="K178" s="44"/>
+      <c r="L178" s="44"/>
+      <c r="M178" s="44"/>
+      <c r="N178" s="44"/>
+      <c r="O178" s="44"/>
+      <c r="P178" s="44"/>
+      <c r="Q178" s="44"/>
+      <c r="R178" s="44"/>
+    </row>
+    <row r="179" spans="1:18" x14ac:dyDescent="0.2">
+      <c r="A179" s="2">
         <v>177</v>
       </c>
-    </row>
-    <row r="180" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B179" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C179" s="7" t="s">
+        <v>105</v>
+      </c>
+      <c r="D179" s="37"/>
+      <c r="E179" s="37"/>
+      <c r="F179" s="38"/>
+      <c r="H179" s="44"/>
+      <c r="I179" s="44"/>
+      <c r="J179" s="44"/>
+      <c r="K179" s="44"/>
+      <c r="L179" s="44"/>
+      <c r="M179" s="44"/>
+      <c r="N179" s="44"/>
+      <c r="O179" s="44"/>
+      <c r="P179" s="44"/>
+      <c r="Q179" s="44"/>
+      <c r="R179" s="44"/>
+    </row>
+    <row r="180" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
         <v>178</v>
       </c>
-    </row>
-    <row r="181" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B180" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C180" s="7"/>
+      <c r="D180" s="37"/>
+      <c r="E180" s="37"/>
+      <c r="F180" s="38"/>
+      <c r="H180" s="44"/>
+      <c r="I180" s="44"/>
+      <c r="J180" s="44"/>
+      <c r="K180" s="44"/>
+      <c r="L180" s="44"/>
+      <c r="M180" s="44"/>
+      <c r="N180" s="44"/>
+      <c r="O180" s="44"/>
+      <c r="P180" s="44"/>
+      <c r="Q180" s="44"/>
+      <c r="R180" s="44"/>
+    </row>
+    <row r="181" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
         <v>179</v>
       </c>
-    </row>
-    <row r="182" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B181" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C181" s="7"/>
+      <c r="D181" s="37"/>
+      <c r="E181" s="37"/>
+      <c r="F181" s="38"/>
+      <c r="H181" s="44"/>
+      <c r="I181" s="44"/>
+      <c r="J181" s="44"/>
+      <c r="K181" s="44"/>
+      <c r="L181" s="44"/>
+      <c r="M181" s="44"/>
+      <c r="N181" s="44"/>
+      <c r="O181" s="44"/>
+      <c r="P181" s="44"/>
+      <c r="Q181" s="44"/>
+      <c r="R181" s="44"/>
+    </row>
+    <row r="182" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
         <v>180</v>
       </c>
-    </row>
-    <row r="183" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B182" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C182" s="7"/>
+      <c r="D182" s="37"/>
+      <c r="E182" s="37"/>
+      <c r="F182" s="38"/>
+      <c r="H182" s="44"/>
+      <c r="I182" s="44"/>
+      <c r="J182" s="44"/>
+      <c r="K182" s="44"/>
+      <c r="L182" s="44"/>
+      <c r="M182" s="44"/>
+      <c r="N182" s="44"/>
+      <c r="O182" s="44"/>
+      <c r="P182" s="44"/>
+      <c r="Q182" s="44"/>
+      <c r="R182" s="44"/>
+    </row>
+    <row r="183" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
         <v>181</v>
       </c>
-    </row>
-    <row r="184" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B183" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C183" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="D183" s="37"/>
+      <c r="E183" s="37"/>
+      <c r="F183" s="38"/>
+      <c r="H183" s="44"/>
+      <c r="I183" s="44"/>
+      <c r="J183" s="44"/>
+      <c r="K183" s="44"/>
+      <c r="L183" s="44"/>
+      <c r="M183" s="44"/>
+      <c r="N183" s="44"/>
+      <c r="O183" s="44"/>
+      <c r="P183" s="44"/>
+      <c r="Q183" s="44"/>
+      <c r="R183" s="44"/>
+    </row>
+    <row r="184" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
         <v>182</v>
       </c>
-    </row>
-    <row r="185" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B184" s="6" t="s">
+        <v>70</v>
+      </c>
+      <c r="C184" s="7"/>
+      <c r="D184" s="37"/>
+      <c r="E184" s="37"/>
+      <c r="F184" s="38"/>
+      <c r="H184" s="44"/>
+      <c r="I184" s="44"/>
+      <c r="J184" s="44"/>
+      <c r="K184" s="44"/>
+      <c r="L184" s="44"/>
+      <c r="M184" s="44"/>
+      <c r="N184" s="44"/>
+      <c r="O184" s="44"/>
+      <c r="P184" s="44"/>
+      <c r="Q184" s="44"/>
+      <c r="R184" s="44"/>
+    </row>
+    <row r="185" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
         <v>183</v>
       </c>
-    </row>
-    <row r="186" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B185" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C185" s="7"/>
+      <c r="D185" s="37"/>
+      <c r="E185" s="37"/>
+      <c r="F185" s="38"/>
+      <c r="H185" s="44"/>
+      <c r="I185" s="44"/>
+      <c r="J185" s="44"/>
+      <c r="K185" s="44"/>
+      <c r="L185" s="44"/>
+      <c r="M185" s="44"/>
+      <c r="N185" s="44"/>
+      <c r="O185" s="44"/>
+      <c r="P185" s="44"/>
+      <c r="Q185" s="44"/>
+      <c r="R185" s="44"/>
+    </row>
+    <row r="186" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
         <v>184</v>
       </c>
-    </row>
-    <row r="187" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B186" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C186" s="7"/>
+      <c r="D186" s="37"/>
+      <c r="E186" s="37"/>
+      <c r="F186" s="38"/>
+      <c r="H186" s="44"/>
+      <c r="I186" s="44"/>
+      <c r="J186" s="44"/>
+      <c r="K186" s="44"/>
+      <c r="L186" s="44"/>
+      <c r="M186" s="44"/>
+      <c r="N186" s="44"/>
+      <c r="O186" s="44"/>
+      <c r="P186" s="44"/>
+      <c r="Q186" s="44"/>
+      <c r="R186" s="44"/>
+    </row>
+    <row r="187" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
         <v>185</v>
       </c>
-    </row>
-    <row r="188" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B187" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C187" s="7"/>
+      <c r="D187" s="37"/>
+      <c r="E187" s="37"/>
+      <c r="F187" s="38"/>
+      <c r="H187" s="44"/>
+      <c r="I187" s="44"/>
+      <c r="J187" s="44"/>
+      <c r="K187" s="44"/>
+      <c r="L187" s="44"/>
+      <c r="M187" s="44"/>
+      <c r="N187" s="44"/>
+      <c r="O187" s="44"/>
+      <c r="P187" s="44"/>
+      <c r="Q187" s="44"/>
+      <c r="R187" s="44"/>
+    </row>
+    <row r="188" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
         <v>186</v>
       </c>
-    </row>
-    <row r="189" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B188" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="C188" s="7"/>
+      <c r="D188" s="37"/>
+      <c r="E188" s="37"/>
+      <c r="F188" s="38"/>
+      <c r="H188" s="44"/>
+      <c r="I188" s="44"/>
+      <c r="J188" s="44"/>
+      <c r="K188" s="44"/>
+      <c r="L188" s="44"/>
+      <c r="M188" s="44"/>
+      <c r="N188" s="44"/>
+      <c r="O188" s="44"/>
+      <c r="P188" s="44"/>
+      <c r="Q188" s="44"/>
+      <c r="R188" s="44"/>
+    </row>
+    <row r="189" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
         <v>187</v>
       </c>
-    </row>
-    <row r="190" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B189" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="C189" s="7" t="s">
+        <v>106</v>
+      </c>
+      <c r="D189" s="37"/>
+      <c r="E189" s="37"/>
+      <c r="F189" s="38"/>
+      <c r="H189" s="44"/>
+      <c r="I189" s="44"/>
+      <c r="J189" s="44"/>
+      <c r="K189" s="44"/>
+      <c r="L189" s="44"/>
+      <c r="M189" s="44"/>
+      <c r="N189" s="44"/>
+      <c r="O189" s="44"/>
+      <c r="P189" s="44"/>
+      <c r="Q189" s="44"/>
+      <c r="R189" s="44"/>
+    </row>
+    <row r="190" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
         <v>188</v>
       </c>
-    </row>
-    <row r="191" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B190" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="C190" s="7"/>
+      <c r="D190" s="37"/>
+      <c r="E190" s="37"/>
+      <c r="F190" s="38"/>
+      <c r="H190" s="44"/>
+      <c r="I190" s="44"/>
+      <c r="J190" s="44"/>
+      <c r="K190" s="44"/>
+      <c r="L190" s="44"/>
+      <c r="M190" s="44"/>
+      <c r="N190" s="44"/>
+      <c r="O190" s="44"/>
+      <c r="P190" s="44"/>
+      <c r="Q190" s="44"/>
+      <c r="R190" s="44"/>
+    </row>
+    <row r="191" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
         <v>189</v>
       </c>
-    </row>
-    <row r="192" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B191" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C191" s="7"/>
+      <c r="D191" s="37"/>
+      <c r="E191" s="37"/>
+      <c r="F191" s="38"/>
+      <c r="H191" s="44"/>
+      <c r="I191" s="44"/>
+      <c r="J191" s="44"/>
+      <c r="K191" s="44"/>
+      <c r="L191" s="44"/>
+      <c r="M191" s="44"/>
+      <c r="N191" s="44"/>
+      <c r="O191" s="44"/>
+      <c r="P191" s="44"/>
+      <c r="Q191" s="44"/>
+      <c r="R191" s="44"/>
+    </row>
+    <row r="192" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
         <v>190</v>
       </c>
-    </row>
-    <row r="193" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B192" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C192" s="7"/>
+      <c r="D192" s="37"/>
+      <c r="E192" s="37"/>
+      <c r="F192" s="38"/>
+      <c r="H192" s="44"/>
+      <c r="I192" s="44"/>
+      <c r="J192" s="44"/>
+      <c r="K192" s="44"/>
+      <c r="L192" s="44"/>
+      <c r="M192" s="44"/>
+      <c r="N192" s="44"/>
+      <c r="O192" s="44"/>
+      <c r="P192" s="44"/>
+      <c r="Q192" s="44"/>
+      <c r="R192" s="44"/>
+    </row>
+    <row r="193" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
         <v>191</v>
       </c>
-    </row>
-    <row r="194" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B193" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C193" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D193" s="37"/>
+      <c r="E193" s="37"/>
+      <c r="F193" s="38"/>
+      <c r="H193" s="44"/>
+      <c r="I193" s="44"/>
+      <c r="J193" s="44"/>
+      <c r="K193" s="44"/>
+      <c r="L193" s="44"/>
+      <c r="M193" s="44"/>
+      <c r="N193" s="44"/>
+      <c r="O193" s="44"/>
+      <c r="P193" s="44"/>
+      <c r="Q193" s="44"/>
+      <c r="R193" s="44"/>
+    </row>
+    <row r="194" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
         <v>192</v>
       </c>
-    </row>
-    <row r="195" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B194" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C194" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D194" s="37"/>
+      <c r="E194" s="37"/>
+      <c r="F194" s="38"/>
+      <c r="H194" s="44"/>
+      <c r="I194" s="44"/>
+      <c r="J194" s="44"/>
+      <c r="K194" s="44"/>
+      <c r="L194" s="44"/>
+      <c r="M194" s="44"/>
+      <c r="N194" s="44"/>
+      <c r="O194" s="44"/>
+      <c r="P194" s="44"/>
+      <c r="Q194" s="44"/>
+      <c r="R194" s="44"/>
+    </row>
+    <row r="195" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
         <v>193</v>
       </c>
-    </row>
-    <row r="196" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B195" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="C195" s="7"/>
+      <c r="D195" s="37"/>
+      <c r="E195" s="37"/>
+      <c r="F195" s="38"/>
+      <c r="H195" s="44"/>
+      <c r="I195" s="44"/>
+      <c r="J195" s="44"/>
+      <c r="K195" s="44"/>
+      <c r="L195" s="44"/>
+      <c r="M195" s="44"/>
+      <c r="N195" s="44"/>
+      <c r="O195" s="44"/>
+      <c r="P195" s="44"/>
+      <c r="Q195" s="44"/>
+      <c r="R195" s="44"/>
+    </row>
+    <row r="196" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
-    </row>
-    <row r="197" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B196" s="6" t="s">
+        <v>57</v>
+      </c>
+      <c r="C196" s="7"/>
+      <c r="D196" s="37"/>
+      <c r="E196" s="37"/>
+      <c r="F196" s="38"/>
+      <c r="H196" s="44"/>
+      <c r="I196" s="44"/>
+      <c r="J196" s="44"/>
+      <c r="K196" s="44"/>
+      <c r="L196" s="44"/>
+      <c r="M196" s="44"/>
+      <c r="N196" s="44"/>
+      <c r="O196" s="44"/>
+      <c r="P196" s="44"/>
+      <c r="Q196" s="44"/>
+      <c r="R196" s="44"/>
+    </row>
+    <row r="197" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
         <v>195</v>
       </c>
-    </row>
-    <row r="198" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B197" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C197" s="7"/>
+      <c r="D197" s="37"/>
+      <c r="E197" s="37"/>
+      <c r="F197" s="38"/>
+      <c r="H197" s="44"/>
+      <c r="I197" s="44"/>
+      <c r="J197" s="44"/>
+      <c r="K197" s="44"/>
+      <c r="L197" s="44"/>
+      <c r="M197" s="44"/>
+      <c r="N197" s="44"/>
+      <c r="O197" s="44"/>
+      <c r="P197" s="44"/>
+      <c r="Q197" s="44"/>
+      <c r="R197" s="44"/>
+    </row>
+    <row r="198" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
         <v>196</v>
       </c>
-    </row>
-    <row r="199" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B198" s="6" t="s">
+        <v>81</v>
+      </c>
+      <c r="C198" s="7" t="s">
+        <v>107</v>
+      </c>
+      <c r="D198" s="37"/>
+      <c r="E198" s="37"/>
+      <c r="F198" s="38"/>
+    </row>
+    <row r="199" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
         <v>197</v>
       </c>
-    </row>
-    <row r="200" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B199" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C199" s="7"/>
+      <c r="D199" s="37"/>
+      <c r="E199" s="37"/>
+      <c r="F199" s="38"/>
+    </row>
+    <row r="200" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
         <v>198</v>
       </c>
-    </row>
-    <row r="201" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B200" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="C200" s="7"/>
+      <c r="D200" s="37"/>
+      <c r="E200" s="37"/>
+      <c r="F200" s="38"/>
+    </row>
+    <row r="201" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
         <v>199</v>
       </c>
-    </row>
-    <row r="202" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B201" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="C201" s="7"/>
+      <c r="D201" s="37"/>
+      <c r="E201" s="37"/>
+      <c r="F201" s="38"/>
+    </row>
+    <row r="202" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
         <v>200</v>
       </c>
-    </row>
-    <row r="203" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B202" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="C202" s="7"/>
+      <c r="D202" s="37"/>
+      <c r="E202" s="37"/>
+      <c r="F202" s="38"/>
+    </row>
+    <row r="203" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
         <v>201</v>
       </c>
-    </row>
-    <row r="204" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B203" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="C203" s="7"/>
+      <c r="D203" s="37"/>
+      <c r="E203" s="37"/>
+      <c r="F203" s="38"/>
+    </row>
+    <row r="204" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
-    </row>
-    <row r="205" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B204" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="C204" s="7"/>
+      <c r="D204" s="37"/>
+      <c r="E204" s="37"/>
+      <c r="F204" s="38"/>
+    </row>
+    <row r="205" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
         <v>203</v>
       </c>
-    </row>
-    <row r="206" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B205" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="C205" s="7" t="s">
+        <v>78</v>
+      </c>
+      <c r="D205" s="37"/>
+      <c r="E205" s="37"/>
+      <c r="F205" s="38"/>
+    </row>
+    <row r="206" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
         <v>204</v>
       </c>
-    </row>
-    <row r="207" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B206" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="C206" s="7"/>
+      <c r="D206" s="37"/>
+      <c r="E206" s="37"/>
+      <c r="F206" s="38"/>
+    </row>
+    <row r="207" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
         <v>205</v>
       </c>
-    </row>
-    <row r="208" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B207" s="6" t="s">
+        <v>67</v>
+      </c>
+      <c r="C207" s="7"/>
+      <c r="D207" s="37"/>
+      <c r="E207" s="37"/>
+      <c r="F207" s="38"/>
+    </row>
+    <row r="208" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
         <v>206</v>
       </c>
-    </row>
-    <row r="209" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B208" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C208" s="7"/>
+      <c r="D208" s="37"/>
+      <c r="E208" s="37"/>
+      <c r="F208" s="38"/>
+    </row>
+    <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
         <v>207</v>
       </c>
-    </row>
-    <row r="210" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B209" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="C209" s="7"/>
+      <c r="D209" s="37"/>
+      <c r="E209" s="37"/>
+      <c r="F209" s="38"/>
+    </row>
+    <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
         <v>208</v>
       </c>
-    </row>
-    <row r="211" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B210" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="C210" s="7"/>
+      <c r="D210" s="37"/>
+      <c r="E210" s="37"/>
+      <c r="F210" s="38"/>
+    </row>
+    <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
         <v>209</v>
       </c>
-    </row>
-    <row r="212" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B211" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="C211" s="7" t="s">
+        <v>79</v>
+      </c>
+      <c r="D211" s="37"/>
+      <c r="E211" s="37"/>
+      <c r="F211" s="38"/>
+    </row>
+    <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
         <v>210</v>
       </c>
-    </row>
-    <row r="213" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B212" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C212" s="7"/>
+      <c r="D212" s="37"/>
+      <c r="E212" s="37"/>
+      <c r="F212" s="38"/>
+    </row>
+    <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
         <v>211</v>
       </c>
-    </row>
-    <row r="214" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B213" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C213" s="7"/>
+      <c r="D213" s="37"/>
+      <c r="E213" s="37"/>
+      <c r="F213" s="38"/>
+    </row>
+    <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
         <v>212</v>
       </c>
-    </row>
-    <row r="215" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B214" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="C214" s="7"/>
+      <c r="D214" s="37"/>
+      <c r="E214" s="37"/>
+      <c r="F214" s="38"/>
+    </row>
+    <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
         <v>213</v>
       </c>
-    </row>
-    <row r="216" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B215" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="C215" s="7"/>
+      <c r="D215" s="37"/>
+      <c r="E215" s="37"/>
+      <c r="F215" s="38"/>
+    </row>
+    <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
         <v>214</v>
       </c>
-    </row>
-    <row r="217" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B216" s="6" t="s">
+        <v>82</v>
+      </c>
+      <c r="C216" s="7"/>
+      <c r="D216" s="37"/>
+      <c r="E216" s="37"/>
+      <c r="F216" s="38"/>
+    </row>
+    <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
         <v>215</v>
       </c>
-    </row>
-    <row r="218" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B217" s="23" t="s">
+        <v>35</v>
+      </c>
+      <c r="C217" s="47" t="s">
+        <v>96</v>
+      </c>
+      <c r="D217" s="37"/>
+      <c r="E217" s="37"/>
+      <c r="F217" s="38"/>
+    </row>
+    <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
         <v>216</v>
       </c>
-    </row>
-    <row r="219" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B218" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="C218" s="27"/>
+      <c r="D218" s="37"/>
+      <c r="E218" s="37"/>
+      <c r="F218" s="38"/>
+    </row>
+    <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
         <v>217</v>
       </c>
-    </row>
-    <row r="220" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B219" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="C219" s="27"/>
+      <c r="D219" s="37"/>
+      <c r="E219" s="37"/>
+      <c r="F219" s="38"/>
+    </row>
+    <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
         <v>218</v>
       </c>
-    </row>
-    <row r="221" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B220" s="6" t="s">
+        <v>64</v>
+      </c>
+      <c r="C220" s="27"/>
+      <c r="D220" s="37"/>
+      <c r="E220" s="37"/>
+      <c r="F220" s="38"/>
+    </row>
+    <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
         <v>219</v>
       </c>
-    </row>
-    <row r="222" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B221" s="6" t="s">
+        <v>41</v>
+      </c>
+      <c r="C221" s="27"/>
+      <c r="D221" s="37"/>
+      <c r="E221" s="37"/>
+      <c r="F221" s="38"/>
+    </row>
+    <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
         <v>220</v>
       </c>
-    </row>
-    <row r="223" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B222" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="C222" s="27"/>
+      <c r="D222" s="37"/>
+      <c r="E222" s="37"/>
+      <c r="F222" s="38"/>
+    </row>
+    <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
         <v>221</v>
       </c>
-    </row>
-    <row r="224" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B223" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="C223" s="27"/>
+      <c r="D223" s="37"/>
+      <c r="E223" s="37"/>
+      <c r="F223" s="38"/>
+    </row>
+    <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
         <v>222</v>
       </c>
-    </row>
-    <row r="225" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B224" s="16" t="s">
+        <v>34</v>
+      </c>
+      <c r="C224" s="28"/>
+      <c r="D224" s="37"/>
+      <c r="E224" s="37"/>
+      <c r="F224" s="38"/>
+    </row>
+    <row r="225" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
         <v>223</v>
       </c>
-    </row>
-    <row r="226" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B225" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C225" s="9"/>
+      <c r="D225" s="42"/>
+      <c r="E225" s="42"/>
+      <c r="F225" s="43"/>
+    </row>
+    <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
         <v>224</v>
       </c>
-    </row>
-    <row r="227" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B226" s="1" t="s">
+        <v>55</v>
+      </c>
+      <c r="C226" s="35" t="s">
+        <v>86</v>
+      </c>
+      <c r="D226" s="35" t="s">
+        <v>89</v>
+      </c>
+      <c r="E226" s="35"/>
+      <c r="F226" s="35"/>
+    </row>
+    <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
         <v>225</v>
       </c>
-    </row>
-    <row r="228" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B227" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="C227" s="44"/>
+      <c r="D227" s="44"/>
+      <c r="E227" s="44"/>
+      <c r="F227" s="44"/>
+    </row>
+    <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
         <v>226</v>
       </c>
-    </row>
-    <row r="229" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B228" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="C228" s="44" t="s">
+        <v>85</v>
+      </c>
+      <c r="D228" s="44"/>
+      <c r="E228" s="44"/>
+      <c r="F228" s="44"/>
+    </row>
+    <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
         <v>227</v>
       </c>
-    </row>
-    <row r="230" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B229" s="1" t="s">
+        <v>48</v>
+      </c>
+      <c r="C229" s="44"/>
+      <c r="D229" s="44"/>
+      <c r="E229" s="44"/>
+      <c r="F229" s="44"/>
+    </row>
+    <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
         <v>228</v>
       </c>
-    </row>
-    <row r="231" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B230" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="C230" s="44" t="s">
+        <v>88</v>
+      </c>
+      <c r="D230" s="44"/>
+      <c r="E230" s="44"/>
+      <c r="F230" s="44"/>
+    </row>
+    <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
-    </row>
-    <row r="232" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B231" s="1" t="s">
+        <v>87</v>
+      </c>
+      <c r="C231" s="44"/>
+      <c r="D231" s="44"/>
+      <c r="E231" s="44"/>
+      <c r="F231" s="44"/>
+    </row>
+    <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
         <v>230</v>
       </c>
-    </row>
-    <row r="233" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="B232" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C232" t="s">
+        <v>91</v>
+      </c>
+      <c r="D232" s="44"/>
+      <c r="E232" s="44"/>
+      <c r="F232" s="44"/>
+    </row>
+    <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
-    </row>
-    <row r="234" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="C233" s="45" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="234" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A234" s="1">
         <v>232</v>
       </c>
     </row>
-    <row r="235" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A235" s="1">
         <v>233</v>
       </c>
     </row>
-    <row r="236" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A236" s="1">
         <v>234</v>
       </c>
     </row>
-    <row r="237" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A237" s="1">
         <v>235</v>
       </c>
     </row>
-    <row r="238" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A238" s="1">
         <v>236</v>
       </c>
     </row>
-    <row r="239" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A239" s="1">
         <v>237</v>
       </c>
     </row>
-    <row r="240" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A240" s="1">
         <v>238</v>
       </c>
@@ -7408,22 +8321,30 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="23">
+    <mergeCell ref="H177:R197"/>
+    <mergeCell ref="C217:C224"/>
+    <mergeCell ref="D169:F225"/>
+    <mergeCell ref="C226:C227"/>
+    <mergeCell ref="C228:C229"/>
+    <mergeCell ref="C230:C231"/>
+    <mergeCell ref="D226:F232"/>
+    <mergeCell ref="C61:C68"/>
+    <mergeCell ref="C98:C105"/>
+    <mergeCell ref="D61:F106"/>
+    <mergeCell ref="C107:C114"/>
+    <mergeCell ref="C169:C176"/>
+    <mergeCell ref="C2:F7"/>
+    <mergeCell ref="C8:F33"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="C52:C59"/>
+    <mergeCell ref="D34:F60"/>
     <mergeCell ref="C137:C144"/>
     <mergeCell ref="C150:C157"/>
     <mergeCell ref="C160:C167"/>
     <mergeCell ref="D137:F168"/>
     <mergeCell ref="C128:C135"/>
     <mergeCell ref="D107:F136"/>
-    <mergeCell ref="C2:F7"/>
-    <mergeCell ref="C8:F33"/>
-    <mergeCell ref="C34:C41"/>
-    <mergeCell ref="C52:C59"/>
-    <mergeCell ref="D34:F60"/>
-    <mergeCell ref="C61:C68"/>
-    <mergeCell ref="C98:C105"/>
-    <mergeCell ref="D61:F106"/>
-    <mergeCell ref="C107:C114"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Small Changes to fix the bug in TestingProgram1.
</commit_message>
<xml_diff>
--- a/TestProgram1.xlsx
+++ b/TestProgram1.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\QiTianYi\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6B8CB56C-FBE7-4757-BE41-9377FB1F0327}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55B6031A-CE16-4283-9CFE-457984172170}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{5181C135-F803-4CA6-AFB1-3DD996B2224A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{5181C135-F803-4CA6-AFB1-3DD996B2224A}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="250" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="116">
   <si>
     <t>Memory Location</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -366,10 +366,6 @@
   </si>
   <si>
     <t>LDX IX0,MEM[21]</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>JZ R0,IX0,0</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
@@ -508,15 +504,43 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
+    <t>GOTO COMPARE()</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2=MEM[30]</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R1=PREVIOUS_BIGGER</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>R2=ABS</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>CALL COMPARE</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
     <t>MAIN LOGIC:
 B IS MEM[29]
 A IS MEM[23]. WITH INITIAL VALUE OF 65535
 FOR ENUM IN MEM[500~520] (MACHINE CODE VISITED IN REVERSE ORDER,FROM 520 TO 500):
-IF ABSOLUTEVALUE(ENUM-MEM[30])&gt;A:
+IF ABSOLUTEVALUE(ENUM-MEM[30])&lt;A:
 A=ABSOLUTEVALUE(ENUM-MEM[30])
 B=ENUM
 ELSE:
 DO_NOTHING</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>JNE R0,IX0,0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>TEMP</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -810,7 +834,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="50">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -892,6 +916,18 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -900,6 +936,36 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -916,47 +982,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1">
       <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1274,9 +1301,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{72887D96-2685-464A-84B6-218C724B7504}">
   <dimension ref="A1:R1026"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <pane ySplit="33" topLeftCell="A174" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="P200" sqref="P200"/>
+    <sheetView tabSelected="1" zoomScale="98" zoomScaleNormal="98" workbookViewId="0">
+      <selection activeCell="C2" sqref="C2:F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -1293,6 +1319,9 @@
       <c r="B1" s="1" t="s">
         <v>1</v>
       </c>
+      <c r="C1" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="4">
@@ -1301,12 +1330,12 @@
       <c r="B2" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="39" t="s">
+      <c r="C2" s="41" t="s">
         <v>5</v>
       </c>
-      <c r="D2" s="39"/>
-      <c r="E2" s="39"/>
-      <c r="F2" s="39"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" s="4">
@@ -1315,10 +1344,10 @@
       <c r="B3" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="39"/>
-      <c r="D3" s="39"/>
-      <c r="E3" s="39"/>
-      <c r="F3" s="39"/>
+      <c r="C3" s="41"/>
+      <c r="D3" s="41"/>
+      <c r="E3" s="41"/>
+      <c r="F3" s="41"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" s="4">
@@ -1327,10 +1356,10 @@
       <c r="B4" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="39"/>
-      <c r="D4" s="39"/>
-      <c r="E4" s="39"/>
-      <c r="F4" s="39"/>
+      <c r="C4" s="41"/>
+      <c r="D4" s="41"/>
+      <c r="E4" s="41"/>
+      <c r="F4" s="41"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A5" s="4">
@@ -1339,10 +1368,10 @@
       <c r="B5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C5" s="39"/>
-      <c r="D5" s="39"/>
-      <c r="E5" s="39"/>
-      <c r="F5" s="39"/>
+      <c r="C5" s="41"/>
+      <c r="D5" s="41"/>
+      <c r="E5" s="41"/>
+      <c r="F5" s="41"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" s="4">
@@ -1351,10 +1380,10 @@
       <c r="B6" s="4" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="39"/>
-      <c r="D6" s="39"/>
-      <c r="E6" s="39"/>
-      <c r="F6" s="39"/>
+      <c r="C6" s="41"/>
+      <c r="D6" s="41"/>
+      <c r="E6" s="41"/>
+      <c r="F6" s="41"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A7" s="4">
@@ -1363,10 +1392,10 @@
       <c r="B7" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C7" s="39"/>
-      <c r="D7" s="39"/>
-      <c r="E7" s="39"/>
-      <c r="F7" s="39"/>
+      <c r="C7" s="41"/>
+      <c r="D7" s="41"/>
+      <c r="E7" s="41"/>
+      <c r="F7" s="41"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A8" s="3">
@@ -1375,158 +1404,158 @@
       <c r="B8" s="3" t="s">
         <v>83</v>
       </c>
-      <c r="C8" s="40" t="s">
+      <c r="C8" s="42" t="s">
         <v>7</v>
       </c>
-      <c r="D8" s="41"/>
-      <c r="E8" s="41"/>
-      <c r="F8" s="41"/>
+      <c r="D8" s="43"/>
+      <c r="E8" s="43"/>
+      <c r="F8" s="43"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A9" s="3">
         <v>7</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>90</v>
-      </c>
-      <c r="C9" s="41"/>
-      <c r="D9" s="41"/>
-      <c r="E9" s="41"/>
-      <c r="F9" s="41"/>
+        <v>89</v>
+      </c>
+      <c r="C9" s="43"/>
+      <c r="D9" s="43"/>
+      <c r="E9" s="43"/>
+      <c r="F9" s="43"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" s="3">
         <v>8</v>
       </c>
       <c r="B10" s="12" t="s">
-        <v>94</v>
-      </c>
-      <c r="C10" s="41"/>
-      <c r="D10" s="41"/>
-      <c r="E10" s="41"/>
-      <c r="F10" s="41"/>
+        <v>93</v>
+      </c>
+      <c r="C10" s="43"/>
+      <c r="D10" s="43"/>
+      <c r="E10" s="43"/>
+      <c r="F10" s="43"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A11" s="3">
         <v>9</v>
       </c>
       <c r="B11" s="13" t="s">
-        <v>95</v>
-      </c>
-      <c r="C11" s="41"/>
-      <c r="D11" s="41"/>
-      <c r="E11" s="41"/>
-      <c r="F11" s="41"/>
+        <v>94</v>
+      </c>
+      <c r="C11" s="43"/>
+      <c r="D11" s="43"/>
+      <c r="E11" s="43"/>
+      <c r="F11" s="43"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A12" s="3">
         <v>10</v>
       </c>
       <c r="B12" s="13"/>
-      <c r="C12" s="41"/>
-      <c r="D12" s="41"/>
-      <c r="E12" s="41"/>
-      <c r="F12" s="41"/>
+      <c r="C12" s="43"/>
+      <c r="D12" s="43"/>
+      <c r="E12" s="43"/>
+      <c r="F12" s="43"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A13" s="3">
         <v>11</v>
       </c>
       <c r="B13" s="13"/>
-      <c r="C13" s="41"/>
-      <c r="D13" s="41"/>
-      <c r="E13" s="41"/>
-      <c r="F13" s="41"/>
+      <c r="C13" s="43"/>
+      <c r="D13" s="43"/>
+      <c r="E13" s="43"/>
+      <c r="F13" s="43"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" s="3">
         <v>12</v>
       </c>
       <c r="B14" s="13"/>
-      <c r="C14" s="41"/>
-      <c r="D14" s="41"/>
-      <c r="E14" s="41"/>
-      <c r="F14" s="41"/>
+      <c r="C14" s="43"/>
+      <c r="D14" s="43"/>
+      <c r="E14" s="43"/>
+      <c r="F14" s="43"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A15" s="3">
         <v>13</v>
       </c>
       <c r="B15" s="13"/>
-      <c r="C15" s="41"/>
-      <c r="D15" s="41"/>
-      <c r="E15" s="41"/>
-      <c r="F15" s="41"/>
+      <c r="C15" s="43"/>
+      <c r="D15" s="43"/>
+      <c r="E15" s="43"/>
+      <c r="F15" s="43"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A16" s="3">
         <v>14</v>
       </c>
       <c r="B16" s="13"/>
-      <c r="C16" s="41"/>
-      <c r="D16" s="41"/>
-      <c r="E16" s="41"/>
-      <c r="F16" s="41"/>
+      <c r="C16" s="43"/>
+      <c r="D16" s="43"/>
+      <c r="E16" s="43"/>
+      <c r="F16" s="43"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A17" s="3">
         <v>15</v>
       </c>
       <c r="B17" s="13"/>
-      <c r="C17" s="41"/>
-      <c r="D17" s="41"/>
-      <c r="E17" s="41"/>
-      <c r="F17" s="41"/>
+      <c r="C17" s="43"/>
+      <c r="D17" s="43"/>
+      <c r="E17" s="43"/>
+      <c r="F17" s="43"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A18" s="3">
         <v>16</v>
       </c>
       <c r="B18" s="13"/>
-      <c r="C18" s="41"/>
-      <c r="D18" s="41"/>
-      <c r="E18" s="41"/>
-      <c r="F18" s="41"/>
+      <c r="C18" s="43"/>
+      <c r="D18" s="43"/>
+      <c r="E18" s="43"/>
+      <c r="F18" s="43"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A19" s="3">
         <v>17</v>
       </c>
       <c r="B19" s="13"/>
-      <c r="C19" s="41"/>
-      <c r="D19" s="41"/>
-      <c r="E19" s="41"/>
-      <c r="F19" s="41"/>
+      <c r="C19" s="43"/>
+      <c r="D19" s="43"/>
+      <c r="E19" s="43"/>
+      <c r="F19" s="43"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A20" s="3">
         <v>18</v>
       </c>
       <c r="B20" s="14"/>
-      <c r="C20" s="41"/>
-      <c r="D20" s="41"/>
-      <c r="E20" s="41"/>
-      <c r="F20" s="41"/>
+      <c r="C20" s="43"/>
+      <c r="D20" s="43"/>
+      <c r="E20" s="43"/>
+      <c r="F20" s="43"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A21" s="3">
         <v>19</v>
       </c>
       <c r="B21" s="3"/>
-      <c r="C21" s="41"/>
-      <c r="D21" s="41"/>
-      <c r="E21" s="41"/>
-      <c r="F21" s="41"/>
+      <c r="C21" s="43"/>
+      <c r="D21" s="43"/>
+      <c r="E21" s="43"/>
+      <c r="F21" s="43"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A22" s="3">
         <v>20</v>
       </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="41"/>
-      <c r="D22" s="41"/>
-      <c r="E22" s="41"/>
-      <c r="F22" s="41"/>
+      <c r="C22" s="43"/>
+      <c r="D22" s="43"/>
+      <c r="E22" s="43"/>
+      <c r="F22" s="43"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A23" s="3">
@@ -1535,10 +1564,10 @@
       <c r="B23" s="3">
         <v>210</v>
       </c>
-      <c r="C23" s="41"/>
-      <c r="D23" s="41"/>
-      <c r="E23" s="41"/>
-      <c r="F23" s="41"/>
+      <c r="C23" s="43"/>
+      <c r="D23" s="43"/>
+      <c r="E23" s="43"/>
+      <c r="F23" s="43"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A24" s="3">
@@ -1547,10 +1576,10 @@
       <c r="B24" s="3">
         <v>177</v>
       </c>
-      <c r="C24" s="41"/>
-      <c r="D24" s="41"/>
-      <c r="E24" s="41"/>
-      <c r="F24" s="41"/>
+      <c r="C24" s="43"/>
+      <c r="D24" s="43"/>
+      <c r="E24" s="43"/>
+      <c r="F24" s="43"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A25" s="3">
@@ -1559,10 +1588,10 @@
       <c r="B25" s="3">
         <v>65535</v>
       </c>
-      <c r="C25" s="41"/>
-      <c r="D25" s="41"/>
-      <c r="E25" s="41"/>
-      <c r="F25" s="41"/>
+      <c r="C25" s="43"/>
+      <c r="D25" s="43"/>
+      <c r="E25" s="43"/>
+      <c r="F25" s="43"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A26" s="3">
@@ -1571,10 +1600,10 @@
       <c r="B26" s="3">
         <v>145</v>
       </c>
-      <c r="C26" s="41"/>
-      <c r="D26" s="41"/>
-      <c r="E26" s="41"/>
-      <c r="F26" s="41"/>
+      <c r="C26" s="43"/>
+      <c r="D26" s="43"/>
+      <c r="E26" s="43"/>
+      <c r="F26" s="43"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A27" s="3">
@@ -1583,10 +1612,10 @@
       <c r="B27" s="3">
         <v>105</v>
       </c>
-      <c r="C27" s="41"/>
-      <c r="D27" s="41"/>
-      <c r="E27" s="41"/>
-      <c r="F27" s="41"/>
+      <c r="C27" s="43"/>
+      <c r="D27" s="43"/>
+      <c r="E27" s="43"/>
+      <c r="F27" s="43"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A28" s="3">
@@ -1595,10 +1624,10 @@
       <c r="B28" s="3">
         <v>500</v>
       </c>
-      <c r="C28" s="41"/>
-      <c r="D28" s="41"/>
-      <c r="E28" s="41"/>
-      <c r="F28" s="41"/>
+      <c r="C28" s="43"/>
+      <c r="D28" s="43"/>
+      <c r="E28" s="43"/>
+      <c r="F28" s="43"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A29" s="3">
@@ -1607,10 +1636,10 @@
       <c r="B29" s="3">
         <v>20</v>
       </c>
-      <c r="C29" s="41"/>
-      <c r="D29" s="41"/>
-      <c r="E29" s="41"/>
-      <c r="F29" s="41"/>
+      <c r="C29" s="43"/>
+      <c r="D29" s="43"/>
+      <c r="E29" s="43"/>
+      <c r="F29" s="43"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A30" s="3">
@@ -1619,10 +1648,10 @@
       <c r="B30" s="3">
         <v>67</v>
       </c>
-      <c r="C30" s="41"/>
-      <c r="D30" s="41"/>
-      <c r="E30" s="41"/>
-      <c r="F30" s="41"/>
+      <c r="C30" s="43"/>
+      <c r="D30" s="43"/>
+      <c r="E30" s="43"/>
+      <c r="F30" s="43"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A31" s="3">
@@ -1631,10 +1660,10 @@
       <c r="B31" s="10" t="s">
         <v>28</v>
       </c>
-      <c r="C31" s="41"/>
-      <c r="D31" s="41"/>
-      <c r="E31" s="41"/>
-      <c r="F31" s="41"/>
+      <c r="C31" s="43"/>
+      <c r="D31" s="43"/>
+      <c r="E31" s="43"/>
+      <c r="F31" s="43"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A32" s="3">
@@ -1643,10 +1672,10 @@
       <c r="B32" s="10" t="s">
         <v>27</v>
       </c>
-      <c r="C32" s="41"/>
-      <c r="D32" s="41"/>
-      <c r="E32" s="41"/>
-      <c r="F32" s="41"/>
+      <c r="C32" s="43"/>
+      <c r="D32" s="43"/>
+      <c r="E32" s="43"/>
+      <c r="F32" s="43"/>
     </row>
     <row r="33" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3">
@@ -1655,10 +1684,10 @@
       <c r="B33" s="5">
         <v>32</v>
       </c>
-      <c r="C33" s="41"/>
-      <c r="D33" s="41"/>
-      <c r="E33" s="41"/>
-      <c r="F33" s="41"/>
+      <c r="C33" s="43"/>
+      <c r="D33" s="43"/>
+      <c r="E33" s="43"/>
+      <c r="F33" s="43"/>
     </row>
     <row r="34" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="2">
@@ -1667,14 +1696,14 @@
       <c r="B34" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C34" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D34" s="29" t="s">
-        <v>97</v>
-      </c>
-      <c r="E34" s="29"/>
-      <c r="F34" s="30"/>
+      <c r="C34" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D34" s="33" t="s">
+        <v>96</v>
+      </c>
+      <c r="E34" s="33"/>
+      <c r="F34" s="44"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A35" s="1">
@@ -1683,10 +1712,10 @@
       <c r="B35" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C35" s="27"/>
-      <c r="D35" s="31"/>
-      <c r="E35" s="31"/>
-      <c r="F35" s="32"/>
+      <c r="C35" s="31"/>
+      <c r="D35" s="45"/>
+      <c r="E35" s="45"/>
+      <c r="F35" s="46"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A36" s="1">
@@ -1695,10 +1724,10 @@
       <c r="B36" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C36" s="27"/>
-      <c r="D36" s="31"/>
-      <c r="E36" s="31"/>
-      <c r="F36" s="32"/>
+      <c r="C36" s="31"/>
+      <c r="D36" s="45"/>
+      <c r="E36" s="45"/>
+      <c r="F36" s="46"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A37" s="1">
@@ -1707,10 +1736,10 @@
       <c r="B37" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C37" s="27"/>
-      <c r="D37" s="31"/>
-      <c r="E37" s="31"/>
-      <c r="F37" s="32"/>
+      <c r="C37" s="31"/>
+      <c r="D37" s="45"/>
+      <c r="E37" s="45"/>
+      <c r="F37" s="46"/>
     </row>
     <row r="38" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A38" s="15">
@@ -1719,10 +1748,10 @@
       <c r="B38" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C38" s="27"/>
-      <c r="D38" s="31"/>
-      <c r="E38" s="31"/>
-      <c r="F38" s="32"/>
+      <c r="C38" s="31"/>
+      <c r="D38" s="45"/>
+      <c r="E38" s="45"/>
+      <c r="F38" s="46"/>
     </row>
     <row r="39" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A39" s="15">
@@ -1731,10 +1760,10 @@
       <c r="B39" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C39" s="27"/>
-      <c r="D39" s="31"/>
-      <c r="E39" s="31"/>
-      <c r="F39" s="32"/>
+      <c r="C39" s="31"/>
+      <c r="D39" s="45"/>
+      <c r="E39" s="45"/>
+      <c r="F39" s="46"/>
     </row>
     <row r="40" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A40" s="1">
@@ -1743,10 +1772,10 @@
       <c r="B40" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C40" s="27"/>
-      <c r="D40" s="31"/>
-      <c r="E40" s="31"/>
-      <c r="F40" s="32"/>
+      <c r="C40" s="31"/>
+      <c r="D40" s="45"/>
+      <c r="E40" s="45"/>
+      <c r="F40" s="46"/>
     </row>
     <row r="41" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A41" s="1">
@@ -1755,10 +1784,10 @@
       <c r="B41" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C41" s="28"/>
-      <c r="D41" s="31"/>
-      <c r="E41" s="31"/>
-      <c r="F41" s="32"/>
+      <c r="C41" s="32"/>
+      <c r="D41" s="45"/>
+      <c r="E41" s="45"/>
+      <c r="F41" s="46"/>
     </row>
     <row r="42" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A42" s="1">
@@ -1768,9 +1797,9 @@
         <v>12</v>
       </c>
       <c r="C42" s="17"/>
-      <c r="D42" s="31"/>
-      <c r="E42" s="31"/>
-      <c r="F42" s="32"/>
+      <c r="D42" s="45"/>
+      <c r="E42" s="45"/>
+      <c r="F42" s="46"/>
     </row>
     <row r="43" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A43" s="1">
@@ -1780,9 +1809,9 @@
         <v>13</v>
       </c>
       <c r="C43" s="7"/>
-      <c r="D43" s="31"/>
-      <c r="E43" s="31"/>
-      <c r="F43" s="32"/>
+      <c r="D43" s="45"/>
+      <c r="E43" s="45"/>
+      <c r="F43" s="46"/>
     </row>
     <row r="44" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A44" s="1">
@@ -1792,9 +1821,9 @@
         <v>11</v>
       </c>
       <c r="C44" s="7"/>
-      <c r="D44" s="31"/>
-      <c r="E44" s="31"/>
-      <c r="F44" s="32"/>
+      <c r="D44" s="45"/>
+      <c r="E44" s="45"/>
+      <c r="F44" s="46"/>
     </row>
     <row r="45" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A45" s="1">
@@ -1804,9 +1833,9 @@
         <v>39</v>
       </c>
       <c r="C45" s="7"/>
-      <c r="D45" s="31"/>
-      <c r="E45" s="31"/>
-      <c r="F45" s="32"/>
+      <c r="D45" s="45"/>
+      <c r="E45" s="45"/>
+      <c r="F45" s="46"/>
     </row>
     <row r="46" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A46" s="2">
@@ -1816,9 +1845,9 @@
         <v>9</v>
       </c>
       <c r="C46" s="7"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="31"/>
-      <c r="F46" s="32"/>
+      <c r="D46" s="45"/>
+      <c r="E46" s="45"/>
+      <c r="F46" s="46"/>
     </row>
     <row r="47" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A47" s="2">
@@ -1828,9 +1857,9 @@
         <v>14</v>
       </c>
       <c r="C47" s="7"/>
-      <c r="D47" s="31"/>
-      <c r="E47" s="31"/>
-      <c r="F47" s="32"/>
+      <c r="D47" s="45"/>
+      <c r="E47" s="45"/>
+      <c r="F47" s="46"/>
     </row>
     <row r="48" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A48" s="1">
@@ -1840,9 +1869,9 @@
         <v>40</v>
       </c>
       <c r="C48" s="7"/>
-      <c r="D48" s="31"/>
-      <c r="E48" s="31"/>
-      <c r="F48" s="32"/>
+      <c r="D48" s="45"/>
+      <c r="E48" s="45"/>
+      <c r="F48" s="46"/>
     </row>
     <row r="49" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A49" s="1">
@@ -1852,9 +1881,9 @@
         <v>18</v>
       </c>
       <c r="C49" s="7"/>
-      <c r="D49" s="31"/>
-      <c r="E49" s="31"/>
-      <c r="F49" s="32"/>
+      <c r="D49" s="45"/>
+      <c r="E49" s="45"/>
+      <c r="F49" s="46"/>
     </row>
     <row r="50" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="1">
@@ -1864,9 +1893,9 @@
         <v>19</v>
       </c>
       <c r="C50" s="7"/>
-      <c r="D50" s="31"/>
-      <c r="E50" s="31"/>
-      <c r="F50" s="32"/>
+      <c r="D50" s="45"/>
+      <c r="E50" s="45"/>
+      <c r="F50" s="46"/>
     </row>
     <row r="51" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A51" s="1">
@@ -1876,9 +1905,9 @@
         <v>20</v>
       </c>
       <c r="C51" s="7"/>
-      <c r="D51" s="31"/>
-      <c r="E51" s="31"/>
-      <c r="F51" s="32"/>
+      <c r="D51" s="45"/>
+      <c r="E51" s="45"/>
+      <c r="F51" s="46"/>
     </row>
     <row r="52" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A52" s="1">
@@ -1887,12 +1916,12 @@
       <c r="B52" s="18" t="s">
         <v>35</v>
       </c>
-      <c r="C52" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D52" s="31"/>
-      <c r="E52" s="31"/>
-      <c r="F52" s="32"/>
+      <c r="C52" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D52" s="45"/>
+      <c r="E52" s="45"/>
+      <c r="F52" s="46"/>
     </row>
     <row r="53" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A53" s="1">
@@ -1901,10 +1930,10 @@
       <c r="B53" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C53" s="27"/>
-      <c r="D53" s="31"/>
-      <c r="E53" s="31"/>
-      <c r="F53" s="32"/>
+      <c r="C53" s="31"/>
+      <c r="D53" s="45"/>
+      <c r="E53" s="45"/>
+      <c r="F53" s="46"/>
     </row>
     <row r="54" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A54" s="1">
@@ -1913,10 +1942,10 @@
       <c r="B54" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C54" s="27"/>
-      <c r="D54" s="31"/>
-      <c r="E54" s="31"/>
-      <c r="F54" s="32"/>
+      <c r="C54" s="31"/>
+      <c r="D54" s="45"/>
+      <c r="E54" s="45"/>
+      <c r="F54" s="46"/>
     </row>
     <row r="55" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A55" s="1">
@@ -1925,10 +1954,10 @@
       <c r="B55" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C55" s="27"/>
-      <c r="D55" s="31"/>
-      <c r="E55" s="31"/>
-      <c r="F55" s="32"/>
+      <c r="C55" s="31"/>
+      <c r="D55" s="45"/>
+      <c r="E55" s="45"/>
+      <c r="F55" s="46"/>
     </row>
     <row r="56" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A56" s="1">
@@ -1937,10 +1966,10 @@
       <c r="B56" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C56" s="27"/>
-      <c r="D56" s="31"/>
-      <c r="E56" s="31"/>
-      <c r="F56" s="32"/>
+      <c r="C56" s="31"/>
+      <c r="D56" s="45"/>
+      <c r="E56" s="45"/>
+      <c r="F56" s="46"/>
     </row>
     <row r="57" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A57" s="1">
@@ -1949,10 +1978,10 @@
       <c r="B57" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C57" s="27"/>
-      <c r="D57" s="31"/>
-      <c r="E57" s="31"/>
-      <c r="F57" s="32"/>
+      <c r="C57" s="31"/>
+      <c r="D57" s="45"/>
+      <c r="E57" s="45"/>
+      <c r="F57" s="46"/>
     </row>
     <row r="58" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A58" s="1">
@@ -1961,10 +1990,10 @@
       <c r="B58" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C58" s="27"/>
-      <c r="D58" s="31"/>
-      <c r="E58" s="31"/>
-      <c r="F58" s="32"/>
+      <c r="C58" s="31"/>
+      <c r="D58" s="45"/>
+      <c r="E58" s="45"/>
+      <c r="F58" s="46"/>
     </row>
     <row r="59" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A59" s="1">
@@ -1973,10 +2002,10 @@
       <c r="B59" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C59" s="28"/>
-      <c r="D59" s="31"/>
-      <c r="E59" s="31"/>
-      <c r="F59" s="32"/>
+      <c r="C59" s="32"/>
+      <c r="D59" s="45"/>
+      <c r="E59" s="45"/>
+      <c r="F59" s="46"/>
     </row>
     <row r="60" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A60" s="1">
@@ -1986,9 +2015,9 @@
         <v>10</v>
       </c>
       <c r="C60" s="9"/>
-      <c r="D60" s="33"/>
-      <c r="E60" s="33"/>
-      <c r="F60" s="34"/>
+      <c r="D60" s="47"/>
+      <c r="E60" s="47"/>
+      <c r="F60" s="48"/>
     </row>
     <row r="61" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A61" s="2">
@@ -1997,14 +2026,14 @@
       <c r="B61" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C61" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D61" s="29" t="s">
-        <v>98</v>
-      </c>
-      <c r="E61" s="35"/>
-      <c r="F61" s="36"/>
+      <c r="C61" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D61" s="33" t="s">
+        <v>97</v>
+      </c>
+      <c r="E61" s="34"/>
+      <c r="F61" s="35"/>
     </row>
     <row r="62" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A62" s="1">
@@ -2013,10 +2042,10 @@
       <c r="B62" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C62" s="27"/>
-      <c r="D62" s="37"/>
-      <c r="E62" s="37"/>
-      <c r="F62" s="38"/>
+      <c r="C62" s="31"/>
+      <c r="D62" s="36"/>
+      <c r="E62" s="36"/>
+      <c r="F62" s="37"/>
     </row>
     <row r="63" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A63" s="1">
@@ -2025,10 +2054,10 @@
       <c r="B63" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C63" s="27"/>
-      <c r="D63" s="37"/>
-      <c r="E63" s="37"/>
-      <c r="F63" s="38"/>
+      <c r="C63" s="31"/>
+      <c r="D63" s="36"/>
+      <c r="E63" s="36"/>
+      <c r="F63" s="37"/>
     </row>
     <row r="64" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A64" s="1">
@@ -2037,10 +2066,10 @@
       <c r="B64" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C64" s="27"/>
-      <c r="D64" s="37"/>
-      <c r="E64" s="37"/>
-      <c r="F64" s="38"/>
+      <c r="C64" s="31"/>
+      <c r="D64" s="36"/>
+      <c r="E64" s="36"/>
+      <c r="F64" s="37"/>
     </row>
     <row r="65" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A65" s="1">
@@ -2049,10 +2078,10 @@
       <c r="B65" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C65" s="27"/>
-      <c r="D65" s="37"/>
-      <c r="E65" s="37"/>
-      <c r="F65" s="38"/>
+      <c r="C65" s="31"/>
+      <c r="D65" s="36"/>
+      <c r="E65" s="36"/>
+      <c r="F65" s="37"/>
     </row>
     <row r="66" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A66" s="1">
@@ -2061,10 +2090,10 @@
       <c r="B66" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C66" s="27"/>
-      <c r="D66" s="37"/>
-      <c r="E66" s="37"/>
-      <c r="F66" s="38"/>
+      <c r="C66" s="31"/>
+      <c r="D66" s="36"/>
+      <c r="E66" s="36"/>
+      <c r="F66" s="37"/>
     </row>
     <row r="67" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A67" s="1">
@@ -2073,10 +2102,10 @@
       <c r="B67" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C67" s="27"/>
-      <c r="D67" s="37"/>
-      <c r="E67" s="37"/>
-      <c r="F67" s="38"/>
+      <c r="C67" s="31"/>
+      <c r="D67" s="36"/>
+      <c r="E67" s="36"/>
+      <c r="F67" s="37"/>
     </row>
     <row r="68" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A68" s="1">
@@ -2085,10 +2114,10 @@
       <c r="B68" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C68" s="28"/>
-      <c r="D68" s="37"/>
-      <c r="E68" s="37"/>
-      <c r="F68" s="38"/>
+      <c r="C68" s="32"/>
+      <c r="D68" s="36"/>
+      <c r="E68" s="36"/>
+      <c r="F68" s="37"/>
     </row>
     <row r="69" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A69" s="2">
@@ -2098,9 +2127,9 @@
         <v>15</v>
       </c>
       <c r="C69" s="7"/>
-      <c r="D69" s="37"/>
-      <c r="E69" s="37"/>
-      <c r="F69" s="38"/>
+      <c r="D69" s="36"/>
+      <c r="E69" s="36"/>
+      <c r="F69" s="37"/>
     </row>
     <row r="70" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A70" s="1">
@@ -2110,9 +2139,9 @@
         <v>49</v>
       </c>
       <c r="C70" s="7"/>
-      <c r="D70" s="37"/>
-      <c r="E70" s="37"/>
-      <c r="F70" s="38"/>
+      <c r="D70" s="36"/>
+      <c r="E70" s="36"/>
+      <c r="F70" s="37"/>
     </row>
     <row r="71" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A71" s="1">
@@ -2122,9 +2151,9 @@
         <v>11</v>
       </c>
       <c r="C71" s="7"/>
-      <c r="D71" s="37"/>
-      <c r="E71" s="37"/>
-      <c r="F71" s="38"/>
+      <c r="D71" s="36"/>
+      <c r="E71" s="36"/>
+      <c r="F71" s="37"/>
     </row>
     <row r="72" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A72" s="1">
@@ -2134,9 +2163,9 @@
         <v>8</v>
       </c>
       <c r="C72" s="7"/>
-      <c r="D72" s="37"/>
-      <c r="E72" s="37"/>
-      <c r="F72" s="38"/>
+      <c r="D72" s="36"/>
+      <c r="E72" s="36"/>
+      <c r="F72" s="37"/>
     </row>
     <row r="73" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A73" s="15">
@@ -2146,9 +2175,9 @@
         <v>43</v>
       </c>
       <c r="C73" s="7"/>
-      <c r="D73" s="37"/>
-      <c r="E73" s="37"/>
-      <c r="F73" s="38"/>
+      <c r="D73" s="36"/>
+      <c r="E73" s="36"/>
+      <c r="F73" s="37"/>
     </row>
     <row r="74" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A74" s="1">
@@ -2158,9 +2187,9 @@
         <v>17</v>
       </c>
       <c r="C74" s="7"/>
-      <c r="D74" s="37"/>
-      <c r="E74" s="37"/>
-      <c r="F74" s="38"/>
+      <c r="D74" s="36"/>
+      <c r="E74" s="36"/>
+      <c r="F74" s="37"/>
     </row>
     <row r="75" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A75" s="1">
@@ -2170,9 +2199,9 @@
         <v>12</v>
       </c>
       <c r="C75" s="7"/>
-      <c r="D75" s="37"/>
-      <c r="E75" s="37"/>
-      <c r="F75" s="38"/>
+      <c r="D75" s="36"/>
+      <c r="E75" s="36"/>
+      <c r="F75" s="37"/>
     </row>
     <row r="76" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A76" s="1">
@@ -2182,9 +2211,9 @@
         <v>13</v>
       </c>
       <c r="C76" s="7"/>
-      <c r="D76" s="37"/>
-      <c r="E76" s="37"/>
-      <c r="F76" s="38"/>
+      <c r="D76" s="36"/>
+      <c r="E76" s="36"/>
+      <c r="F76" s="37"/>
     </row>
     <row r="77" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A77" s="1">
@@ -2194,9 +2223,9 @@
         <v>22</v>
       </c>
       <c r="C77" s="7"/>
-      <c r="D77" s="37"/>
-      <c r="E77" s="37"/>
-      <c r="F77" s="38"/>
+      <c r="D77" s="36"/>
+      <c r="E77" s="36"/>
+      <c r="F77" s="37"/>
     </row>
     <row r="78" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A78" s="1">
@@ -2206,9 +2235,9 @@
         <v>15</v>
       </c>
       <c r="C78" s="7"/>
-      <c r="D78" s="37"/>
-      <c r="E78" s="37"/>
-      <c r="F78" s="38"/>
+      <c r="D78" s="36"/>
+      <c r="E78" s="36"/>
+      <c r="F78" s="37"/>
     </row>
     <row r="79" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A79" s="1">
@@ -2218,9 +2247,9 @@
         <v>16</v>
       </c>
       <c r="C79" s="7"/>
-      <c r="D79" s="37"/>
-      <c r="E79" s="37"/>
-      <c r="F79" s="38"/>
+      <c r="D79" s="36"/>
+      <c r="E79" s="36"/>
+      <c r="F79" s="37"/>
     </row>
     <row r="80" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A80" s="1">
@@ -2230,9 +2259,9 @@
         <v>8</v>
       </c>
       <c r="C80" s="7"/>
-      <c r="D80" s="37"/>
-      <c r="E80" s="37"/>
-      <c r="F80" s="38"/>
+      <c r="D80" s="36"/>
+      <c r="E80" s="36"/>
+      <c r="F80" s="37"/>
     </row>
     <row r="81" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A81" s="1">
@@ -2242,9 +2271,9 @@
         <v>30</v>
       </c>
       <c r="C81" s="7"/>
-      <c r="D81" s="37"/>
-      <c r="E81" s="37"/>
-      <c r="F81" s="38"/>
+      <c r="D81" s="36"/>
+      <c r="E81" s="36"/>
+      <c r="F81" s="37"/>
     </row>
     <row r="82" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A82" s="1">
@@ -2254,9 +2283,9 @@
         <v>46</v>
       </c>
       <c r="C82" s="7"/>
-      <c r="D82" s="37"/>
-      <c r="E82" s="37"/>
-      <c r="F82" s="38"/>
+      <c r="D82" s="36"/>
+      <c r="E82" s="36"/>
+      <c r="F82" s="37"/>
     </row>
     <row r="83" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A83" s="1">
@@ -2266,9 +2295,9 @@
         <v>11</v>
       </c>
       <c r="C83" s="7"/>
-      <c r="D83" s="37"/>
-      <c r="E83" s="37"/>
-      <c r="F83" s="38"/>
+      <c r="D83" s="36"/>
+      <c r="E83" s="36"/>
+      <c r="F83" s="37"/>
     </row>
     <row r="84" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A84" s="1">
@@ -2278,9 +2307,9 @@
         <v>17</v>
       </c>
       <c r="C84" s="7"/>
-      <c r="D84" s="37"/>
-      <c r="E84" s="37"/>
-      <c r="F84" s="38"/>
+      <c r="D84" s="36"/>
+      <c r="E84" s="36"/>
+      <c r="F84" s="37"/>
     </row>
     <row r="85" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A85" s="1">
@@ -2290,9 +2319,9 @@
         <v>12</v>
       </c>
       <c r="C85" s="7"/>
-      <c r="D85" s="37"/>
-      <c r="E85" s="37"/>
-      <c r="F85" s="38"/>
+      <c r="D85" s="36"/>
+      <c r="E85" s="36"/>
+      <c r="F85" s="37"/>
     </row>
     <row r="86" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A86" s="1">
@@ -2302,9 +2331,9 @@
         <v>13</v>
       </c>
       <c r="C86" s="7"/>
-      <c r="D86" s="37"/>
-      <c r="E86" s="37"/>
-      <c r="F86" s="38"/>
+      <c r="D86" s="36"/>
+      <c r="E86" s="36"/>
+      <c r="F86" s="37"/>
     </row>
     <row r="87" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A87" s="1">
@@ -2314,9 +2343,9 @@
         <v>26</v>
       </c>
       <c r="C87" s="7"/>
-      <c r="D87" s="37"/>
-      <c r="E87" s="37"/>
-      <c r="F87" s="38"/>
+      <c r="D87" s="36"/>
+      <c r="E87" s="36"/>
+      <c r="F87" s="37"/>
     </row>
     <row r="88" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A88" s="1">
@@ -2326,9 +2355,9 @@
         <v>23</v>
       </c>
       <c r="C88" s="7"/>
-      <c r="D88" s="37"/>
-      <c r="E88" s="37"/>
-      <c r="F88" s="38"/>
+      <c r="D88" s="36"/>
+      <c r="E88" s="36"/>
+      <c r="F88" s="37"/>
     </row>
     <row r="89" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A89" s="1">
@@ -2338,9 +2367,9 @@
         <v>24</v>
       </c>
       <c r="C89" s="7"/>
-      <c r="D89" s="37"/>
-      <c r="E89" s="37"/>
-      <c r="F89" s="38"/>
+      <c r="D89" s="36"/>
+      <c r="E89" s="36"/>
+      <c r="F89" s="37"/>
     </row>
     <row r="90" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A90" s="1">
@@ -2350,9 +2379,9 @@
         <v>25</v>
       </c>
       <c r="C90" s="7"/>
-      <c r="D90" s="37"/>
-      <c r="E90" s="37"/>
-      <c r="F90" s="38"/>
+      <c r="D90" s="36"/>
+      <c r="E90" s="36"/>
+      <c r="F90" s="37"/>
     </row>
     <row r="91" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A91" s="1">
@@ -2362,9 +2391,9 @@
         <v>11</v>
       </c>
       <c r="C91" s="7"/>
-      <c r="D91" s="37"/>
-      <c r="E91" s="37"/>
-      <c r="F91" s="38"/>
+      <c r="D91" s="36"/>
+      <c r="E91" s="36"/>
+      <c r="F91" s="37"/>
     </row>
     <row r="92" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A92" s="1">
@@ -2374,9 +2403,9 @@
         <v>44</v>
       </c>
       <c r="C92" s="7"/>
-      <c r="D92" s="37"/>
-      <c r="E92" s="37"/>
-      <c r="F92" s="38"/>
+      <c r="D92" s="36"/>
+      <c r="E92" s="36"/>
+      <c r="F92" s="37"/>
     </row>
     <row r="93" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A93" s="1">
@@ -2386,9 +2415,9 @@
         <v>29</v>
       </c>
       <c r="C93" s="7"/>
-      <c r="D93" s="37"/>
-      <c r="E93" s="37"/>
-      <c r="F93" s="38"/>
+      <c r="D93" s="36"/>
+      <c r="E93" s="36"/>
+      <c r="F93" s="37"/>
     </row>
     <row r="94" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A94" s="1">
@@ -2398,9 +2427,9 @@
         <v>45</v>
       </c>
       <c r="C94" s="7"/>
-      <c r="D94" s="37"/>
-      <c r="E94" s="37"/>
-      <c r="F94" s="38"/>
+      <c r="D94" s="36"/>
+      <c r="E94" s="36"/>
+      <c r="F94" s="37"/>
     </row>
     <row r="95" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A95" s="1">
@@ -2410,9 +2439,9 @@
         <v>22</v>
       </c>
       <c r="C95" s="7"/>
-      <c r="D95" s="37"/>
-      <c r="E95" s="37"/>
-      <c r="F95" s="38"/>
+      <c r="D95" s="36"/>
+      <c r="E95" s="36"/>
+      <c r="F95" s="37"/>
     </row>
     <row r="96" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A96" s="1">
@@ -2422,9 +2451,9 @@
         <v>30</v>
       </c>
       <c r="C96" s="7"/>
-      <c r="D96" s="37"/>
-      <c r="E96" s="37"/>
-      <c r="F96" s="38"/>
+      <c r="D96" s="36"/>
+      <c r="E96" s="36"/>
+      <c r="F96" s="37"/>
     </row>
     <row r="97" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A97" s="1">
@@ -2434,9 +2463,9 @@
         <v>47</v>
       </c>
       <c r="C97" s="7"/>
-      <c r="D97" s="37"/>
-      <c r="E97" s="37"/>
-      <c r="F97" s="38"/>
+      <c r="D97" s="36"/>
+      <c r="E97" s="36"/>
+      <c r="F97" s="37"/>
     </row>
     <row r="98" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A98" s="2">
@@ -2445,12 +2474,12 @@
       <c r="B98" s="21" t="s">
         <v>35</v>
       </c>
-      <c r="C98" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D98" s="37"/>
-      <c r="E98" s="37"/>
-      <c r="F98" s="38"/>
+      <c r="C98" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D98" s="36"/>
+      <c r="E98" s="36"/>
+      <c r="F98" s="37"/>
     </row>
     <row r="99" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A99" s="1">
@@ -2459,10 +2488,10 @@
       <c r="B99" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C99" s="27"/>
-      <c r="D99" s="37"/>
-      <c r="E99" s="37"/>
-      <c r="F99" s="38"/>
+      <c r="C99" s="31"/>
+      <c r="D99" s="36"/>
+      <c r="E99" s="36"/>
+      <c r="F99" s="37"/>
     </row>
     <row r="100" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A100" s="1">
@@ -2471,10 +2500,10 @@
       <c r="B100" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C100" s="27"/>
-      <c r="D100" s="37"/>
-      <c r="E100" s="37"/>
-      <c r="F100" s="38"/>
+      <c r="C100" s="31"/>
+      <c r="D100" s="36"/>
+      <c r="E100" s="36"/>
+      <c r="F100" s="37"/>
     </row>
     <row r="101" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A101" s="1">
@@ -2483,10 +2512,10 @@
       <c r="B101" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C101" s="27"/>
-      <c r="D101" s="37"/>
-      <c r="E101" s="37"/>
-      <c r="F101" s="38"/>
+      <c r="C101" s="31"/>
+      <c r="D101" s="36"/>
+      <c r="E101" s="36"/>
+      <c r="F101" s="37"/>
     </row>
     <row r="102" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A102" s="1">
@@ -2495,10 +2524,10 @@
       <c r="B102" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C102" s="27"/>
-      <c r="D102" s="37"/>
-      <c r="E102" s="37"/>
-      <c r="F102" s="38"/>
+      <c r="C102" s="31"/>
+      <c r="D102" s="36"/>
+      <c r="E102" s="36"/>
+      <c r="F102" s="37"/>
     </row>
     <row r="103" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A103" s="1">
@@ -2507,10 +2536,10 @@
       <c r="B103" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C103" s="27"/>
-      <c r="D103" s="37"/>
-      <c r="E103" s="37"/>
-      <c r="F103" s="38"/>
+      <c r="C103" s="31"/>
+      <c r="D103" s="36"/>
+      <c r="E103" s="36"/>
+      <c r="F103" s="37"/>
     </row>
     <row r="104" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A104" s="1">
@@ -2519,10 +2548,10 @@
       <c r="B104" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C104" s="27"/>
-      <c r="D104" s="37"/>
-      <c r="E104" s="37"/>
-      <c r="F104" s="38"/>
+      <c r="C104" s="31"/>
+      <c r="D104" s="36"/>
+      <c r="E104" s="36"/>
+      <c r="F104" s="37"/>
     </row>
     <row r="105" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A105" s="1">
@@ -2531,10 +2560,10 @@
       <c r="B105" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C105" s="28"/>
-      <c r="D105" s="37"/>
-      <c r="E105" s="37"/>
-      <c r="F105" s="38"/>
+      <c r="C105" s="32"/>
+      <c r="D105" s="36"/>
+      <c r="E105" s="36"/>
+      <c r="F105" s="37"/>
     </row>
     <row r="106" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A106" s="1">
@@ -2544,9 +2573,9 @@
         <v>10</v>
       </c>
       <c r="C106" s="9"/>
-      <c r="D106" s="42"/>
-      <c r="E106" s="42"/>
-      <c r="F106" s="43"/>
+      <c r="D106" s="38"/>
+      <c r="E106" s="38"/>
+      <c r="F106" s="39"/>
     </row>
     <row r="107" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A107" s="2">
@@ -2555,14 +2584,14 @@
       <c r="B107" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C107" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D107" s="29" t="s">
-        <v>99</v>
-      </c>
-      <c r="E107" s="35"/>
-      <c r="F107" s="36"/>
+      <c r="C107" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D107" s="33" t="s">
+        <v>98</v>
+      </c>
+      <c r="E107" s="34"/>
+      <c r="F107" s="35"/>
     </row>
     <row r="108" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A108" s="1">
@@ -2571,10 +2600,10 @@
       <c r="B108" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C108" s="27"/>
-      <c r="D108" s="37"/>
-      <c r="E108" s="37"/>
-      <c r="F108" s="38"/>
+      <c r="C108" s="31"/>
+      <c r="D108" s="36"/>
+      <c r="E108" s="36"/>
+      <c r="F108" s="37"/>
     </row>
     <row r="109" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A109" s="1">
@@ -2583,10 +2612,10 @@
       <c r="B109" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C109" s="27"/>
-      <c r="D109" s="37"/>
-      <c r="E109" s="37"/>
-      <c r="F109" s="38"/>
+      <c r="C109" s="31"/>
+      <c r="D109" s="36"/>
+      <c r="E109" s="36"/>
+      <c r="F109" s="37"/>
     </row>
     <row r="110" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A110" s="1">
@@ -2595,10 +2624,10 @@
       <c r="B110" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C110" s="27"/>
-      <c r="D110" s="37"/>
-      <c r="E110" s="37"/>
-      <c r="F110" s="38"/>
+      <c r="C110" s="31"/>
+      <c r="D110" s="36"/>
+      <c r="E110" s="36"/>
+      <c r="F110" s="37"/>
     </row>
     <row r="111" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A111" s="1">
@@ -2607,10 +2636,10 @@
       <c r="B111" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C111" s="27"/>
-      <c r="D111" s="37"/>
-      <c r="E111" s="37"/>
-      <c r="F111" s="38"/>
+      <c r="C111" s="31"/>
+      <c r="D111" s="36"/>
+      <c r="E111" s="36"/>
+      <c r="F111" s="37"/>
     </row>
     <row r="112" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A112" s="1">
@@ -2619,10 +2648,10 @@
       <c r="B112" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C112" s="27"/>
-      <c r="D112" s="37"/>
-      <c r="E112" s="37"/>
-      <c r="F112" s="38"/>
+      <c r="C112" s="31"/>
+      <c r="D112" s="36"/>
+      <c r="E112" s="36"/>
+      <c r="F112" s="37"/>
     </row>
     <row r="113" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A113" s="1">
@@ -2631,10 +2660,10 @@
       <c r="B113" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C113" s="27"/>
-      <c r="D113" s="37"/>
-      <c r="E113" s="37"/>
-      <c r="F113" s="38"/>
+      <c r="C113" s="31"/>
+      <c r="D113" s="36"/>
+      <c r="E113" s="36"/>
+      <c r="F113" s="37"/>
     </row>
     <row r="114" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A114" s="1">
@@ -2643,10 +2672,10 @@
       <c r="B114" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C114" s="28"/>
-      <c r="D114" s="37"/>
-      <c r="E114" s="37"/>
-      <c r="F114" s="38"/>
+      <c r="C114" s="32"/>
+      <c r="D114" s="36"/>
+      <c r="E114" s="36"/>
+      <c r="F114" s="37"/>
     </row>
     <row r="115" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A115" s="2">
@@ -2656,9 +2685,9 @@
         <v>11</v>
       </c>
       <c r="C115" s="7"/>
-      <c r="D115" s="37"/>
-      <c r="E115" s="37"/>
-      <c r="F115" s="38"/>
+      <c r="D115" s="36"/>
+      <c r="E115" s="36"/>
+      <c r="F115" s="37"/>
     </row>
     <row r="116" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A116" s="1">
@@ -2668,9 +2697,9 @@
         <v>48</v>
       </c>
       <c r="C116" s="7"/>
-      <c r="D116" s="37"/>
-      <c r="E116" s="37"/>
-      <c r="F116" s="38"/>
+      <c r="D116" s="36"/>
+      <c r="E116" s="36"/>
+      <c r="F116" s="37"/>
     </row>
     <row r="117" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A117" s="1">
@@ -2680,9 +2709,9 @@
         <v>50</v>
       </c>
       <c r="C117" s="7"/>
-      <c r="D117" s="37"/>
-      <c r="E117" s="37"/>
-      <c r="F117" s="38"/>
+      <c r="D117" s="36"/>
+      <c r="E117" s="36"/>
+      <c r="F117" s="37"/>
     </row>
     <row r="118" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A118" s="1">
@@ -2692,9 +2721,9 @@
         <v>51</v>
       </c>
       <c r="C118" s="7"/>
-      <c r="D118" s="37"/>
-      <c r="E118" s="37"/>
-      <c r="F118" s="38"/>
+      <c r="D118" s="36"/>
+      <c r="E118" s="36"/>
+      <c r="F118" s="37"/>
     </row>
     <row r="119" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A119" s="1">
@@ -2704,9 +2733,9 @@
         <v>33</v>
       </c>
       <c r="C119" s="7"/>
-      <c r="D119" s="37"/>
-      <c r="E119" s="37"/>
-      <c r="F119" s="38"/>
+      <c r="D119" s="36"/>
+      <c r="E119" s="36"/>
+      <c r="F119" s="37"/>
     </row>
     <row r="120" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A120" s="1">
@@ -2716,9 +2745,9 @@
         <v>52</v>
       </c>
       <c r="C120" s="7"/>
-      <c r="D120" s="37"/>
-      <c r="E120" s="37"/>
-      <c r="F120" s="38"/>
+      <c r="D120" s="36"/>
+      <c r="E120" s="36"/>
+      <c r="F120" s="37"/>
     </row>
     <row r="121" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A121" s="1">
@@ -2728,9 +2757,9 @@
         <v>23</v>
       </c>
       <c r="C121" s="7"/>
-      <c r="D121" s="37"/>
-      <c r="E121" s="37"/>
-      <c r="F121" s="38"/>
+      <c r="D121" s="36"/>
+      <c r="E121" s="36"/>
+      <c r="F121" s="37"/>
     </row>
     <row r="122" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A122" s="1">
@@ -2740,9 +2769,9 @@
         <v>53</v>
       </c>
       <c r="C122" s="7"/>
-      <c r="D122" s="37"/>
-      <c r="E122" s="37"/>
-      <c r="F122" s="38"/>
+      <c r="D122" s="36"/>
+      <c r="E122" s="36"/>
+      <c r="F122" s="37"/>
     </row>
     <row r="123" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A123" s="1">
@@ -2752,9 +2781,9 @@
         <v>50</v>
       </c>
       <c r="C123" s="7"/>
-      <c r="D123" s="37"/>
-      <c r="E123" s="37"/>
-      <c r="F123" s="38"/>
+      <c r="D123" s="36"/>
+      <c r="E123" s="36"/>
+      <c r="F123" s="37"/>
     </row>
     <row r="124" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A124" s="1">
@@ -2764,9 +2793,9 @@
         <v>42</v>
       </c>
       <c r="C124" s="7"/>
-      <c r="D124" s="37"/>
-      <c r="E124" s="37"/>
-      <c r="F124" s="38"/>
+      <c r="D124" s="36"/>
+      <c r="E124" s="36"/>
+      <c r="F124" s="37"/>
     </row>
     <row r="125" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A125" s="1">
@@ -2776,9 +2805,9 @@
         <v>54</v>
       </c>
       <c r="C125" s="7"/>
-      <c r="D125" s="37"/>
-      <c r="E125" s="37"/>
-      <c r="F125" s="38"/>
+      <c r="D125" s="36"/>
+      <c r="E125" s="36"/>
+      <c r="F125" s="37"/>
     </row>
     <row r="126" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A126" s="1">
@@ -2788,9 +2817,9 @@
         <v>55</v>
       </c>
       <c r="C126" s="7"/>
-      <c r="D126" s="37"/>
-      <c r="E126" s="37"/>
-      <c r="F126" s="38"/>
+      <c r="D126" s="36"/>
+      <c r="E126" s="36"/>
+      <c r="F126" s="37"/>
     </row>
     <row r="127" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A127" s="1">
@@ -2800,9 +2829,9 @@
         <v>56</v>
       </c>
       <c r="C127" s="7"/>
-      <c r="D127" s="37"/>
-      <c r="E127" s="37"/>
-      <c r="F127" s="38"/>
+      <c r="D127" s="36"/>
+      <c r="E127" s="36"/>
+      <c r="F127" s="37"/>
     </row>
     <row r="128" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A128" s="15">
@@ -2811,12 +2840,12 @@
       <c r="B128" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C128" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D128" s="37"/>
-      <c r="E128" s="37"/>
-      <c r="F128" s="38"/>
+      <c r="C128" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D128" s="36"/>
+      <c r="E128" s="36"/>
+      <c r="F128" s="37"/>
     </row>
     <row r="129" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A129" s="1">
@@ -2825,10 +2854,10 @@
       <c r="B129" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C129" s="27"/>
-      <c r="D129" s="37"/>
-      <c r="E129" s="37"/>
-      <c r="F129" s="38"/>
+      <c r="C129" s="31"/>
+      <c r="D129" s="36"/>
+      <c r="E129" s="36"/>
+      <c r="F129" s="37"/>
     </row>
     <row r="130" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A130" s="1">
@@ -2837,10 +2866,10 @@
       <c r="B130" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C130" s="27"/>
-      <c r="D130" s="37"/>
-      <c r="E130" s="37"/>
-      <c r="F130" s="38"/>
+      <c r="C130" s="31"/>
+      <c r="D130" s="36"/>
+      <c r="E130" s="36"/>
+      <c r="F130" s="37"/>
     </row>
     <row r="131" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A131" s="1">
@@ -2849,10 +2878,10 @@
       <c r="B131" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C131" s="27"/>
-      <c r="D131" s="37"/>
-      <c r="E131" s="37"/>
-      <c r="F131" s="38"/>
+      <c r="C131" s="31"/>
+      <c r="D131" s="36"/>
+      <c r="E131" s="36"/>
+      <c r="F131" s="37"/>
     </row>
     <row r="132" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A132" s="1">
@@ -2861,10 +2890,10 @@
       <c r="B132" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C132" s="27"/>
-      <c r="D132" s="37"/>
-      <c r="E132" s="37"/>
-      <c r="F132" s="38"/>
+      <c r="C132" s="31"/>
+      <c r="D132" s="36"/>
+      <c r="E132" s="36"/>
+      <c r="F132" s="37"/>
     </row>
     <row r="133" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A133" s="1">
@@ -2873,10 +2902,10 @@
       <c r="B133" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C133" s="27"/>
-      <c r="D133" s="37"/>
-      <c r="E133" s="37"/>
-      <c r="F133" s="38"/>
+      <c r="C133" s="31"/>
+      <c r="D133" s="36"/>
+      <c r="E133" s="36"/>
+      <c r="F133" s="37"/>
     </row>
     <row r="134" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A134" s="1">
@@ -2885,10 +2914,10 @@
       <c r="B134" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C134" s="27"/>
-      <c r="D134" s="37"/>
-      <c r="E134" s="37"/>
-      <c r="F134" s="38"/>
+      <c r="C134" s="31"/>
+      <c r="D134" s="36"/>
+      <c r="E134" s="36"/>
+      <c r="F134" s="37"/>
     </row>
     <row r="135" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A135" s="1">
@@ -2897,10 +2926,10 @@
       <c r="B135" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C135" s="28"/>
-      <c r="D135" s="37"/>
-      <c r="E135" s="37"/>
-      <c r="F135" s="38"/>
+      <c r="C135" s="32"/>
+      <c r="D135" s="36"/>
+      <c r="E135" s="36"/>
+      <c r="F135" s="37"/>
     </row>
     <row r="136" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A136" s="1">
@@ -2910,9 +2939,9 @@
         <v>10</v>
       </c>
       <c r="C136" s="7"/>
-      <c r="D136" s="37"/>
-      <c r="E136" s="37"/>
-      <c r="F136" s="38"/>
+      <c r="D136" s="36"/>
+      <c r="E136" s="36"/>
+      <c r="F136" s="37"/>
     </row>
     <row r="137" spans="1:6" ht="15" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A137" s="1">
@@ -2921,14 +2950,14 @@
       <c r="B137" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C137" s="46" t="s">
-        <v>93</v>
-      </c>
-      <c r="D137" s="29" t="s">
-        <v>103</v>
-      </c>
-      <c r="E137" s="29"/>
-      <c r="F137" s="30"/>
+      <c r="C137" s="40" t="s">
+        <v>92</v>
+      </c>
+      <c r="D137" s="33" t="s">
+        <v>102</v>
+      </c>
+      <c r="E137" s="33"/>
+      <c r="F137" s="44"/>
     </row>
     <row r="138" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A138" s="1">
@@ -2937,10 +2966,10 @@
       <c r="B138" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C138" s="27"/>
-      <c r="D138" s="31"/>
-      <c r="E138" s="31"/>
-      <c r="F138" s="32"/>
+      <c r="C138" s="31"/>
+      <c r="D138" s="45"/>
+      <c r="E138" s="45"/>
+      <c r="F138" s="46"/>
     </row>
     <row r="139" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A139" s="1">
@@ -2949,10 +2978,10 @@
       <c r="B139" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C139" s="27"/>
-      <c r="D139" s="31"/>
-      <c r="E139" s="31"/>
-      <c r="F139" s="32"/>
+      <c r="C139" s="31"/>
+      <c r="D139" s="45"/>
+      <c r="E139" s="45"/>
+      <c r="F139" s="46"/>
     </row>
     <row r="140" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A140" s="1">
@@ -2961,10 +2990,10 @@
       <c r="B140" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C140" s="27"/>
-      <c r="D140" s="31"/>
-      <c r="E140" s="31"/>
-      <c r="F140" s="32"/>
+      <c r="C140" s="31"/>
+      <c r="D140" s="45"/>
+      <c r="E140" s="45"/>
+      <c r="F140" s="46"/>
     </row>
     <row r="141" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A141" s="1">
@@ -2973,10 +3002,10 @@
       <c r="B141" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C141" s="27"/>
-      <c r="D141" s="31"/>
-      <c r="E141" s="31"/>
-      <c r="F141" s="32"/>
+      <c r="C141" s="31"/>
+      <c r="D141" s="45"/>
+      <c r="E141" s="45"/>
+      <c r="F141" s="46"/>
     </row>
     <row r="142" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A142" s="1">
@@ -2985,10 +3014,10 @@
       <c r="B142" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C142" s="27"/>
-      <c r="D142" s="31"/>
-      <c r="E142" s="31"/>
-      <c r="F142" s="32"/>
+      <c r="C142" s="31"/>
+      <c r="D142" s="45"/>
+      <c r="E142" s="45"/>
+      <c r="F142" s="46"/>
     </row>
     <row r="143" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A143" s="1">
@@ -2997,10 +3026,10 @@
       <c r="B143" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C143" s="27"/>
-      <c r="D143" s="31"/>
-      <c r="E143" s="31"/>
-      <c r="F143" s="32"/>
+      <c r="C143" s="31"/>
+      <c r="D143" s="45"/>
+      <c r="E143" s="45"/>
+      <c r="F143" s="46"/>
     </row>
     <row r="144" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A144" s="1">
@@ -3009,10 +3038,10 @@
       <c r="B144" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C144" s="28"/>
-      <c r="D144" s="31"/>
-      <c r="E144" s="31"/>
-      <c r="F144" s="32"/>
+      <c r="C144" s="32"/>
+      <c r="D144" s="45"/>
+      <c r="E144" s="45"/>
+      <c r="F144" s="46"/>
     </row>
     <row r="145" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A145" s="1">
@@ -3022,9 +3051,9 @@
         <v>57</v>
       </c>
       <c r="C145" s="7"/>
-      <c r="D145" s="31"/>
-      <c r="E145" s="31"/>
-      <c r="F145" s="32"/>
+      <c r="D145" s="45"/>
+      <c r="E145" s="45"/>
+      <c r="F145" s="46"/>
     </row>
     <row r="146" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A146" s="1">
@@ -3034,9 +3063,9 @@
         <v>58</v>
       </c>
       <c r="C146" s="7"/>
-      <c r="D146" s="31"/>
-      <c r="E146" s="31"/>
-      <c r="F146" s="32"/>
+      <c r="D146" s="45"/>
+      <c r="E146" s="45"/>
+      <c r="F146" s="46"/>
     </row>
     <row r="147" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A147" s="1">
@@ -3046,9 +3075,9 @@
         <v>62</v>
       </c>
       <c r="C147" s="7"/>
-      <c r="D147" s="31"/>
-      <c r="E147" s="31"/>
-      <c r="F147" s="32"/>
+      <c r="D147" s="45"/>
+      <c r="E147" s="45"/>
+      <c r="F147" s="46"/>
     </row>
     <row r="148" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A148" s="1">
@@ -3058,9 +3087,9 @@
         <v>63</v>
       </c>
       <c r="C148" s="7"/>
-      <c r="D148" s="31"/>
-      <c r="E148" s="31"/>
-      <c r="F148" s="32"/>
+      <c r="D148" s="45"/>
+      <c r="E148" s="45"/>
+      <c r="F148" s="46"/>
     </row>
     <row r="149" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A149" s="1">
@@ -3070,11 +3099,11 @@
         <v>61</v>
       </c>
       <c r="C149" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D149" s="31"/>
-      <c r="E149" s="31"/>
-      <c r="F149" s="32"/>
+        <v>99</v>
+      </c>
+      <c r="D149" s="45"/>
+      <c r="E149" s="45"/>
+      <c r="F149" s="46"/>
     </row>
     <row r="150" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A150" s="1">
@@ -3083,12 +3112,12 @@
       <c r="B150" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C150" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D150" s="31"/>
-      <c r="E150" s="31"/>
-      <c r="F150" s="32"/>
+      <c r="C150" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D150" s="45"/>
+      <c r="E150" s="45"/>
+      <c r="F150" s="46"/>
     </row>
     <row r="151" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A151" s="1">
@@ -3097,10 +3126,10 @@
       <c r="B151" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C151" s="27"/>
-      <c r="D151" s="31"/>
-      <c r="E151" s="31"/>
-      <c r="F151" s="32"/>
+      <c r="C151" s="31"/>
+      <c r="D151" s="45"/>
+      <c r="E151" s="45"/>
+      <c r="F151" s="46"/>
     </row>
     <row r="152" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A152" s="1">
@@ -3109,10 +3138,10 @@
       <c r="B152" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C152" s="27"/>
-      <c r="D152" s="31"/>
-      <c r="E152" s="31"/>
-      <c r="F152" s="32"/>
+      <c r="C152" s="31"/>
+      <c r="D152" s="45"/>
+      <c r="E152" s="45"/>
+      <c r="F152" s="46"/>
     </row>
     <row r="153" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A153" s="1">
@@ -3121,10 +3150,10 @@
       <c r="B153" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C153" s="27"/>
-      <c r="D153" s="31"/>
-      <c r="E153" s="31"/>
-      <c r="F153" s="32"/>
+      <c r="C153" s="31"/>
+      <c r="D153" s="45"/>
+      <c r="E153" s="45"/>
+      <c r="F153" s="46"/>
     </row>
     <row r="154" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A154" s="1">
@@ -3133,10 +3162,10 @@
       <c r="B154" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C154" s="27"/>
-      <c r="D154" s="31"/>
-      <c r="E154" s="31"/>
-      <c r="F154" s="32"/>
+      <c r="C154" s="31"/>
+      <c r="D154" s="45"/>
+      <c r="E154" s="45"/>
+      <c r="F154" s="46"/>
     </row>
     <row r="155" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A155" s="1">
@@ -3145,10 +3174,10 @@
       <c r="B155" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C155" s="27"/>
-      <c r="D155" s="31"/>
-      <c r="E155" s="31"/>
-      <c r="F155" s="32"/>
+      <c r="C155" s="31"/>
+      <c r="D155" s="45"/>
+      <c r="E155" s="45"/>
+      <c r="F155" s="46"/>
     </row>
     <row r="156" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A156" s="1">
@@ -3157,10 +3186,10 @@
       <c r="B156" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C156" s="27"/>
-      <c r="D156" s="31"/>
-      <c r="E156" s="31"/>
-      <c r="F156" s="32"/>
+      <c r="C156" s="31"/>
+      <c r="D156" s="45"/>
+      <c r="E156" s="45"/>
+      <c r="F156" s="46"/>
     </row>
     <row r="157" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A157" s="1">
@@ -3169,10 +3198,10 @@
       <c r="B157" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C157" s="28"/>
-      <c r="D157" s="31"/>
-      <c r="E157" s="31"/>
-      <c r="F157" s="32"/>
+      <c r="C157" s="32"/>
+      <c r="D157" s="45"/>
+      <c r="E157" s="45"/>
+      <c r="F157" s="46"/>
     </row>
     <row r="158" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A158" s="15">
@@ -3182,11 +3211,11 @@
         <v>59</v>
       </c>
       <c r="C158" s="25" t="s">
-        <v>101</v>
-      </c>
-      <c r="D158" s="31"/>
-      <c r="E158" s="31"/>
-      <c r="F158" s="32"/>
+        <v>100</v>
+      </c>
+      <c r="D158" s="45"/>
+      <c r="E158" s="45"/>
+      <c r="F158" s="46"/>
     </row>
     <row r="159" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A159" s="2">
@@ -3196,11 +3225,11 @@
         <v>61</v>
       </c>
       <c r="C159" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="D159" s="31"/>
-      <c r="E159" s="31"/>
-      <c r="F159" s="32"/>
+        <v>99</v>
+      </c>
+      <c r="D159" s="45"/>
+      <c r="E159" s="45"/>
+      <c r="F159" s="46"/>
     </row>
     <row r="160" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A160" s="1">
@@ -3209,12 +3238,12 @@
       <c r="B160" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C160" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D160" s="31"/>
-      <c r="E160" s="31"/>
-      <c r="F160" s="32"/>
+      <c r="C160" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D160" s="45"/>
+      <c r="E160" s="45"/>
+      <c r="F160" s="46"/>
     </row>
     <row r="161" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A161" s="1">
@@ -3223,10 +3252,10 @@
       <c r="B161" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C161" s="27"/>
-      <c r="D161" s="31"/>
-      <c r="E161" s="31"/>
-      <c r="F161" s="32"/>
+      <c r="C161" s="31"/>
+      <c r="D161" s="45"/>
+      <c r="E161" s="45"/>
+      <c r="F161" s="46"/>
     </row>
     <row r="162" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A162" s="1">
@@ -3235,10 +3264,10 @@
       <c r="B162" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C162" s="27"/>
-      <c r="D162" s="31"/>
-      <c r="E162" s="31"/>
-      <c r="F162" s="32"/>
+      <c r="C162" s="31"/>
+      <c r="D162" s="45"/>
+      <c r="E162" s="45"/>
+      <c r="F162" s="46"/>
     </row>
     <row r="163" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A163" s="1">
@@ -3247,10 +3276,10 @@
       <c r="B163" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C163" s="27"/>
-      <c r="D163" s="31"/>
-      <c r="E163" s="31"/>
-      <c r="F163" s="32"/>
+      <c r="C163" s="31"/>
+      <c r="D163" s="45"/>
+      <c r="E163" s="45"/>
+      <c r="F163" s="46"/>
     </row>
     <row r="164" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A164" s="1">
@@ -3259,10 +3288,10 @@
       <c r="B164" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C164" s="27"/>
-      <c r="D164" s="31"/>
-      <c r="E164" s="31"/>
-      <c r="F164" s="32"/>
+      <c r="C164" s="31"/>
+      <c r="D164" s="45"/>
+      <c r="E164" s="45"/>
+      <c r="F164" s="46"/>
     </row>
     <row r="165" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A165" s="1">
@@ -3271,10 +3300,10 @@
       <c r="B165" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C165" s="27"/>
-      <c r="D165" s="31"/>
-      <c r="E165" s="31"/>
-      <c r="F165" s="32"/>
+      <c r="C165" s="31"/>
+      <c r="D165" s="45"/>
+      <c r="E165" s="45"/>
+      <c r="F165" s="46"/>
     </row>
     <row r="166" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A166" s="1">
@@ -3283,10 +3312,10 @@
       <c r="B166" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C166" s="27"/>
-      <c r="D166" s="31"/>
-      <c r="E166" s="31"/>
-      <c r="F166" s="32"/>
+      <c r="C166" s="31"/>
+      <c r="D166" s="45"/>
+      <c r="E166" s="45"/>
+      <c r="F166" s="46"/>
     </row>
     <row r="167" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A167" s="1">
@@ -3295,10 +3324,10 @@
       <c r="B167" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C167" s="28"/>
-      <c r="D167" s="31"/>
-      <c r="E167" s="31"/>
-      <c r="F167" s="32"/>
+      <c r="C167" s="32"/>
+      <c r="D167" s="45"/>
+      <c r="E167" s="45"/>
+      <c r="F167" s="46"/>
     </row>
     <row r="168" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A168" s="1">
@@ -3308,11 +3337,11 @@
         <v>60</v>
       </c>
       <c r="C168" s="26" t="s">
-        <v>102</v>
-      </c>
-      <c r="D168" s="33"/>
-      <c r="E168" s="33"/>
-      <c r="F168" s="34"/>
+        <v>101</v>
+      </c>
+      <c r="D168" s="47"/>
+      <c r="E168" s="47"/>
+      <c r="F168" s="48"/>
     </row>
     <row r="169" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A169" s="1">
@@ -3321,14 +3350,14 @@
       <c r="B169" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="C169" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D169" s="29" t="s">
-        <v>104</v>
-      </c>
-      <c r="E169" s="35"/>
-      <c r="F169" s="36"/>
+      <c r="C169" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D169" s="33" t="s">
+        <v>103</v>
+      </c>
+      <c r="E169" s="34"/>
+      <c r="F169" s="35"/>
     </row>
     <row r="170" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A170" s="1">
@@ -3337,10 +3366,10 @@
       <c r="B170" s="6" t="s">
         <v>31</v>
       </c>
-      <c r="C170" s="27"/>
-      <c r="D170" s="37"/>
-      <c r="E170" s="37"/>
-      <c r="F170" s="38"/>
+      <c r="C170" s="31"/>
+      <c r="D170" s="36"/>
+      <c r="E170" s="36"/>
+      <c r="F170" s="37"/>
     </row>
     <row r="171" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A171" s="1">
@@ -3349,10 +3378,10 @@
       <c r="B171" s="6" t="s">
         <v>34</v>
       </c>
-      <c r="C171" s="27"/>
-      <c r="D171" s="37"/>
-      <c r="E171" s="37"/>
-      <c r="F171" s="38"/>
+      <c r="C171" s="31"/>
+      <c r="D171" s="36"/>
+      <c r="E171" s="36"/>
+      <c r="F171" s="37"/>
     </row>
     <row r="172" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A172" s="1">
@@ -3361,10 +3390,10 @@
       <c r="B172" s="6" t="s">
         <v>35</v>
       </c>
-      <c r="C172" s="27"/>
-      <c r="D172" s="37"/>
-      <c r="E172" s="37"/>
-      <c r="F172" s="38"/>
+      <c r="C172" s="31"/>
+      <c r="D172" s="36"/>
+      <c r="E172" s="36"/>
+      <c r="F172" s="37"/>
     </row>
     <row r="173" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A173" s="1">
@@ -3373,10 +3402,10 @@
       <c r="B173" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C173" s="27"/>
-      <c r="D173" s="37"/>
-      <c r="E173" s="37"/>
-      <c r="F173" s="38"/>
+      <c r="C173" s="31"/>
+      <c r="D173" s="36"/>
+      <c r="E173" s="36"/>
+      <c r="F173" s="37"/>
     </row>
     <row r="174" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A174" s="1">
@@ -3385,10 +3414,10 @@
       <c r="B174" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C174" s="27"/>
-      <c r="D174" s="37"/>
-      <c r="E174" s="37"/>
-      <c r="F174" s="38"/>
+      <c r="C174" s="31"/>
+      <c r="D174" s="36"/>
+      <c r="E174" s="36"/>
+      <c r="F174" s="37"/>
     </row>
     <row r="175" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A175" s="1">
@@ -3397,10 +3426,10 @@
       <c r="B175" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="C175" s="27"/>
-      <c r="D175" s="37"/>
-      <c r="E175" s="37"/>
-      <c r="F175" s="38"/>
+      <c r="C175" s="31"/>
+      <c r="D175" s="36"/>
+      <c r="E175" s="36"/>
+      <c r="F175" s="37"/>
     </row>
     <row r="176" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A176" s="1">
@@ -3409,10 +3438,10 @@
       <c r="B176" s="16" t="s">
         <v>38</v>
       </c>
-      <c r="C176" s="28"/>
-      <c r="D176" s="37"/>
-      <c r="E176" s="37"/>
-      <c r="F176" s="38"/>
+      <c r="C176" s="32"/>
+      <c r="D176" s="36"/>
+      <c r="E176" s="36"/>
+      <c r="F176" s="37"/>
     </row>
     <row r="177" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A177" s="1">
@@ -3422,22 +3451,22 @@
         <v>65</v>
       </c>
       <c r="C177" s="7"/>
-      <c r="D177" s="37"/>
-      <c r="E177" s="37"/>
-      <c r="F177" s="38"/>
-      <c r="H177" s="48" t="s">
-        <v>109</v>
-      </c>
-      <c r="I177" s="44"/>
-      <c r="J177" s="44"/>
-      <c r="K177" s="44"/>
-      <c r="L177" s="44"/>
-      <c r="M177" s="44"/>
-      <c r="N177" s="44"/>
-      <c r="O177" s="44"/>
-      <c r="P177" s="44"/>
-      <c r="Q177" s="44"/>
-      <c r="R177" s="44"/>
+      <c r="D177" s="36"/>
+      <c r="E177" s="36"/>
+      <c r="F177" s="37"/>
+      <c r="H177" s="28" t="s">
+        <v>113</v>
+      </c>
+      <c r="I177" s="29"/>
+      <c r="J177" s="29"/>
+      <c r="K177" s="29"/>
+      <c r="L177" s="29"/>
+      <c r="M177" s="29"/>
+      <c r="N177" s="29"/>
+      <c r="O177" s="29"/>
+      <c r="P177" s="29"/>
+      <c r="Q177" s="29"/>
+      <c r="R177" s="29"/>
     </row>
     <row r="178" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A178" s="1">
@@ -3447,20 +3476,20 @@
         <v>54</v>
       </c>
       <c r="C178" s="7"/>
-      <c r="D178" s="37"/>
-      <c r="E178" s="37"/>
-      <c r="F178" s="38"/>
-      <c r="H178" s="44"/>
-      <c r="I178" s="44"/>
-      <c r="J178" s="44"/>
-      <c r="K178" s="44"/>
-      <c r="L178" s="44"/>
-      <c r="M178" s="44"/>
-      <c r="N178" s="44"/>
-      <c r="O178" s="44"/>
-      <c r="P178" s="44"/>
-      <c r="Q178" s="44"/>
-      <c r="R178" s="44"/>
+      <c r="D178" s="36"/>
+      <c r="E178" s="36"/>
+      <c r="F178" s="37"/>
+      <c r="H178" s="29"/>
+      <c r="I178" s="29"/>
+      <c r="J178" s="29"/>
+      <c r="K178" s="29"/>
+      <c r="L178" s="29"/>
+      <c r="M178" s="29"/>
+      <c r="N178" s="29"/>
+      <c r="O178" s="29"/>
+      <c r="P178" s="29"/>
+      <c r="Q178" s="29"/>
+      <c r="R178" s="29"/>
     </row>
     <row r="179" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A179" s="2">
@@ -3470,22 +3499,22 @@
         <v>66</v>
       </c>
       <c r="C179" s="7" t="s">
-        <v>105</v>
-      </c>
-      <c r="D179" s="37"/>
-      <c r="E179" s="37"/>
-      <c r="F179" s="38"/>
-      <c r="H179" s="44"/>
-      <c r="I179" s="44"/>
-      <c r="J179" s="44"/>
-      <c r="K179" s="44"/>
-      <c r="L179" s="44"/>
-      <c r="M179" s="44"/>
-      <c r="N179" s="44"/>
-      <c r="O179" s="44"/>
-      <c r="P179" s="44"/>
-      <c r="Q179" s="44"/>
-      <c r="R179" s="44"/>
+        <v>104</v>
+      </c>
+      <c r="D179" s="36"/>
+      <c r="E179" s="36"/>
+      <c r="F179" s="37"/>
+      <c r="H179" s="29"/>
+      <c r="I179" s="29"/>
+      <c r="J179" s="29"/>
+      <c r="K179" s="29"/>
+      <c r="L179" s="29"/>
+      <c r="M179" s="29"/>
+      <c r="N179" s="29"/>
+      <c r="O179" s="29"/>
+      <c r="P179" s="29"/>
+      <c r="Q179" s="29"/>
+      <c r="R179" s="29"/>
     </row>
     <row r="180" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A180" s="1">
@@ -3495,20 +3524,20 @@
         <v>67</v>
       </c>
       <c r="C180" s="7"/>
-      <c r="D180" s="37"/>
-      <c r="E180" s="37"/>
-      <c r="F180" s="38"/>
-      <c r="H180" s="44"/>
-      <c r="I180" s="44"/>
-      <c r="J180" s="44"/>
-      <c r="K180" s="44"/>
-      <c r="L180" s="44"/>
-      <c r="M180" s="44"/>
-      <c r="N180" s="44"/>
-      <c r="O180" s="44"/>
-      <c r="P180" s="44"/>
-      <c r="Q180" s="44"/>
-      <c r="R180" s="44"/>
+      <c r="D180" s="36"/>
+      <c r="E180" s="36"/>
+      <c r="F180" s="37"/>
+      <c r="H180" s="29"/>
+      <c r="I180" s="29"/>
+      <c r="J180" s="29"/>
+      <c r="K180" s="29"/>
+      <c r="L180" s="29"/>
+      <c r="M180" s="29"/>
+      <c r="N180" s="29"/>
+      <c r="O180" s="29"/>
+      <c r="P180" s="29"/>
+      <c r="Q180" s="29"/>
+      <c r="R180" s="29"/>
     </row>
     <row r="181" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A181" s="1">
@@ -3518,20 +3547,20 @@
         <v>33</v>
       </c>
       <c r="C181" s="7"/>
-      <c r="D181" s="37"/>
-      <c r="E181" s="37"/>
-      <c r="F181" s="38"/>
-      <c r="H181" s="44"/>
-      <c r="I181" s="44"/>
-      <c r="J181" s="44"/>
-      <c r="K181" s="44"/>
-      <c r="L181" s="44"/>
-      <c r="M181" s="44"/>
-      <c r="N181" s="44"/>
-      <c r="O181" s="44"/>
-      <c r="P181" s="44"/>
-      <c r="Q181" s="44"/>
-      <c r="R181" s="44"/>
+      <c r="D181" s="36"/>
+      <c r="E181" s="36"/>
+      <c r="F181" s="37"/>
+      <c r="H181" s="29"/>
+      <c r="I181" s="29"/>
+      <c r="J181" s="29"/>
+      <c r="K181" s="29"/>
+      <c r="L181" s="29"/>
+      <c r="M181" s="29"/>
+      <c r="N181" s="29"/>
+      <c r="O181" s="29"/>
+      <c r="P181" s="29"/>
+      <c r="Q181" s="29"/>
+      <c r="R181" s="29"/>
     </row>
     <row r="182" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A182" s="1">
@@ -3541,20 +3570,20 @@
         <v>52</v>
       </c>
       <c r="C182" s="7"/>
-      <c r="D182" s="37"/>
-      <c r="E182" s="37"/>
-      <c r="F182" s="38"/>
-      <c r="H182" s="44"/>
-      <c r="I182" s="44"/>
-      <c r="J182" s="44"/>
-      <c r="K182" s="44"/>
-      <c r="L182" s="44"/>
-      <c r="M182" s="44"/>
-      <c r="N182" s="44"/>
-      <c r="O182" s="44"/>
-      <c r="P182" s="44"/>
-      <c r="Q182" s="44"/>
-      <c r="R182" s="44"/>
+      <c r="D182" s="36"/>
+      <c r="E182" s="36"/>
+      <c r="F182" s="37"/>
+      <c r="H182" s="29"/>
+      <c r="I182" s="29"/>
+      <c r="J182" s="29"/>
+      <c r="K182" s="29"/>
+      <c r="L182" s="29"/>
+      <c r="M182" s="29"/>
+      <c r="N182" s="29"/>
+      <c r="O182" s="29"/>
+      <c r="P182" s="29"/>
+      <c r="Q182" s="29"/>
+      <c r="R182" s="29"/>
     </row>
     <row r="183" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A183" s="1">
@@ -3566,20 +3595,20 @@
       <c r="C183" s="7" t="s">
         <v>69</v>
       </c>
-      <c r="D183" s="37"/>
-      <c r="E183" s="37"/>
-      <c r="F183" s="38"/>
-      <c r="H183" s="44"/>
-      <c r="I183" s="44"/>
-      <c r="J183" s="44"/>
-      <c r="K183" s="44"/>
-      <c r="L183" s="44"/>
-      <c r="M183" s="44"/>
-      <c r="N183" s="44"/>
-      <c r="O183" s="44"/>
-      <c r="P183" s="44"/>
-      <c r="Q183" s="44"/>
-      <c r="R183" s="44"/>
+      <c r="D183" s="36"/>
+      <c r="E183" s="36"/>
+      <c r="F183" s="37"/>
+      <c r="H183" s="29"/>
+      <c r="I183" s="29"/>
+      <c r="J183" s="29"/>
+      <c r="K183" s="29"/>
+      <c r="L183" s="29"/>
+      <c r="M183" s="29"/>
+      <c r="N183" s="29"/>
+      <c r="O183" s="29"/>
+      <c r="P183" s="29"/>
+      <c r="Q183" s="29"/>
+      <c r="R183" s="29"/>
     </row>
     <row r="184" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A184" s="1">
@@ -3588,21 +3617,23 @@
       <c r="B184" s="6" t="s">
         <v>70</v>
       </c>
-      <c r="C184" s="7"/>
-      <c r="D184" s="37"/>
-      <c r="E184" s="37"/>
-      <c r="F184" s="38"/>
-      <c r="H184" s="44"/>
-      <c r="I184" s="44"/>
-      <c r="J184" s="44"/>
-      <c r="K184" s="44"/>
-      <c r="L184" s="44"/>
-      <c r="M184" s="44"/>
-      <c r="N184" s="44"/>
-      <c r="O184" s="44"/>
-      <c r="P184" s="44"/>
-      <c r="Q184" s="44"/>
-      <c r="R184" s="44"/>
+      <c r="C184" s="7" t="s">
+        <v>109</v>
+      </c>
+      <c r="D184" s="36"/>
+      <c r="E184" s="36"/>
+      <c r="F184" s="37"/>
+      <c r="H184" s="29"/>
+      <c r="I184" s="29"/>
+      <c r="J184" s="29"/>
+      <c r="K184" s="29"/>
+      <c r="L184" s="29"/>
+      <c r="M184" s="29"/>
+      <c r="N184" s="29"/>
+      <c r="O184" s="29"/>
+      <c r="P184" s="29"/>
+      <c r="Q184" s="29"/>
+      <c r="R184" s="29"/>
     </row>
     <row r="185" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A185" s="1">
@@ -3612,20 +3643,20 @@
         <v>55</v>
       </c>
       <c r="C185" s="7"/>
-      <c r="D185" s="37"/>
-      <c r="E185" s="37"/>
-      <c r="F185" s="38"/>
-      <c r="H185" s="44"/>
-      <c r="I185" s="44"/>
-      <c r="J185" s="44"/>
-      <c r="K185" s="44"/>
-      <c r="L185" s="44"/>
-      <c r="M185" s="44"/>
-      <c r="N185" s="44"/>
-      <c r="O185" s="44"/>
-      <c r="P185" s="44"/>
-      <c r="Q185" s="44"/>
-      <c r="R185" s="44"/>
+      <c r="D185" s="36"/>
+      <c r="E185" s="36"/>
+      <c r="F185" s="37"/>
+      <c r="H185" s="29"/>
+      <c r="I185" s="29"/>
+      <c r="J185" s="29"/>
+      <c r="K185" s="29"/>
+      <c r="L185" s="29"/>
+      <c r="M185" s="29"/>
+      <c r="N185" s="29"/>
+      <c r="O185" s="29"/>
+      <c r="P185" s="29"/>
+      <c r="Q185" s="29"/>
+      <c r="R185" s="29"/>
     </row>
     <row r="186" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A186" s="1">
@@ -3634,21 +3665,23 @@
       <c r="B186" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C186" s="7"/>
-      <c r="D186" s="37"/>
-      <c r="E186" s="37"/>
-      <c r="F186" s="38"/>
-      <c r="H186" s="44"/>
-      <c r="I186" s="44"/>
-      <c r="J186" s="44"/>
-      <c r="K186" s="44"/>
-      <c r="L186" s="44"/>
-      <c r="M186" s="44"/>
-      <c r="N186" s="44"/>
-      <c r="O186" s="44"/>
-      <c r="P186" s="44"/>
-      <c r="Q186" s="44"/>
-      <c r="R186" s="44"/>
+      <c r="C186" s="7" t="s">
+        <v>108</v>
+      </c>
+      <c r="D186" s="36"/>
+      <c r="E186" s="36"/>
+      <c r="F186" s="37"/>
+      <c r="H186" s="29"/>
+      <c r="I186" s="29"/>
+      <c r="J186" s="29"/>
+      <c r="K186" s="29"/>
+      <c r="L186" s="29"/>
+      <c r="M186" s="29"/>
+      <c r="N186" s="29"/>
+      <c r="O186" s="29"/>
+      <c r="P186" s="29"/>
+      <c r="Q186" s="29"/>
+      <c r="R186" s="29"/>
     </row>
     <row r="187" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A187" s="1">
@@ -3658,20 +3691,20 @@
         <v>74</v>
       </c>
       <c r="C187" s="7"/>
-      <c r="D187" s="37"/>
-      <c r="E187" s="37"/>
-      <c r="F187" s="38"/>
-      <c r="H187" s="44"/>
-      <c r="I187" s="44"/>
-      <c r="J187" s="44"/>
-      <c r="K187" s="44"/>
-      <c r="L187" s="44"/>
-      <c r="M187" s="44"/>
-      <c r="N187" s="44"/>
-      <c r="O187" s="44"/>
-      <c r="P187" s="44"/>
-      <c r="Q187" s="44"/>
-      <c r="R187" s="44"/>
+      <c r="D187" s="36"/>
+      <c r="E187" s="36"/>
+      <c r="F187" s="37"/>
+      <c r="H187" s="29"/>
+      <c r="I187" s="29"/>
+      <c r="J187" s="29"/>
+      <c r="K187" s="29"/>
+      <c r="L187" s="29"/>
+      <c r="M187" s="29"/>
+      <c r="N187" s="29"/>
+      <c r="O187" s="29"/>
+      <c r="P187" s="29"/>
+      <c r="Q187" s="29"/>
+      <c r="R187" s="29"/>
     </row>
     <row r="188" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A188" s="1">
@@ -3681,20 +3714,20 @@
         <v>80</v>
       </c>
       <c r="C188" s="7"/>
-      <c r="D188" s="37"/>
-      <c r="E188" s="37"/>
-      <c r="F188" s="38"/>
-      <c r="H188" s="44"/>
-      <c r="I188" s="44"/>
-      <c r="J188" s="44"/>
-      <c r="K188" s="44"/>
-      <c r="L188" s="44"/>
-      <c r="M188" s="44"/>
-      <c r="N188" s="44"/>
-      <c r="O188" s="44"/>
-      <c r="P188" s="44"/>
-      <c r="Q188" s="44"/>
-      <c r="R188" s="44"/>
+      <c r="D188" s="36"/>
+      <c r="E188" s="36"/>
+      <c r="F188" s="37"/>
+      <c r="H188" s="29"/>
+      <c r="I188" s="29"/>
+      <c r="J188" s="29"/>
+      <c r="K188" s="29"/>
+      <c r="L188" s="29"/>
+      <c r="M188" s="29"/>
+      <c r="N188" s="29"/>
+      <c r="O188" s="29"/>
+      <c r="P188" s="29"/>
+      <c r="Q188" s="29"/>
+      <c r="R188" s="29"/>
     </row>
     <row r="189" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A189" s="1">
@@ -3704,22 +3737,22 @@
         <v>72</v>
       </c>
       <c r="C189" s="7" t="s">
-        <v>106</v>
-      </c>
-      <c r="D189" s="37"/>
-      <c r="E189" s="37"/>
-      <c r="F189" s="38"/>
-      <c r="H189" s="44"/>
-      <c r="I189" s="44"/>
-      <c r="J189" s="44"/>
-      <c r="K189" s="44"/>
-      <c r="L189" s="44"/>
-      <c r="M189" s="44"/>
-      <c r="N189" s="44"/>
-      <c r="O189" s="44"/>
-      <c r="P189" s="44"/>
-      <c r="Q189" s="44"/>
-      <c r="R189" s="44"/>
+        <v>105</v>
+      </c>
+      <c r="D189" s="36"/>
+      <c r="E189" s="36"/>
+      <c r="F189" s="37"/>
+      <c r="H189" s="29"/>
+      <c r="I189" s="29"/>
+      <c r="J189" s="29"/>
+      <c r="K189" s="29"/>
+      <c r="L189" s="29"/>
+      <c r="M189" s="29"/>
+      <c r="N189" s="29"/>
+      <c r="O189" s="29"/>
+      <c r="P189" s="29"/>
+      <c r="Q189" s="29"/>
+      <c r="R189" s="29"/>
     </row>
     <row r="190" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A190" s="1">
@@ -3729,20 +3762,20 @@
         <v>73</v>
       </c>
       <c r="C190" s="7"/>
-      <c r="D190" s="37"/>
-      <c r="E190" s="37"/>
-      <c r="F190" s="38"/>
-      <c r="H190" s="44"/>
-      <c r="I190" s="44"/>
-      <c r="J190" s="44"/>
-      <c r="K190" s="44"/>
-      <c r="L190" s="44"/>
-      <c r="M190" s="44"/>
-      <c r="N190" s="44"/>
-      <c r="O190" s="44"/>
-      <c r="P190" s="44"/>
-      <c r="Q190" s="44"/>
-      <c r="R190" s="44"/>
+      <c r="D190" s="36"/>
+      <c r="E190" s="36"/>
+      <c r="F190" s="37"/>
+      <c r="H190" s="29"/>
+      <c r="I190" s="29"/>
+      <c r="J190" s="29"/>
+      <c r="K190" s="29"/>
+      <c r="L190" s="29"/>
+      <c r="M190" s="29"/>
+      <c r="N190" s="29"/>
+      <c r="O190" s="29"/>
+      <c r="P190" s="29"/>
+      <c r="Q190" s="29"/>
+      <c r="R190" s="29"/>
     </row>
     <row r="191" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A191" s="1">
@@ -3752,20 +3785,20 @@
         <v>57</v>
       </c>
       <c r="C191" s="7"/>
-      <c r="D191" s="37"/>
-      <c r="E191" s="37"/>
-      <c r="F191" s="38"/>
-      <c r="H191" s="44"/>
-      <c r="I191" s="44"/>
-      <c r="J191" s="44"/>
-      <c r="K191" s="44"/>
-      <c r="L191" s="44"/>
-      <c r="M191" s="44"/>
-      <c r="N191" s="44"/>
-      <c r="O191" s="44"/>
-      <c r="P191" s="44"/>
-      <c r="Q191" s="44"/>
-      <c r="R191" s="44"/>
+      <c r="D191" s="36"/>
+      <c r="E191" s="36"/>
+      <c r="F191" s="37"/>
+      <c r="H191" s="29"/>
+      <c r="I191" s="29"/>
+      <c r="J191" s="29"/>
+      <c r="K191" s="29"/>
+      <c r="L191" s="29"/>
+      <c r="M191" s="29"/>
+      <c r="N191" s="29"/>
+      <c r="O191" s="29"/>
+      <c r="P191" s="29"/>
+      <c r="Q191" s="29"/>
+      <c r="R191" s="29"/>
     </row>
     <row r="192" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A192" s="1">
@@ -3775,20 +3808,20 @@
         <v>74</v>
       </c>
       <c r="C192" s="7"/>
-      <c r="D192" s="37"/>
-      <c r="E192" s="37"/>
-      <c r="F192" s="38"/>
-      <c r="H192" s="44"/>
-      <c r="I192" s="44"/>
-      <c r="J192" s="44"/>
-      <c r="K192" s="44"/>
-      <c r="L192" s="44"/>
-      <c r="M192" s="44"/>
-      <c r="N192" s="44"/>
-      <c r="O192" s="44"/>
-      <c r="P192" s="44"/>
-      <c r="Q192" s="44"/>
-      <c r="R192" s="44"/>
+      <c r="D192" s="36"/>
+      <c r="E192" s="36"/>
+      <c r="F192" s="37"/>
+      <c r="H192" s="29"/>
+      <c r="I192" s="29"/>
+      <c r="J192" s="29"/>
+      <c r="K192" s="29"/>
+      <c r="L192" s="29"/>
+      <c r="M192" s="29"/>
+      <c r="N192" s="29"/>
+      <c r="O192" s="29"/>
+      <c r="P192" s="29"/>
+      <c r="Q192" s="29"/>
+      <c r="R192" s="29"/>
     </row>
     <row r="193" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A193" s="1">
@@ -3798,22 +3831,22 @@
         <v>81</v>
       </c>
       <c r="C193" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D193" s="37"/>
-      <c r="E193" s="37"/>
-      <c r="F193" s="38"/>
-      <c r="H193" s="44"/>
-      <c r="I193" s="44"/>
-      <c r="J193" s="44"/>
-      <c r="K193" s="44"/>
-      <c r="L193" s="44"/>
-      <c r="M193" s="44"/>
-      <c r="N193" s="44"/>
-      <c r="O193" s="44"/>
-      <c r="P193" s="44"/>
-      <c r="Q193" s="44"/>
-      <c r="R193" s="44"/>
+        <v>106</v>
+      </c>
+      <c r="D193" s="36"/>
+      <c r="E193" s="36"/>
+      <c r="F193" s="37"/>
+      <c r="H193" s="29"/>
+      <c r="I193" s="29"/>
+      <c r="J193" s="29"/>
+      <c r="K193" s="29"/>
+      <c r="L193" s="29"/>
+      <c r="M193" s="29"/>
+      <c r="N193" s="29"/>
+      <c r="O193" s="29"/>
+      <c r="P193" s="29"/>
+      <c r="Q193" s="29"/>
+      <c r="R193" s="29"/>
     </row>
     <row r="194" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A194" s="1">
@@ -3823,22 +3856,22 @@
         <v>57</v>
       </c>
       <c r="C194" s="7" t="s">
-        <v>108</v>
-      </c>
-      <c r="D194" s="37"/>
-      <c r="E194" s="37"/>
-      <c r="F194" s="38"/>
-      <c r="H194" s="44"/>
-      <c r="I194" s="44"/>
-      <c r="J194" s="44"/>
-      <c r="K194" s="44"/>
-      <c r="L194" s="44"/>
-      <c r="M194" s="44"/>
-      <c r="N194" s="44"/>
-      <c r="O194" s="44"/>
-      <c r="P194" s="44"/>
-      <c r="Q194" s="44"/>
-      <c r="R194" s="44"/>
+        <v>107</v>
+      </c>
+      <c r="D194" s="36"/>
+      <c r="E194" s="36"/>
+      <c r="F194" s="37"/>
+      <c r="H194" s="29"/>
+      <c r="I194" s="29"/>
+      <c r="J194" s="29"/>
+      <c r="K194" s="29"/>
+      <c r="L194" s="29"/>
+      <c r="M194" s="29"/>
+      <c r="N194" s="29"/>
+      <c r="O194" s="29"/>
+      <c r="P194" s="29"/>
+      <c r="Q194" s="29"/>
+      <c r="R194" s="29"/>
     </row>
     <row r="195" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A195" s="1">
@@ -3848,43 +3881,43 @@
         <v>58</v>
       </c>
       <c r="C195" s="7"/>
-      <c r="D195" s="37"/>
-      <c r="E195" s="37"/>
-      <c r="F195" s="38"/>
-      <c r="H195" s="44"/>
-      <c r="I195" s="44"/>
-      <c r="J195" s="44"/>
-      <c r="K195" s="44"/>
-      <c r="L195" s="44"/>
-      <c r="M195" s="44"/>
-      <c r="N195" s="44"/>
-      <c r="O195" s="44"/>
-      <c r="P195" s="44"/>
-      <c r="Q195" s="44"/>
-      <c r="R195" s="44"/>
+      <c r="D195" s="36"/>
+      <c r="E195" s="36"/>
+      <c r="F195" s="37"/>
+      <c r="H195" s="29"/>
+      <c r="I195" s="29"/>
+      <c r="J195" s="29"/>
+      <c r="K195" s="29"/>
+      <c r="L195" s="29"/>
+      <c r="M195" s="29"/>
+      <c r="N195" s="29"/>
+      <c r="O195" s="29"/>
+      <c r="P195" s="29"/>
+      <c r="Q195" s="29"/>
+      <c r="R195" s="29"/>
     </row>
     <row r="196" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A196" s="1">
         <v>194</v>
       </c>
       <c r="B196" s="6" t="s">
-        <v>57</v>
+        <v>72</v>
       </c>
       <c r="C196" s="7"/>
-      <c r="D196" s="37"/>
-      <c r="E196" s="37"/>
-      <c r="F196" s="38"/>
-      <c r="H196" s="44"/>
-      <c r="I196" s="44"/>
-      <c r="J196" s="44"/>
-      <c r="K196" s="44"/>
-      <c r="L196" s="44"/>
-      <c r="M196" s="44"/>
-      <c r="N196" s="44"/>
-      <c r="O196" s="44"/>
-      <c r="P196" s="44"/>
-      <c r="Q196" s="44"/>
-      <c r="R196" s="44"/>
+      <c r="D196" s="36"/>
+      <c r="E196" s="36"/>
+      <c r="F196" s="37"/>
+      <c r="H196" s="29"/>
+      <c r="I196" s="29"/>
+      <c r="J196" s="29"/>
+      <c r="K196" s="29"/>
+      <c r="L196" s="29"/>
+      <c r="M196" s="29"/>
+      <c r="N196" s="29"/>
+      <c r="O196" s="29"/>
+      <c r="P196" s="29"/>
+      <c r="Q196" s="29"/>
+      <c r="R196" s="29"/>
     </row>
     <row r="197" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A197" s="1">
@@ -3894,20 +3927,20 @@
         <v>74</v>
       </c>
       <c r="C197" s="7"/>
-      <c r="D197" s="37"/>
-      <c r="E197" s="37"/>
-      <c r="F197" s="38"/>
-      <c r="H197" s="44"/>
-      <c r="I197" s="44"/>
-      <c r="J197" s="44"/>
-      <c r="K197" s="44"/>
-      <c r="L197" s="44"/>
-      <c r="M197" s="44"/>
-      <c r="N197" s="44"/>
-      <c r="O197" s="44"/>
-      <c r="P197" s="44"/>
-      <c r="Q197" s="44"/>
-      <c r="R197" s="44"/>
+      <c r="D197" s="36"/>
+      <c r="E197" s="36"/>
+      <c r="F197" s="37"/>
+      <c r="H197" s="29"/>
+      <c r="I197" s="29"/>
+      <c r="J197" s="29"/>
+      <c r="K197" s="29"/>
+      <c r="L197" s="29"/>
+      <c r="M197" s="29"/>
+      <c r="N197" s="29"/>
+      <c r="O197" s="29"/>
+      <c r="P197" s="29"/>
+      <c r="Q197" s="29"/>
+      <c r="R197" s="29"/>
     </row>
     <row r="198" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A198" s="1">
@@ -3917,11 +3950,11 @@
         <v>81</v>
       </c>
       <c r="C198" s="7" t="s">
-        <v>107</v>
-      </c>
-      <c r="D198" s="37"/>
-      <c r="E198" s="37"/>
-      <c r="F198" s="38"/>
+        <v>106</v>
+      </c>
+      <c r="D198" s="36"/>
+      <c r="E198" s="36"/>
+      <c r="F198" s="37"/>
     </row>
     <row r="199" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A199" s="1">
@@ -3930,10 +3963,12 @@
       <c r="B199" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="C199" s="7"/>
-      <c r="D199" s="37"/>
-      <c r="E199" s="37"/>
-      <c r="F199" s="38"/>
+      <c r="C199" s="7" t="s">
+        <v>110</v>
+      </c>
+      <c r="D199" s="36"/>
+      <c r="E199" s="36"/>
+      <c r="F199" s="37"/>
     </row>
     <row r="200" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A200" s="1">
@@ -3942,10 +3977,12 @@
       <c r="B200" s="6" t="s">
         <v>76</v>
       </c>
-      <c r="C200" s="7"/>
-      <c r="D200" s="37"/>
-      <c r="E200" s="37"/>
-      <c r="F200" s="38"/>
+      <c r="C200" s="7" t="s">
+        <v>111</v>
+      </c>
+      <c r="D200" s="36"/>
+      <c r="E200" s="36"/>
+      <c r="F200" s="37"/>
     </row>
     <row r="201" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A201" s="1">
@@ -3955,9 +3992,9 @@
         <v>55</v>
       </c>
       <c r="C201" s="7"/>
-      <c r="D201" s="37"/>
-      <c r="E201" s="37"/>
-      <c r="F201" s="38"/>
+      <c r="D201" s="36"/>
+      <c r="E201" s="36"/>
+      <c r="F201" s="37"/>
     </row>
     <row r="202" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A202" s="1">
@@ -3966,10 +4003,12 @@
       <c r="B202" s="6" t="s">
         <v>71</v>
       </c>
-      <c r="C202" s="7"/>
-      <c r="D202" s="37"/>
-      <c r="E202" s="37"/>
-      <c r="F202" s="38"/>
+      <c r="C202" s="49" t="s">
+        <v>112</v>
+      </c>
+      <c r="D202" s="36"/>
+      <c r="E202" s="36"/>
+      <c r="F202" s="37"/>
     </row>
     <row r="203" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A203" s="1">
@@ -3979,21 +4018,21 @@
         <v>83</v>
       </c>
       <c r="C203" s="7"/>
-      <c r="D203" s="37"/>
-      <c r="E203" s="37"/>
-      <c r="F203" s="38"/>
+      <c r="D203" s="36"/>
+      <c r="E203" s="36"/>
+      <c r="F203" s="37"/>
     </row>
     <row r="204" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A204" s="1">
         <v>202</v>
       </c>
       <c r="B204" s="6" t="s">
-        <v>84</v>
+        <v>114</v>
       </c>
       <c r="C204" s="7"/>
-      <c r="D204" s="37"/>
-      <c r="E204" s="37"/>
-      <c r="F204" s="38"/>
+      <c r="D204" s="36"/>
+      <c r="E204" s="36"/>
+      <c r="F204" s="37"/>
     </row>
     <row r="205" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A205" s="1">
@@ -4005,9 +4044,9 @@
       <c r="C205" s="7" t="s">
         <v>78</v>
       </c>
-      <c r="D205" s="37"/>
-      <c r="E205" s="37"/>
-      <c r="F205" s="38"/>
+      <c r="D205" s="36"/>
+      <c r="E205" s="36"/>
+      <c r="F205" s="37"/>
     </row>
     <row r="206" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A206" s="1">
@@ -4017,9 +4056,9 @@
         <v>66</v>
       </c>
       <c r="C206" s="7"/>
-      <c r="D206" s="37"/>
-      <c r="E206" s="37"/>
-      <c r="F206" s="38"/>
+      <c r="D206" s="36"/>
+      <c r="E206" s="36"/>
+      <c r="F206" s="37"/>
     </row>
     <row r="207" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A207" s="1">
@@ -4029,9 +4068,9 @@
         <v>67</v>
       </c>
       <c r="C207" s="7"/>
-      <c r="D207" s="37"/>
-      <c r="E207" s="37"/>
-      <c r="F207" s="38"/>
+      <c r="D207" s="36"/>
+      <c r="E207" s="36"/>
+      <c r="F207" s="37"/>
     </row>
     <row r="208" spans="1:18" x14ac:dyDescent="0.2">
       <c r="A208" s="1">
@@ -4041,9 +4080,9 @@
         <v>33</v>
       </c>
       <c r="C208" s="7"/>
-      <c r="D208" s="37"/>
-      <c r="E208" s="37"/>
-      <c r="F208" s="38"/>
+      <c r="D208" s="36"/>
+      <c r="E208" s="36"/>
+      <c r="F208" s="37"/>
     </row>
     <row r="209" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A209" s="1">
@@ -4053,9 +4092,9 @@
         <v>52</v>
       </c>
       <c r="C209" s="7"/>
-      <c r="D209" s="37"/>
-      <c r="E209" s="37"/>
-      <c r="F209" s="38"/>
+      <c r="D209" s="36"/>
+      <c r="E209" s="36"/>
+      <c r="F209" s="37"/>
     </row>
     <row r="210" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A210" s="1">
@@ -4065,9 +4104,9 @@
         <v>68</v>
       </c>
       <c r="C210" s="7"/>
-      <c r="D210" s="37"/>
-      <c r="E210" s="37"/>
-      <c r="F210" s="38"/>
+      <c r="D210" s="36"/>
+      <c r="E210" s="36"/>
+      <c r="F210" s="37"/>
     </row>
     <row r="211" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A211" s="1">
@@ -4079,9 +4118,9 @@
       <c r="C211" s="7" t="s">
         <v>79</v>
       </c>
-      <c r="D211" s="37"/>
-      <c r="E211" s="37"/>
-      <c r="F211" s="38"/>
+      <c r="D211" s="36"/>
+      <c r="E211" s="36"/>
+      <c r="F211" s="37"/>
     </row>
     <row r="212" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A212" s="1">
@@ -4091,9 +4130,9 @@
         <v>50</v>
       </c>
       <c r="C212" s="7"/>
-      <c r="D212" s="37"/>
-      <c r="E212" s="37"/>
-      <c r="F212" s="38"/>
+      <c r="D212" s="36"/>
+      <c r="E212" s="36"/>
+      <c r="F212" s="37"/>
     </row>
     <row r="213" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A213" s="1">
@@ -4103,9 +4142,9 @@
         <v>42</v>
       </c>
       <c r="C213" s="7"/>
-      <c r="D213" s="37"/>
-      <c r="E213" s="37"/>
-      <c r="F213" s="38"/>
+      <c r="D213" s="36"/>
+      <c r="E213" s="36"/>
+      <c r="F213" s="37"/>
     </row>
     <row r="214" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A214" s="1">
@@ -4115,9 +4154,9 @@
         <v>54</v>
       </c>
       <c r="C214" s="7"/>
-      <c r="D214" s="37"/>
-      <c r="E214" s="37"/>
-      <c r="F214" s="38"/>
+      <c r="D214" s="36"/>
+      <c r="E214" s="36"/>
+      <c r="F214" s="37"/>
     </row>
     <row r="215" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A215" s="1">
@@ -4127,9 +4166,9 @@
         <v>74</v>
       </c>
       <c r="C215" s="7"/>
-      <c r="D215" s="37"/>
-      <c r="E215" s="37"/>
-      <c r="F215" s="38"/>
+      <c r="D215" s="36"/>
+      <c r="E215" s="36"/>
+      <c r="F215" s="37"/>
     </row>
     <row r="216" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A216" s="1">
@@ -4139,9 +4178,9 @@
         <v>82</v>
       </c>
       <c r="C216" s="7"/>
-      <c r="D216" s="37"/>
-      <c r="E216" s="37"/>
-      <c r="F216" s="38"/>
+      <c r="D216" s="36"/>
+      <c r="E216" s="36"/>
+      <c r="F216" s="37"/>
     </row>
     <row r="217" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A217" s="1">
@@ -4150,12 +4189,12 @@
       <c r="B217" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="C217" s="47" t="s">
-        <v>96</v>
-      </c>
-      <c r="D217" s="37"/>
-      <c r="E217" s="37"/>
-      <c r="F217" s="38"/>
+      <c r="C217" s="30" t="s">
+        <v>95</v>
+      </c>
+      <c r="D217" s="36"/>
+      <c r="E217" s="36"/>
+      <c r="F217" s="37"/>
     </row>
     <row r="218" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A218" s="1">
@@ -4164,10 +4203,10 @@
       <c r="B218" s="6" t="s">
         <v>36</v>
       </c>
-      <c r="C218" s="27"/>
-      <c r="D218" s="37"/>
-      <c r="E218" s="37"/>
-      <c r="F218" s="38"/>
+      <c r="C218" s="31"/>
+      <c r="D218" s="36"/>
+      <c r="E218" s="36"/>
+      <c r="F218" s="37"/>
     </row>
     <row r="219" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A219" s="1">
@@ -4176,10 +4215,10 @@
       <c r="B219" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="C219" s="27"/>
-      <c r="D219" s="37"/>
-      <c r="E219" s="37"/>
-      <c r="F219" s="38"/>
+      <c r="C219" s="31"/>
+      <c r="D219" s="36"/>
+      <c r="E219" s="36"/>
+      <c r="F219" s="37"/>
     </row>
     <row r="220" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A220" s="1">
@@ -4188,10 +4227,10 @@
       <c r="B220" s="6" t="s">
         <v>64</v>
       </c>
-      <c r="C220" s="27"/>
-      <c r="D220" s="37"/>
-      <c r="E220" s="37"/>
-      <c r="F220" s="38"/>
+      <c r="C220" s="31"/>
+      <c r="D220" s="36"/>
+      <c r="E220" s="36"/>
+      <c r="F220" s="37"/>
     </row>
     <row r="221" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A221" s="1">
@@ -4200,10 +4239,10 @@
       <c r="B221" s="6" t="s">
         <v>41</v>
       </c>
-      <c r="C221" s="27"/>
-      <c r="D221" s="37"/>
-      <c r="E221" s="37"/>
-      <c r="F221" s="38"/>
+      <c r="C221" s="31"/>
+      <c r="D221" s="36"/>
+      <c r="E221" s="36"/>
+      <c r="F221" s="37"/>
     </row>
     <row r="222" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A222" s="1">
@@ -4212,10 +4251,10 @@
       <c r="B222" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C222" s="27"/>
-      <c r="D222" s="37"/>
-      <c r="E222" s="37"/>
-      <c r="F222" s="38"/>
+      <c r="C222" s="31"/>
+      <c r="D222" s="36"/>
+      <c r="E222" s="36"/>
+      <c r="F222" s="37"/>
     </row>
     <row r="223" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A223" s="1">
@@ -4224,10 +4263,10 @@
       <c r="B223" s="6" t="s">
         <v>42</v>
       </c>
-      <c r="C223" s="27"/>
-      <c r="D223" s="37"/>
-      <c r="E223" s="37"/>
-      <c r="F223" s="38"/>
+      <c r="C223" s="31"/>
+      <c r="D223" s="36"/>
+      <c r="E223" s="36"/>
+      <c r="F223" s="37"/>
     </row>
     <row r="224" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A224" s="1">
@@ -4236,10 +4275,10 @@
       <c r="B224" s="16" t="s">
         <v>34</v>
       </c>
-      <c r="C224" s="28"/>
-      <c r="D224" s="37"/>
-      <c r="E224" s="37"/>
-      <c r="F224" s="38"/>
+      <c r="C224" s="32"/>
+      <c r="D224" s="36"/>
+      <c r="E224" s="36"/>
+      <c r="F224" s="37"/>
     </row>
     <row r="225" spans="1:6" ht="15.75" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A225" s="1">
@@ -4249,9 +4288,9 @@
         <v>10</v>
       </c>
       <c r="C225" s="9"/>
-      <c r="D225" s="42"/>
-      <c r="E225" s="42"/>
-      <c r="F225" s="43"/>
+      <c r="D225" s="38"/>
+      <c r="E225" s="38"/>
+      <c r="F225" s="39"/>
     </row>
     <row r="226" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A226" s="1">
@@ -4260,14 +4299,14 @@
       <c r="B226" s="1" t="s">
         <v>55</v>
       </c>
-      <c r="C226" s="35" t="s">
-        <v>86</v>
-      </c>
-      <c r="D226" s="35" t="s">
-        <v>89</v>
-      </c>
-      <c r="E226" s="35"/>
-      <c r="F226" s="35"/>
+      <c r="C226" s="34" t="s">
+        <v>85</v>
+      </c>
+      <c r="D226" s="34" t="s">
+        <v>88</v>
+      </c>
+      <c r="E226" s="34"/>
+      <c r="F226" s="34"/>
     </row>
     <row r="227" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A227" s="1">
@@ -4276,10 +4315,10 @@
       <c r="B227" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C227" s="44"/>
-      <c r="D227" s="44"/>
-      <c r="E227" s="44"/>
-      <c r="F227" s="44"/>
+      <c r="C227" s="29"/>
+      <c r="D227" s="29"/>
+      <c r="E227" s="29"/>
+      <c r="F227" s="29"/>
     </row>
     <row r="228" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A228" s="1">
@@ -4288,12 +4327,12 @@
       <c r="B228" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="C228" s="44" t="s">
-        <v>85</v>
-      </c>
-      <c r="D228" s="44"/>
-      <c r="E228" s="44"/>
-      <c r="F228" s="44"/>
+      <c r="C228" s="29" t="s">
+        <v>84</v>
+      </c>
+      <c r="D228" s="29"/>
+      <c r="E228" s="29"/>
+      <c r="F228" s="29"/>
     </row>
     <row r="229" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A229" s="1">
@@ -4302,10 +4341,10 @@
       <c r="B229" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="C229" s="44"/>
-      <c r="D229" s="44"/>
-      <c r="E229" s="44"/>
-      <c r="F229" s="44"/>
+      <c r="C229" s="29"/>
+      <c r="D229" s="29"/>
+      <c r="E229" s="29"/>
+      <c r="F229" s="29"/>
     </row>
     <row r="230" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A230" s="1">
@@ -4314,24 +4353,24 @@
       <c r="B230" s="1" t="s">
         <v>62</v>
       </c>
-      <c r="C230" s="44" t="s">
-        <v>88</v>
-      </c>
-      <c r="D230" s="44"/>
-      <c r="E230" s="44"/>
-      <c r="F230" s="44"/>
+      <c r="C230" s="29" t="s">
+        <v>87</v>
+      </c>
+      <c r="D230" s="29"/>
+      <c r="E230" s="29"/>
+      <c r="F230" s="29"/>
     </row>
     <row r="231" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A231" s="1">
         <v>229</v>
       </c>
       <c r="B231" s="1" t="s">
-        <v>87</v>
-      </c>
-      <c r="C231" s="44"/>
-      <c r="D231" s="44"/>
-      <c r="E231" s="44"/>
-      <c r="F231" s="44"/>
+        <v>86</v>
+      </c>
+      <c r="C231" s="29"/>
+      <c r="D231" s="29"/>
+      <c r="E231" s="29"/>
+      <c r="F231" s="29"/>
     </row>
     <row r="232" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A232" s="1">
@@ -4341,18 +4380,18 @@
         <v>9</v>
       </c>
       <c r="C232" t="s">
-        <v>91</v>
-      </c>
-      <c r="D232" s="44"/>
-      <c r="E232" s="44"/>
-      <c r="F232" s="44"/>
+        <v>90</v>
+      </c>
+      <c r="D232" s="29"/>
+      <c r="E232" s="29"/>
+      <c r="F232" s="29"/>
     </row>
     <row r="233" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A233" s="1">
         <v>231</v>
       </c>
-      <c r="C233" s="45" t="s">
-        <v>92</v>
+      <c r="C233" s="27" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="234" spans="1:6" x14ac:dyDescent="0.2">
@@ -8322,11 +8361,11 @@
     </row>
   </sheetData>
   <mergeCells count="23">
-    <mergeCell ref="H177:R197"/>
-    <mergeCell ref="C217:C224"/>
-    <mergeCell ref="D169:F225"/>
-    <mergeCell ref="C226:C227"/>
-    <mergeCell ref="C228:C229"/>
+    <mergeCell ref="C2:F7"/>
+    <mergeCell ref="C8:F33"/>
+    <mergeCell ref="C34:C41"/>
+    <mergeCell ref="C52:C59"/>
+    <mergeCell ref="D34:F60"/>
     <mergeCell ref="C230:C231"/>
     <mergeCell ref="D226:F232"/>
     <mergeCell ref="C61:C68"/>
@@ -8334,17 +8373,17 @@
     <mergeCell ref="D61:F106"/>
     <mergeCell ref="C107:C114"/>
     <mergeCell ref="C169:C176"/>
-    <mergeCell ref="C2:F7"/>
-    <mergeCell ref="C8:F33"/>
-    <mergeCell ref="C34:C41"/>
-    <mergeCell ref="C52:C59"/>
-    <mergeCell ref="D34:F60"/>
     <mergeCell ref="C137:C144"/>
     <mergeCell ref="C150:C157"/>
     <mergeCell ref="C160:C167"/>
     <mergeCell ref="D137:F168"/>
     <mergeCell ref="C128:C135"/>
     <mergeCell ref="D107:F136"/>
+    <mergeCell ref="H177:R197"/>
+    <mergeCell ref="C217:C224"/>
+    <mergeCell ref="D169:F225"/>
+    <mergeCell ref="C226:C227"/>
+    <mergeCell ref="C228:C229"/>
   </mergeCells>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>